<commit_message>
Atualização de bases das ligas, do dia: 28-04-2024 às 23:19
</commit_message>
<xml_diff>
--- a/Canada Premier League/Canada Premier League.xlsx
+++ b/Canada Premier League/Canada Premier League.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="39">
   <si>
     <t>id</t>
   </si>
@@ -95,9 +95,6 @@
   </si>
   <si>
     <t>PL_AhUnder</t>
-  </si>
-  <si>
-    <t>7803364</t>
   </si>
   <si>
     <t>Canada Premier League</t>
@@ -495,7 +492,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB98"/>
+  <dimension ref="A1:AB99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -592,16 +589,16 @@
         <v>6240282</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D2" s="2">
         <v>45079.95833333334</v>
       </c>
       <c r="E2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G2">
         <v>3</v>
@@ -610,7 +607,7 @@
         <v>6</v>
       </c>
       <c r="I2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J2">
         <v>4</v>
@@ -678,16 +675,16 @@
         <v>6227808</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D3" s="2">
         <v>45080.70833333334</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -696,7 +693,7 @@
         <v>1</v>
       </c>
       <c r="I3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J3">
         <v>3.2</v>
@@ -764,16 +761,16 @@
         <v>6227809</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D4" s="2">
         <v>45080.83333333334</v>
       </c>
       <c r="E4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G4">
         <v>2</v>
@@ -782,7 +779,7 @@
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J4">
         <v>2.1</v>
@@ -850,16 +847,16 @@
         <v>6227810</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D5" s="2">
         <v>45081.66666666666</v>
       </c>
       <c r="E5" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" t="s">
         <v>32</v>
-      </c>
-      <c r="F5" t="s">
-        <v>33</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -868,7 +865,7 @@
         <v>1</v>
       </c>
       <c r="I5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J5">
         <v>3.25</v>
@@ -936,16 +933,16 @@
         <v>6227811</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D6" s="2">
         <v>45086.85416666666</v>
       </c>
       <c r="E6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G6">
         <v>2</v>
@@ -954,7 +951,7 @@
         <v>1</v>
       </c>
       <c r="I6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J6">
         <v>2.45</v>
@@ -1022,16 +1019,16 @@
         <v>6227812</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D7" s="2">
         <v>45087.58333333334</v>
       </c>
       <c r="E7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G7">
         <v>2</v>
@@ -1040,7 +1037,7 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J7">
         <v>2.7</v>
@@ -1108,16 +1105,16 @@
         <v>6227813</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D8" s="2">
         <v>45087.83333333334</v>
       </c>
       <c r="E8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" t="s">
         <v>35</v>
-      </c>
-      <c r="F8" t="s">
-        <v>36</v>
       </c>
       <c r="G8">
         <v>0</v>
@@ -1126,7 +1123,7 @@
         <v>1</v>
       </c>
       <c r="I8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J8">
         <v>2.25</v>
@@ -1194,16 +1191,16 @@
         <v>6240281</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D9" s="2">
         <v>45088.75</v>
       </c>
       <c r="E9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G9">
         <v>3</v>
@@ -1212,7 +1209,7 @@
         <v>1</v>
       </c>
       <c r="I9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J9">
         <v>1.909</v>
@@ -1280,16 +1277,16 @@
         <v>6227814</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10" s="2">
         <v>45093.875</v>
       </c>
       <c r="E10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G10">
         <v>2</v>
@@ -1298,7 +1295,7 @@
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J10">
         <v>2.1</v>
@@ -1363,67 +1360,67 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>6227815</v>
+        <v>6240280</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D11" s="2">
         <v>45094.625</v>
       </c>
       <c r="E11" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G11">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J11">
-        <v>2.6</v>
+        <v>1.571</v>
       </c>
       <c r="K11">
-        <v>3.2</v>
+        <v>3.4</v>
       </c>
       <c r="L11">
-        <v>2.4</v>
+        <v>5.5</v>
       </c>
       <c r="M11">
-        <v>3.3</v>
+        <v>1.444</v>
       </c>
       <c r="N11">
-        <v>3</v>
+        <v>3.8</v>
       </c>
       <c r="O11">
-        <v>2.15</v>
+        <v>6</v>
       </c>
       <c r="P11">
-        <v>0.25</v>
+        <v>-1.25</v>
       </c>
       <c r="Q11">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="R11">
-        <v>1.875</v>
+        <v>1.85</v>
       </c>
       <c r="S11">
-        <v>2.25</v>
+        <v>2.75</v>
       </c>
       <c r="T11">
-        <v>2</v>
+        <v>1.975</v>
       </c>
       <c r="U11">
-        <v>1.8</v>
+        <v>1.825</v>
       </c>
       <c r="V11">
-        <v>2.3</v>
+        <v>0.444</v>
       </c>
       <c r="W11">
         <v>-1</v>
@@ -1432,16 +1429,16 @@
         <v>-1</v>
       </c>
       <c r="Y11">
-        <v>0.925</v>
+        <v>-0.5</v>
       </c>
       <c r="Z11">
-        <v>-1</v>
+        <v>0.425</v>
       </c>
       <c r="AA11">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AB11">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
     </row>
     <row r="12" spans="1:28">
@@ -1449,67 +1446,67 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>6240280</v>
+        <v>6227815</v>
       </c>
       <c r="C12" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D12" s="2">
         <v>45094.625</v>
       </c>
       <c r="E12" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F12" t="s">
         <v>29</v>
       </c>
       <c r="G12">
+        <v>3</v>
+      </c>
+      <c r="H12">
         <v>1</v>
       </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
       <c r="I12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J12">
-        <v>1.571</v>
+        <v>2.6</v>
       </c>
       <c r="K12">
-        <v>3.4</v>
+        <v>3.2</v>
       </c>
       <c r="L12">
-        <v>5.5</v>
+        <v>2.4</v>
       </c>
       <c r="M12">
-        <v>1.444</v>
+        <v>3.3</v>
       </c>
       <c r="N12">
-        <v>3.8</v>
+        <v>3</v>
       </c>
       <c r="O12">
-        <v>6</v>
+        <v>2.15</v>
       </c>
       <c r="P12">
-        <v>-1.25</v>
+        <v>0.25</v>
       </c>
       <c r="Q12">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="R12">
-        <v>1.85</v>
+        <v>1.875</v>
       </c>
       <c r="S12">
-        <v>2.75</v>
+        <v>2.25</v>
       </c>
       <c r="T12">
-        <v>1.975</v>
+        <v>2</v>
       </c>
       <c r="U12">
-        <v>1.825</v>
+        <v>1.8</v>
       </c>
       <c r="V12">
-        <v>0.444</v>
+        <v>2.3</v>
       </c>
       <c r="W12">
         <v>-1</v>
@@ -1518,16 +1515,16 @@
         <v>-1</v>
       </c>
       <c r="Y12">
-        <v>-0.5</v>
+        <v>0.925</v>
       </c>
       <c r="Z12">
-        <v>0.425</v>
+        <v>-1</v>
       </c>
       <c r="AA12">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AB12">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="13" spans="1:28">
@@ -1538,16 +1535,16 @@
         <v>6227816</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D13" s="2">
         <v>45095.70833333334</v>
       </c>
       <c r="E13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G13">
         <v>1</v>
@@ -1556,7 +1553,7 @@
         <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J13">
         <v>1.615</v>
@@ -1624,16 +1621,16 @@
         <v>6240279</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D14" s="2">
         <v>45097.95833333334</v>
       </c>
       <c r="E14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G14">
         <v>2</v>
@@ -1642,7 +1639,7 @@
         <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J14">
         <v>5.2</v>
@@ -1707,49 +1704,49 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>6227817</v>
+        <v>6227818</v>
       </c>
       <c r="C15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D15" s="2">
-        <v>45098.83333333334</v>
+        <v>45098.95833333334</v>
       </c>
       <c r="E15" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F15" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G15">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H15">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I15" t="s">
         <v>38</v>
       </c>
       <c r="J15">
-        <v>2.5</v>
+        <v>1.666</v>
       </c>
       <c r="K15">
-        <v>2.9</v>
+        <v>3.4</v>
       </c>
       <c r="L15">
-        <v>2.875</v>
+        <v>5</v>
       </c>
       <c r="M15">
-        <v>2.25</v>
+        <v>1.533</v>
       </c>
       <c r="N15">
-        <v>3.1</v>
+        <v>3.6</v>
       </c>
       <c r="O15">
-        <v>3.2</v>
+        <v>6</v>
       </c>
       <c r="P15">
-        <v>-0.25</v>
+        <v>-1</v>
       </c>
       <c r="Q15">
         <v>1.95</v>
@@ -1761,31 +1758,31 @@
         <v>2.25</v>
       </c>
       <c r="T15">
-        <v>1.875</v>
+        <v>1.8</v>
       </c>
       <c r="U15">
-        <v>1.925</v>
+        <v>2</v>
       </c>
       <c r="V15">
-        <v>-1</v>
+        <v>0.5329999999999999</v>
       </c>
       <c r="W15">
-        <v>2.1</v>
+        <v>-1</v>
       </c>
       <c r="X15">
         <v>-1</v>
       </c>
       <c r="Y15">
-        <v>-0.5</v>
+        <v>0</v>
       </c>
       <c r="Z15">
-        <v>0.425</v>
+        <v>0</v>
       </c>
       <c r="AA15">
-        <v>0.875</v>
+        <v>-1</v>
       </c>
       <c r="AB15">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:28">
@@ -1793,49 +1790,49 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>6227818</v>
+        <v>6227817</v>
       </c>
       <c r="C16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D16" s="2">
-        <v>45098.95833333334</v>
+        <v>45098.83333333334</v>
       </c>
       <c r="E16" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I16" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="J16">
-        <v>1.666</v>
+        <v>2.5</v>
       </c>
       <c r="K16">
-        <v>3.4</v>
+        <v>2.9</v>
       </c>
       <c r="L16">
-        <v>5</v>
+        <v>2.875</v>
       </c>
       <c r="M16">
-        <v>1.533</v>
+        <v>2.25</v>
       </c>
       <c r="N16">
-        <v>3.6</v>
+        <v>3.1</v>
       </c>
       <c r="O16">
-        <v>6</v>
+        <v>3.2</v>
       </c>
       <c r="P16">
-        <v>-1</v>
+        <v>-0.25</v>
       </c>
       <c r="Q16">
         <v>1.95</v>
@@ -1847,31 +1844,31 @@
         <v>2.25</v>
       </c>
       <c r="T16">
-        <v>1.8</v>
+        <v>1.875</v>
       </c>
       <c r="U16">
-        <v>2</v>
+        <v>1.925</v>
       </c>
       <c r="V16">
-        <v>0.5329999999999999</v>
+        <v>-1</v>
       </c>
       <c r="W16">
-        <v>-1</v>
+        <v>2.1</v>
       </c>
       <c r="X16">
         <v>-1</v>
       </c>
       <c r="Y16">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="Z16">
-        <v>0</v>
+        <v>0.425</v>
       </c>
       <c r="AA16">
-        <v>-1</v>
+        <v>0.875</v>
       </c>
       <c r="AB16">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="17" spans="1:28">
@@ -1882,16 +1879,16 @@
         <v>6227819</v>
       </c>
       <c r="C17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D17" s="2">
         <v>45101.75</v>
       </c>
       <c r="E17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G17">
         <v>2</v>
@@ -1900,7 +1897,7 @@
         <v>1</v>
       </c>
       <c r="I17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J17">
         <v>1.8</v>
@@ -1968,16 +1965,16 @@
         <v>6240278</v>
       </c>
       <c r="C18" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D18" s="2">
         <v>45102.66666666666</v>
       </c>
       <c r="E18" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G18">
         <v>1</v>
@@ -1986,7 +1983,7 @@
         <v>0</v>
       </c>
       <c r="I18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J18">
         <v>1.571</v>
@@ -2054,16 +2051,16 @@
         <v>6227820</v>
       </c>
       <c r="C19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D19" s="2">
         <v>45102.79166666666</v>
       </c>
       <c r="E19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G19">
         <v>4</v>
@@ -2072,7 +2069,7 @@
         <v>3</v>
       </c>
       <c r="I19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J19">
         <v>1.909</v>
@@ -2140,16 +2137,16 @@
         <v>6227821</v>
       </c>
       <c r="C20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D20" s="2">
         <v>45107.79166666666</v>
       </c>
       <c r="E20" t="s">
+        <v>33</v>
+      </c>
+      <c r="F20" t="s">
         <v>34</v>
-      </c>
-      <c r="F20" t="s">
-        <v>35</v>
       </c>
       <c r="G20">
         <v>2</v>
@@ -2158,7 +2155,7 @@
         <v>1</v>
       </c>
       <c r="I20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J20">
         <v>2.4</v>
@@ -2226,16 +2223,16 @@
         <v>6227822</v>
       </c>
       <c r="C21" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D21" s="2">
         <v>45107.9375</v>
       </c>
       <c r="E21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F21" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G21">
         <v>2</v>
@@ -2244,7 +2241,7 @@
         <v>2</v>
       </c>
       <c r="I21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J21">
         <v>1.727</v>
@@ -2312,16 +2309,16 @@
         <v>6227823</v>
       </c>
       <c r="C22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D22" s="2">
         <v>45108.66666666666</v>
       </c>
       <c r="E22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G22">
         <v>0</v>
@@ -2330,7 +2327,7 @@
         <v>2</v>
       </c>
       <c r="I22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J22">
         <v>2.4</v>
@@ -2398,16 +2395,16 @@
         <v>6240277</v>
       </c>
       <c r="C23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D23" s="2">
         <v>45109.72916666666</v>
       </c>
       <c r="E23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F23" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G23">
         <v>1</v>
@@ -2416,7 +2413,7 @@
         <v>2</v>
       </c>
       <c r="I23" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J23">
         <v>3.25</v>
@@ -2484,16 +2481,16 @@
         <v>6240276</v>
       </c>
       <c r="C24" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D24" s="2">
         <v>45114.95833333334</v>
       </c>
       <c r="E24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F24" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G24">
         <v>2</v>
@@ -2502,7 +2499,7 @@
         <v>1</v>
       </c>
       <c r="I24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J24">
         <v>4.5</v>
@@ -2570,16 +2567,16 @@
         <v>6227824</v>
       </c>
       <c r="C25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D25" s="2">
         <v>45115.91666666666</v>
       </c>
       <c r="E25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G25">
         <v>1</v>
@@ -2588,7 +2585,7 @@
         <v>2</v>
       </c>
       <c r="I25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J25">
         <v>1.727</v>
@@ -2656,16 +2653,16 @@
         <v>6227825</v>
       </c>
       <c r="C26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D26" s="2">
         <v>45116.66666666666</v>
       </c>
       <c r="E26" t="s">
+        <v>30</v>
+      </c>
+      <c r="F26" t="s">
         <v>31</v>
-      </c>
-      <c r="F26" t="s">
-        <v>32</v>
       </c>
       <c r="G26">
         <v>2</v>
@@ -2674,7 +2671,7 @@
         <v>0</v>
       </c>
       <c r="I26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J26">
         <v>2.25</v>
@@ -2742,16 +2739,16 @@
         <v>6227826</v>
       </c>
       <c r="C27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D27" s="2">
         <v>45116.85416666666</v>
       </c>
       <c r="E27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G27">
         <v>0</v>
@@ -2760,7 +2757,7 @@
         <v>4</v>
       </c>
       <c r="I27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J27">
         <v>2.6</v>
@@ -2828,16 +2825,16 @@
         <v>6227827</v>
       </c>
       <c r="C28" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D28" s="2">
         <v>45118.79166666666</v>
       </c>
       <c r="E28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F28" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G28">
         <v>2</v>
@@ -2846,7 +2843,7 @@
         <v>1</v>
       </c>
       <c r="I28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J28">
         <v>2.75</v>
@@ -2914,16 +2911,16 @@
         <v>6227828</v>
       </c>
       <c r="C29" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D29" s="2">
         <v>45119.89583333334</v>
       </c>
       <c r="E29" t="s">
+        <v>29</v>
+      </c>
+      <c r="F29" t="s">
         <v>30</v>
-      </c>
-      <c r="F29" t="s">
-        <v>31</v>
       </c>
       <c r="G29">
         <v>0</v>
@@ -2932,7 +2929,7 @@
         <v>2</v>
       </c>
       <c r="I29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J29">
         <v>1.85</v>
@@ -3000,16 +2997,16 @@
         <v>6227829</v>
       </c>
       <c r="C30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D30" s="2">
         <v>45121.85416666666</v>
       </c>
       <c r="E30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G30">
         <v>0</v>
@@ -3018,7 +3015,7 @@
         <v>0</v>
       </c>
       <c r="I30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J30">
         <v>3.5</v>
@@ -3086,16 +3083,16 @@
         <v>6227830</v>
       </c>
       <c r="C31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D31" s="2">
         <v>45122.70833333334</v>
       </c>
       <c r="E31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G31">
         <v>1</v>
@@ -3104,7 +3101,7 @@
         <v>0</v>
       </c>
       <c r="I31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J31">
         <v>2.1</v>
@@ -3172,16 +3169,16 @@
         <v>6227831</v>
       </c>
       <c r="C32" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D32" s="2">
         <v>45122.83333333334</v>
       </c>
       <c r="E32" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F32" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G32">
         <v>1</v>
@@ -3190,7 +3187,7 @@
         <v>1</v>
       </c>
       <c r="I32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J32">
         <v>1.909</v>
@@ -3258,16 +3255,16 @@
         <v>6240275</v>
       </c>
       <c r="C33" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D33" s="2">
         <v>45123.625</v>
       </c>
       <c r="E33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F33" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G33">
         <v>3</v>
@@ -3276,7 +3273,7 @@
         <v>1</v>
       </c>
       <c r="I33" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J33">
         <v>1.5</v>
@@ -3344,16 +3341,16 @@
         <v>6227832</v>
       </c>
       <c r="C34" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D34" s="2">
         <v>45128.95833333334</v>
       </c>
       <c r="E34" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G34">
         <v>0</v>
@@ -3362,7 +3359,7 @@
         <v>2</v>
       </c>
       <c r="I34" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J34">
         <v>2.4</v>
@@ -3430,16 +3427,16 @@
         <v>6240274</v>
       </c>
       <c r="C35" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D35" s="2">
         <v>45129.83333333334</v>
       </c>
       <c r="E35" t="s">
+        <v>28</v>
+      </c>
+      <c r="F35" t="s">
         <v>29</v>
-      </c>
-      <c r="F35" t="s">
-        <v>30</v>
       </c>
       <c r="G35">
         <v>1</v>
@@ -3448,7 +3445,7 @@
         <v>5</v>
       </c>
       <c r="I35" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J35">
         <v>2.8</v>
@@ -3513,46 +3510,46 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>6227833</v>
+        <v>6227834</v>
       </c>
       <c r="C36" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D36" s="2">
-        <v>45130.70833333334</v>
+        <v>45130.83333333334</v>
       </c>
       <c r="E36" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F36" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G36">
         <v>1</v>
       </c>
       <c r="H36">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I36" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="J36">
-        <v>2.5</v>
+        <v>2.3</v>
       </c>
       <c r="K36">
         <v>3</v>
       </c>
       <c r="L36">
-        <v>2.6</v>
+        <v>2.9</v>
       </c>
       <c r="M36">
         <v>2.625</v>
       </c>
       <c r="N36">
-        <v>3.1</v>
+        <v>2.9</v>
       </c>
       <c r="O36">
-        <v>2.375</v>
+        <v>2.55</v>
       </c>
       <c r="P36">
         <v>0</v>
@@ -3567,31 +3564,31 @@
         <v>2.5</v>
       </c>
       <c r="T36">
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="U36">
-        <v>1.9</v>
+        <v>1.8</v>
       </c>
       <c r="V36">
-        <v>1.625</v>
+        <v>-1</v>
       </c>
       <c r="W36">
         <v>-1</v>
       </c>
       <c r="X36">
-        <v>-1</v>
+        <v>1.55</v>
       </c>
       <c r="Y36">
+        <v>-1</v>
+      </c>
+      <c r="Z36">
+        <v>0.8</v>
+      </c>
+      <c r="AA36">
         <v>1</v>
       </c>
-      <c r="Z36">
-        <v>-1</v>
-      </c>
-      <c r="AA36">
-        <v>-1</v>
-      </c>
       <c r="AB36">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="37" spans="1:28">
@@ -3599,46 +3596,46 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>6227834</v>
+        <v>6227833</v>
       </c>
       <c r="C37" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D37" s="2">
-        <v>45130.83333333334</v>
+        <v>45130.70833333334</v>
       </c>
       <c r="E37" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F37" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="G37">
         <v>1</v>
       </c>
       <c r="H37">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I37" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J37">
-        <v>2.3</v>
+        <v>2.5</v>
       </c>
       <c r="K37">
         <v>3</v>
       </c>
       <c r="L37">
-        <v>2.9</v>
+        <v>2.6</v>
       </c>
       <c r="M37">
         <v>2.625</v>
       </c>
       <c r="N37">
-        <v>2.9</v>
+        <v>3.1</v>
       </c>
       <c r="O37">
-        <v>2.55</v>
+        <v>2.375</v>
       </c>
       <c r="P37">
         <v>0</v>
@@ -3653,31 +3650,31 @@
         <v>2.5</v>
       </c>
       <c r="T37">
-        <v>2</v>
+        <v>1.9</v>
       </c>
       <c r="U37">
-        <v>1.8</v>
+        <v>1.9</v>
       </c>
       <c r="V37">
-        <v>-1</v>
+        <v>1.625</v>
       </c>
       <c r="W37">
         <v>-1</v>
       </c>
       <c r="X37">
-        <v>1.55</v>
+        <v>-1</v>
       </c>
       <c r="Y37">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Z37">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
       <c r="AA37">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AB37">
-        <v>-1</v>
+        <v>0.8999999999999999</v>
       </c>
     </row>
     <row r="38" spans="1:28">
@@ -3688,16 +3685,16 @@
         <v>6240273</v>
       </c>
       <c r="C38" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D38" s="2">
         <v>45135.83333333334</v>
       </c>
       <c r="E38" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F38" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G38">
         <v>2</v>
@@ -3706,7 +3703,7 @@
         <v>0</v>
       </c>
       <c r="I38" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J38">
         <v>1.3</v>
@@ -3774,16 +3771,16 @@
         <v>6227835</v>
       </c>
       <c r="C39" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D39" s="2">
         <v>45136.70833333334</v>
       </c>
       <c r="E39" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F39" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G39">
         <v>0</v>
@@ -3792,7 +3789,7 @@
         <v>3</v>
       </c>
       <c r="I39" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J39">
         <v>2.9</v>
@@ -3860,16 +3857,16 @@
         <v>6227836</v>
       </c>
       <c r="C40" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D40" s="2">
         <v>45136.83333333334</v>
       </c>
       <c r="E40" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F40" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G40">
         <v>1</v>
@@ -3878,7 +3875,7 @@
         <v>0</v>
       </c>
       <c r="I40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J40">
         <v>2.6</v>
@@ -3946,16 +3943,16 @@
         <v>6227837</v>
       </c>
       <c r="C41" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D41" s="2">
         <v>45137.625</v>
       </c>
       <c r="E41" t="s">
+        <v>32</v>
+      </c>
+      <c r="F41" t="s">
         <v>33</v>
-      </c>
-      <c r="F41" t="s">
-        <v>34</v>
       </c>
       <c r="G41">
         <v>0</v>
@@ -3964,7 +3961,7 @@
         <v>2</v>
       </c>
       <c r="I41" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J41">
         <v>2.2</v>
@@ -4032,16 +4029,16 @@
         <v>6227838</v>
       </c>
       <c r="C42" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D42" s="2">
         <v>45142.91666666666</v>
       </c>
       <c r="E42" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F42" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G42">
         <v>3</v>
@@ -4050,7 +4047,7 @@
         <v>0</v>
       </c>
       <c r="I42" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J42">
         <v>2.625</v>
@@ -4118,16 +4115,16 @@
         <v>6227839</v>
       </c>
       <c r="C43" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D43" s="2">
         <v>45143.83333333334</v>
       </c>
       <c r="E43" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F43" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G43">
         <v>3</v>
@@ -4136,7 +4133,7 @@
         <v>3</v>
       </c>
       <c r="I43" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J43">
         <v>2</v>
@@ -4204,16 +4201,16 @@
         <v>6240272</v>
       </c>
       <c r="C44" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D44" s="2">
         <v>45144.75</v>
       </c>
       <c r="E44" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F44" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G44">
         <v>0</v>
@@ -4222,7 +4219,7 @@
         <v>0</v>
       </c>
       <c r="I44" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J44">
         <v>2.9</v>
@@ -4290,16 +4287,16 @@
         <v>6227840</v>
       </c>
       <c r="C45" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D45" s="2">
         <v>45145.625</v>
       </c>
       <c r="E45" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F45" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G45">
         <v>1</v>
@@ -4308,7 +4305,7 @@
         <v>2</v>
       </c>
       <c r="I45" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J45">
         <v>2.75</v>
@@ -4376,16 +4373,16 @@
         <v>6227841</v>
       </c>
       <c r="C46" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D46" s="2">
         <v>45149.875</v>
       </c>
       <c r="E46" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F46" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G46">
         <v>3</v>
@@ -4394,7 +4391,7 @@
         <v>2</v>
       </c>
       <c r="I46" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J46">
         <v>2.875</v>
@@ -4462,16 +4459,16 @@
         <v>6240271</v>
       </c>
       <c r="C47" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D47" s="2">
         <v>45150.66666666666</v>
       </c>
       <c r="E47" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F47" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G47">
         <v>3</v>
@@ -4480,7 +4477,7 @@
         <v>0</v>
       </c>
       <c r="I47" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J47">
         <v>1.444</v>
@@ -4548,16 +4545,16 @@
         <v>6227842</v>
       </c>
       <c r="C48" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D48" s="2">
         <v>45150.83333333334</v>
       </c>
       <c r="E48" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F48" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G48">
         <v>3</v>
@@ -4566,7 +4563,7 @@
         <v>3</v>
       </c>
       <c r="I48" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J48">
         <v>1.727</v>
@@ -4634,16 +4631,16 @@
         <v>6227843</v>
       </c>
       <c r="C49" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D49" s="2">
         <v>45151.72916666666</v>
       </c>
       <c r="E49" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F49" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G49">
         <v>0</v>
@@ -4652,7 +4649,7 @@
         <v>1</v>
       </c>
       <c r="I49" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J49">
         <v>1.8</v>
@@ -4720,16 +4717,16 @@
         <v>6227844</v>
       </c>
       <c r="C50" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D50" s="2">
         <v>45156.875</v>
       </c>
       <c r="E50" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F50" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G50">
         <v>1</v>
@@ -4738,7 +4735,7 @@
         <v>3</v>
       </c>
       <c r="I50" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J50">
         <v>2.8</v>
@@ -4806,16 +4803,16 @@
         <v>6240270</v>
       </c>
       <c r="C51" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D51" s="2">
         <v>45157.70833333334</v>
       </c>
       <c r="E51" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F51" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G51">
         <v>3</v>
@@ -4824,7 +4821,7 @@
         <v>2</v>
       </c>
       <c r="I51" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J51">
         <v>7</v>
@@ -4892,16 +4889,16 @@
         <v>6227855</v>
       </c>
       <c r="C52" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D52" s="2">
         <v>45157.83333333334</v>
       </c>
       <c r="E52" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F52" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G52">
         <v>1</v>
@@ -4910,7 +4907,7 @@
         <v>1</v>
       </c>
       <c r="I52" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J52">
         <v>1.727</v>
@@ -4978,16 +4975,16 @@
         <v>6227861</v>
       </c>
       <c r="C53" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D53" s="2">
         <v>45158.75</v>
       </c>
       <c r="E53" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F53" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G53">
         <v>2</v>
@@ -4996,7 +4993,7 @@
         <v>1</v>
       </c>
       <c r="I53" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J53">
         <v>1.571</v>
@@ -5064,16 +5061,16 @@
         <v>6240269</v>
       </c>
       <c r="C54" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D54" s="2">
         <v>45163.85416666666</v>
       </c>
       <c r="E54" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F54" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G54">
         <v>2</v>
@@ -5082,7 +5079,7 @@
         <v>1</v>
       </c>
       <c r="I54" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J54">
         <v>1.8</v>
@@ -5150,16 +5147,16 @@
         <v>6227862</v>
       </c>
       <c r="C55" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D55" s="2">
         <v>45164.66666666666</v>
       </c>
       <c r="E55" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F55" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G55">
         <v>3</v>
@@ -5168,7 +5165,7 @@
         <v>0</v>
       </c>
       <c r="I55" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J55">
         <v>2</v>
@@ -5236,16 +5233,16 @@
         <v>6227863</v>
       </c>
       <c r="C56" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D56" s="2">
         <v>45164.83333333334</v>
       </c>
       <c r="E56" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F56" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G56">
         <v>0</v>
@@ -5254,7 +5251,7 @@
         <v>0</v>
       </c>
       <c r="I56" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J56">
         <v>2.5</v>
@@ -5322,16 +5319,16 @@
         <v>6227864</v>
       </c>
       <c r="C57" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D57" s="2">
         <v>45165.75</v>
       </c>
       <c r="E57" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F57" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G57">
         <v>1</v>
@@ -5340,7 +5337,7 @@
         <v>0</v>
       </c>
       <c r="I57" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J57">
         <v>2.4</v>
@@ -5405,82 +5402,82 @@
         <v>56</v>
       </c>
       <c r="B58">
-        <v>6227865</v>
+        <v>6227866</v>
       </c>
       <c r="C58" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D58" s="2">
-        <v>45171.70833333334</v>
+        <v>45171.83333333334</v>
       </c>
       <c r="E58" t="s">
+        <v>30</v>
+      </c>
+      <c r="F58" t="s">
+        <v>29</v>
+      </c>
+      <c r="G58">
+        <v>1</v>
+      </c>
+      <c r="H58">
+        <v>2</v>
+      </c>
+      <c r="I58" t="s">
         <v>36</v>
       </c>
-      <c r="F58" t="s">
-        <v>32</v>
-      </c>
-      <c r="G58">
+      <c r="J58">
+        <v>2.4</v>
+      </c>
+      <c r="K58">
+        <v>3.2</v>
+      </c>
+      <c r="L58">
+        <v>2.6</v>
+      </c>
+      <c r="M58">
+        <v>2.8</v>
+      </c>
+      <c r="N58">
+        <v>3</v>
+      </c>
+      <c r="O58">
+        <v>2.375</v>
+      </c>
+      <c r="P58">
+        <v>0</v>
+      </c>
+      <c r="Q58">
+        <v>2.05</v>
+      </c>
+      <c r="R58">
+        <v>1.75</v>
+      </c>
+      <c r="S58">
         <v>2</v>
       </c>
-      <c r="H58">
-        <v>1</v>
-      </c>
-      <c r="I58" t="s">
-        <v>39</v>
-      </c>
-      <c r="J58">
-        <v>1.7</v>
-      </c>
-      <c r="K58">
-        <v>3.4</v>
-      </c>
-      <c r="L58">
-        <v>4.333</v>
-      </c>
-      <c r="M58">
-        <v>1.65</v>
-      </c>
-      <c r="N58">
-        <v>3.5</v>
-      </c>
-      <c r="O58">
-        <v>4.75</v>
-      </c>
-      <c r="P58">
-        <v>-0.75</v>
-      </c>
-      <c r="Q58">
-        <v>1.85</v>
-      </c>
-      <c r="R58">
-        <v>1.95</v>
-      </c>
-      <c r="S58">
-        <v>2.5</v>
-      </c>
       <c r="T58">
-        <v>1.925</v>
+        <v>1.775</v>
       </c>
       <c r="U58">
-        <v>1.875</v>
+        <v>2.025</v>
       </c>
       <c r="V58">
-        <v>0.6499999999999999</v>
+        <v>-1</v>
       </c>
       <c r="W58">
         <v>-1</v>
       </c>
       <c r="X58">
-        <v>-1</v>
+        <v>1.375</v>
       </c>
       <c r="Y58">
-        <v>0.425</v>
+        <v>-1</v>
       </c>
       <c r="Z58">
-        <v>-0.5</v>
+        <v>0.75</v>
       </c>
       <c r="AA58">
-        <v>0.925</v>
+        <v>0.7749999999999999</v>
       </c>
       <c r="AB58">
         <v>-1</v>
@@ -5491,82 +5488,82 @@
         <v>57</v>
       </c>
       <c r="B59">
-        <v>6227866</v>
+        <v>6227865</v>
       </c>
       <c r="C59" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D59" s="2">
-        <v>45171.83333333334</v>
+        <v>45171.70833333334</v>
       </c>
       <c r="E59" t="s">
+        <v>35</v>
+      </c>
+      <c r="F59" t="s">
         <v>31</v>
       </c>
-      <c r="F59" t="s">
-        <v>30</v>
-      </c>
       <c r="G59">
+        <v>2</v>
+      </c>
+      <c r="H59">
         <v>1</v>
       </c>
-      <c r="H59">
-        <v>2</v>
-      </c>
       <c r="I59" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J59">
-        <v>2.4</v>
+        <v>1.7</v>
       </c>
       <c r="K59">
-        <v>3.2</v>
+        <v>3.4</v>
       </c>
       <c r="L59">
-        <v>2.6</v>
+        <v>4.333</v>
       </c>
       <c r="M59">
-        <v>2.8</v>
+        <v>1.65</v>
       </c>
       <c r="N59">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="O59">
-        <v>2.375</v>
+        <v>4.75</v>
       </c>
       <c r="P59">
-        <v>0</v>
+        <v>-0.75</v>
       </c>
       <c r="Q59">
-        <v>2.05</v>
+        <v>1.85</v>
       </c>
       <c r="R59">
-        <v>1.75</v>
+        <v>1.95</v>
       </c>
       <c r="S59">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="T59">
-        <v>1.775</v>
+        <v>1.925</v>
       </c>
       <c r="U59">
-        <v>2.025</v>
+        <v>1.875</v>
       </c>
       <c r="V59">
-        <v>-1</v>
+        <v>0.6499999999999999</v>
       </c>
       <c r="W59">
         <v>-1</v>
       </c>
       <c r="X59">
-        <v>1.375</v>
+        <v>-1</v>
       </c>
       <c r="Y59">
-        <v>-1</v>
+        <v>0.425</v>
       </c>
       <c r="Z59">
-        <v>0.75</v>
+        <v>-0.5</v>
       </c>
       <c r="AA59">
-        <v>0.7749999999999999</v>
+        <v>0.925</v>
       </c>
       <c r="AB59">
         <v>-1</v>
@@ -5580,16 +5577,16 @@
         <v>6240268</v>
       </c>
       <c r="C60" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D60" s="2">
         <v>45172.75</v>
       </c>
       <c r="E60" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F60" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G60">
         <v>0</v>
@@ -5598,7 +5595,7 @@
         <v>3</v>
       </c>
       <c r="I60" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J60">
         <v>6</v>
@@ -5666,16 +5663,16 @@
         <v>6227867</v>
       </c>
       <c r="C61" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D61" s="2">
         <v>45173.625</v>
       </c>
       <c r="E61" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F61" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G61">
         <v>1</v>
@@ -5684,7 +5681,7 @@
         <v>2</v>
       </c>
       <c r="I61" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J61">
         <v>1.8</v>
@@ -5749,85 +5746,85 @@
         <v>60</v>
       </c>
       <c r="B62">
-        <v>6227868</v>
+        <v>6227869</v>
       </c>
       <c r="C62" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D62" s="2">
-        <v>45177.83333333334</v>
+        <v>45177.95833333334</v>
       </c>
       <c r="E62" t="s">
+        <v>35</v>
+      </c>
+      <c r="F62" t="s">
         <v>33</v>
-      </c>
-      <c r="F62" t="s">
-        <v>32</v>
       </c>
       <c r="G62">
         <v>1</v>
       </c>
       <c r="H62">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I62" t="s">
         <v>37</v>
       </c>
       <c r="J62">
-        <v>2.15</v>
+        <v>1.75</v>
       </c>
       <c r="K62">
-        <v>3.25</v>
+        <v>3.3</v>
       </c>
       <c r="L62">
-        <v>3</v>
+        <v>4.2</v>
       </c>
       <c r="M62">
+        <v>1.6</v>
+      </c>
+      <c r="N62">
+        <v>3.6</v>
+      </c>
+      <c r="O62">
+        <v>5</v>
+      </c>
+      <c r="P62">
+        <v>-0.75</v>
+      </c>
+      <c r="Q62">
+        <v>1.8</v>
+      </c>
+      <c r="R62">
+        <v>2</v>
+      </c>
+      <c r="S62">
+        <v>2.5</v>
+      </c>
+      <c r="T62">
         <v>1.85</v>
       </c>
-      <c r="N62">
-        <v>3.4</v>
-      </c>
-      <c r="O62">
-        <v>3.6</v>
-      </c>
-      <c r="P62">
-        <v>-0.5</v>
-      </c>
-      <c r="Q62">
-        <v>1.9</v>
-      </c>
-      <c r="R62">
-        <v>1.9</v>
-      </c>
-      <c r="S62">
-        <v>2.75</v>
-      </c>
-      <c r="T62">
-        <v>1.825</v>
-      </c>
       <c r="U62">
-        <v>1.975</v>
+        <v>1.95</v>
       </c>
       <c r="V62">
         <v>-1</v>
       </c>
       <c r="W62">
-        <v>-1</v>
+        <v>2.6</v>
       </c>
       <c r="X62">
-        <v>2.6</v>
+        <v>-1</v>
       </c>
       <c r="Y62">
         <v>-1</v>
       </c>
       <c r="Z62">
-        <v>0.8999999999999999</v>
+        <v>1</v>
       </c>
       <c r="AA62">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
       <c r="AB62">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="63" spans="1:28">
@@ -5835,85 +5832,85 @@
         <v>61</v>
       </c>
       <c r="B63">
-        <v>6227869</v>
+        <v>6227868</v>
       </c>
       <c r="C63" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D63" s="2">
-        <v>45177.95833333334</v>
+        <v>45177.83333333334</v>
       </c>
       <c r="E63" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F63" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G63">
         <v>1</v>
       </c>
       <c r="H63">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I63" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J63">
-        <v>1.75</v>
+        <v>2.15</v>
       </c>
       <c r="K63">
-        <v>3.3</v>
+        <v>3.25</v>
       </c>
       <c r="L63">
-        <v>4.2</v>
+        <v>3</v>
       </c>
       <c r="M63">
-        <v>1.6</v>
+        <v>1.85</v>
       </c>
       <c r="N63">
+        <v>3.4</v>
+      </c>
+      <c r="O63">
         <v>3.6</v>
       </c>
-      <c r="O63">
-        <v>5</v>
-      </c>
       <c r="P63">
-        <v>-0.75</v>
+        <v>-0.5</v>
       </c>
       <c r="Q63">
-        <v>1.8</v>
+        <v>1.9</v>
       </c>
       <c r="R63">
-        <v>2</v>
+        <v>1.9</v>
       </c>
       <c r="S63">
-        <v>2.5</v>
+        <v>2.75</v>
       </c>
       <c r="T63">
-        <v>1.85</v>
+        <v>1.825</v>
       </c>
       <c r="U63">
-        <v>1.95</v>
+        <v>1.975</v>
       </c>
       <c r="V63">
         <v>-1</v>
       </c>
       <c r="W63">
+        <v>-1</v>
+      </c>
+      <c r="X63">
         <v>2.6</v>
       </c>
-      <c r="X63">
-        <v>-1</v>
-      </c>
       <c r="Y63">
         <v>-1</v>
       </c>
       <c r="Z63">
-        <v>1</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AA63">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
       <c r="AB63">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="64" spans="1:28">
@@ -5924,16 +5921,16 @@
         <v>6227870</v>
       </c>
       <c r="C64" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D64" s="2">
         <v>45178.83333333334</v>
       </c>
       <c r="E64" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F64" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G64">
         <v>0</v>
@@ -5942,7 +5939,7 @@
         <v>0</v>
       </c>
       <c r="I64" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J64">
         <v>1.909</v>
@@ -6010,16 +6007,16 @@
         <v>6240267</v>
       </c>
       <c r="C65" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D65" s="2">
         <v>45178.95833333334</v>
       </c>
       <c r="E65" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F65" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G65">
         <v>2</v>
@@ -6028,7 +6025,7 @@
         <v>1</v>
       </c>
       <c r="I65" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J65">
         <v>3.5</v>
@@ -6096,16 +6093,16 @@
         <v>6227871</v>
       </c>
       <c r="C66" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D66" s="2">
         <v>45181.79166666666</v>
       </c>
       <c r="E66" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F66" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G66">
         <v>1</v>
@@ -6114,7 +6111,7 @@
         <v>2</v>
       </c>
       <c r="I66" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J66">
         <v>2.6</v>
@@ -6182,16 +6179,16 @@
         <v>6227872</v>
       </c>
       <c r="C67" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D67" s="2">
         <v>45182.77083333334</v>
       </c>
       <c r="E67" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F67" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G67">
         <v>1</v>
@@ -6200,7 +6197,7 @@
         <v>1</v>
       </c>
       <c r="I67" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J67">
         <v>2.5</v>
@@ -6268,16 +6265,16 @@
         <v>6240266</v>
       </c>
       <c r="C68" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D68" s="2">
         <v>45185.75</v>
       </c>
       <c r="E68" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F68" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G68">
         <v>2</v>
@@ -6286,7 +6283,7 @@
         <v>1</v>
       </c>
       <c r="I68" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J68">
         <v>1.285</v>
@@ -6354,16 +6351,16 @@
         <v>6227874</v>
       </c>
       <c r="C69" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D69" s="2">
         <v>45186.625</v>
       </c>
       <c r="E69" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F69" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G69">
         <v>2</v>
@@ -6372,7 +6369,7 @@
         <v>3</v>
       </c>
       <c r="I69" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J69">
         <v>3.1</v>
@@ -6440,16 +6437,16 @@
         <v>6227875</v>
       </c>
       <c r="C70" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D70" s="2">
         <v>45186.75</v>
       </c>
       <c r="E70" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F70" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G70">
         <v>1</v>
@@ -6458,7 +6455,7 @@
         <v>4</v>
       </c>
       <c r="I70" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J70">
         <v>3</v>
@@ -6526,16 +6523,16 @@
         <v>6227873</v>
       </c>
       <c r="C71" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D71" s="2">
         <v>45187.79166666666</v>
       </c>
       <c r="E71" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F71" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G71">
         <v>3</v>
@@ -6544,7 +6541,7 @@
         <v>2</v>
       </c>
       <c r="I71" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J71">
         <v>2.625</v>
@@ -6612,16 +6609,16 @@
         <v>6240265</v>
       </c>
       <c r="C72" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D72" s="2">
         <v>45189.875</v>
       </c>
       <c r="E72" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F72" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G72">
         <v>0</v>
@@ -6630,7 +6627,7 @@
         <v>1</v>
       </c>
       <c r="I72" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J72">
         <v>1.615</v>
@@ -6695,85 +6692,85 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>6227876</v>
+        <v>6227877</v>
       </c>
       <c r="C73" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D73" s="2">
-        <v>45192.58333333334</v>
+        <v>45192.83333333334</v>
       </c>
       <c r="E73" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F73" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G73">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H73">
         <v>1</v>
       </c>
       <c r="I73" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J73">
-        <v>3.6</v>
+        <v>2</v>
       </c>
       <c r="K73">
-        <v>3.4</v>
+        <v>3.2</v>
       </c>
       <c r="L73">
-        <v>1.909</v>
+        <v>3.3</v>
       </c>
       <c r="M73">
-        <v>3.75</v>
+        <v>2.25</v>
       </c>
       <c r="N73">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="O73">
-        <v>1.833</v>
+        <v>2.875</v>
       </c>
       <c r="P73">
-        <v>0.5</v>
+        <v>-0.25</v>
       </c>
       <c r="Q73">
-        <v>1.9</v>
+        <v>2.025</v>
       </c>
       <c r="R73">
-        <v>1.9</v>
+        <v>1.775</v>
       </c>
       <c r="S73">
-        <v>2.75</v>
+        <v>2.25</v>
       </c>
       <c r="T73">
-        <v>1.9</v>
+        <v>1.825</v>
       </c>
       <c r="U73">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="V73">
-        <v>-1</v>
+        <v>1.25</v>
       </c>
       <c r="W73">
         <v>-1</v>
       </c>
       <c r="X73">
-        <v>0.833</v>
+        <v>-1</v>
       </c>
       <c r="Y73">
-        <v>-1</v>
+        <v>1.025</v>
       </c>
       <c r="Z73">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AA73">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
       <c r="AB73">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="74" spans="1:28">
@@ -6781,43 +6778,43 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>6240264</v>
+        <v>6227876</v>
       </c>
       <c r="C74" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D74" s="2">
-        <v>45192.70833333334</v>
+        <v>45192.58333333334</v>
       </c>
       <c r="E74" t="s">
+        <v>32</v>
+      </c>
+      <c r="F74" t="s">
         <v>29</v>
       </c>
-      <c r="F74" t="s">
-        <v>34</v>
-      </c>
       <c r="G74">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H74">
         <v>1</v>
       </c>
       <c r="I74" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="J74">
-        <v>3.75</v>
+        <v>3.6</v>
       </c>
       <c r="K74">
         <v>3.4</v>
       </c>
       <c r="L74">
-        <v>1.8</v>
+        <v>1.909</v>
       </c>
       <c r="M74">
-        <v>3.6</v>
+        <v>3.75</v>
       </c>
       <c r="N74">
-        <v>3.4</v>
+        <v>3.5</v>
       </c>
       <c r="O74">
         <v>1.833</v>
@@ -6826,40 +6823,40 @@
         <v>0.5</v>
       </c>
       <c r="Q74">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="R74">
-        <v>1.875</v>
+        <v>1.9</v>
       </c>
       <c r="S74">
         <v>2.75</v>
       </c>
       <c r="T74">
-        <v>1.95</v>
+        <v>1.9</v>
       </c>
       <c r="U74">
-        <v>1.85</v>
+        <v>1.9</v>
       </c>
       <c r="V74">
-        <v>2.6</v>
+        <v>-1</v>
       </c>
       <c r="W74">
         <v>-1</v>
       </c>
       <c r="X74">
-        <v>-1</v>
+        <v>0.833</v>
       </c>
       <c r="Y74">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
       <c r="Z74">
-        <v>-1</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AA74">
-        <v>0.475</v>
+        <v>-1</v>
       </c>
       <c r="AB74">
-        <v>-0.5</v>
+        <v>0.8999999999999999</v>
       </c>
     </row>
     <row r="75" spans="1:28">
@@ -6867,67 +6864,67 @@
         <v>73</v>
       </c>
       <c r="B75">
-        <v>6227877</v>
+        <v>6240264</v>
       </c>
       <c r="C75" t="s">
+        <v>27</v>
+      </c>
+      <c r="D75" s="2">
+        <v>45192.70833333334</v>
+      </c>
+      <c r="E75" t="s">
         <v>28</v>
       </c>
-      <c r="D75" s="2">
-        <v>45192.83333333334</v>
-      </c>
-      <c r="E75" t="s">
-        <v>35</v>
-      </c>
       <c r="F75" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G75">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H75">
         <v>1</v>
       </c>
       <c r="I75" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J75">
-        <v>2</v>
+        <v>3.75</v>
       </c>
       <c r="K75">
-        <v>3.2</v>
+        <v>3.4</v>
       </c>
       <c r="L75">
-        <v>3.3</v>
+        <v>1.8</v>
       </c>
       <c r="M75">
-        <v>2.25</v>
+        <v>3.6</v>
       </c>
       <c r="N75">
-        <v>3</v>
+        <v>3.4</v>
       </c>
       <c r="O75">
-        <v>2.875</v>
+        <v>1.833</v>
       </c>
       <c r="P75">
-        <v>-0.25</v>
+        <v>0.5</v>
       </c>
       <c r="Q75">
-        <v>2.025</v>
+        <v>1.925</v>
       </c>
       <c r="R75">
-        <v>1.775</v>
+        <v>1.875</v>
       </c>
       <c r="S75">
-        <v>2.25</v>
+        <v>2.75</v>
       </c>
       <c r="T75">
-        <v>1.825</v>
+        <v>1.95</v>
       </c>
       <c r="U75">
-        <v>1.975</v>
+        <v>1.85</v>
       </c>
       <c r="V75">
-        <v>1.25</v>
+        <v>2.6</v>
       </c>
       <c r="W75">
         <v>-1</v>
@@ -6936,16 +6933,16 @@
         <v>-1</v>
       </c>
       <c r="Y75">
-        <v>1.025</v>
+        <v>0.925</v>
       </c>
       <c r="Z75">
         <v>-1</v>
       </c>
       <c r="AA75">
-        <v>0.825</v>
+        <v>0.475</v>
       </c>
       <c r="AB75">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="76" spans="1:28">
@@ -6956,16 +6953,16 @@
         <v>6227878</v>
       </c>
       <c r="C76" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D76" s="2">
         <v>45193.625</v>
       </c>
       <c r="E76" t="s">
+        <v>30</v>
+      </c>
+      <c r="F76" t="s">
         <v>31</v>
-      </c>
-      <c r="F76" t="s">
-        <v>32</v>
       </c>
       <c r="G76">
         <v>0</v>
@@ -6974,7 +6971,7 @@
         <v>1</v>
       </c>
       <c r="I76" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J76">
         <v>2.1</v>
@@ -7042,16 +7039,16 @@
         <v>6227879</v>
       </c>
       <c r="C77" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D77" s="2">
         <v>45198.91666666666</v>
       </c>
       <c r="E77" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F77" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G77">
         <v>2</v>
@@ -7060,7 +7057,7 @@
         <v>1</v>
       </c>
       <c r="I77" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J77">
         <v>1.615</v>
@@ -7125,58 +7122,58 @@
         <v>76</v>
       </c>
       <c r="B78">
-        <v>6227880</v>
+        <v>6240263</v>
       </c>
       <c r="C78" t="s">
+        <v>27</v>
+      </c>
+      <c r="D78" s="2">
+        <v>45199.75</v>
+      </c>
+      <c r="E78" t="s">
+        <v>35</v>
+      </c>
+      <c r="F78" t="s">
         <v>28</v>
       </c>
-      <c r="D78" s="2">
-        <v>45199.625</v>
-      </c>
-      <c r="E78" t="s">
-        <v>34</v>
-      </c>
-      <c r="F78" t="s">
-        <v>35</v>
-      </c>
       <c r="G78">
+        <v>1</v>
+      </c>
+      <c r="H78">
         <v>2</v>
       </c>
-      <c r="H78">
-        <v>1</v>
-      </c>
       <c r="I78" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="J78">
-        <v>2.625</v>
+        <v>1.285</v>
       </c>
       <c r="K78">
-        <v>3.4</v>
+        <v>5</v>
       </c>
       <c r="L78">
-        <v>2.4</v>
+        <v>8.5</v>
       </c>
       <c r="M78">
-        <v>2.9</v>
+        <v>1.3</v>
       </c>
       <c r="N78">
-        <v>3.4</v>
+        <v>5.5</v>
       </c>
       <c r="O78">
-        <v>2.2</v>
+        <v>6</v>
       </c>
       <c r="P78">
-        <v>0.25</v>
+        <v>-1.5</v>
       </c>
       <c r="Q78">
-        <v>1.875</v>
+        <v>1.775</v>
       </c>
       <c r="R78">
         <v>1.925</v>
       </c>
       <c r="S78">
-        <v>2.5</v>
+        <v>3.25</v>
       </c>
       <c r="T78">
         <v>1.975</v>
@@ -7185,25 +7182,25 @@
         <v>1.825</v>
       </c>
       <c r="V78">
-        <v>1.9</v>
+        <v>-1</v>
       </c>
       <c r="W78">
         <v>-1</v>
       </c>
       <c r="X78">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="Y78">
-        <v>0.875</v>
+        <v>-1</v>
       </c>
       <c r="Z78">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
       <c r="AA78">
-        <v>0.9750000000000001</v>
+        <v>-0.5</v>
       </c>
       <c r="AB78">
-        <v>-1</v>
+        <v>0.4125</v>
       </c>
     </row>
     <row r="79" spans="1:28">
@@ -7211,58 +7208,58 @@
         <v>77</v>
       </c>
       <c r="B79">
-        <v>6240263</v>
+        <v>6227880</v>
       </c>
       <c r="C79" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D79" s="2">
-        <v>45199.75</v>
+        <v>45199.625</v>
       </c>
       <c r="E79" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F79" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="G79">
+        <v>2</v>
+      </c>
+      <c r="H79">
         <v>1</v>
       </c>
-      <c r="H79">
-        <v>2</v>
-      </c>
       <c r="I79" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J79">
-        <v>1.285</v>
+        <v>2.625</v>
       </c>
       <c r="K79">
-        <v>5</v>
+        <v>3.4</v>
       </c>
       <c r="L79">
-        <v>8.5</v>
+        <v>2.4</v>
       </c>
       <c r="M79">
-        <v>1.3</v>
+        <v>2.9</v>
       </c>
       <c r="N79">
-        <v>5.5</v>
+        <v>3.4</v>
       </c>
       <c r="O79">
-        <v>6</v>
+        <v>2.2</v>
       </c>
       <c r="P79">
-        <v>-1.5</v>
+        <v>0.25</v>
       </c>
       <c r="Q79">
-        <v>1.775</v>
+        <v>1.875</v>
       </c>
       <c r="R79">
         <v>1.925</v>
       </c>
       <c r="S79">
-        <v>3.25</v>
+        <v>2.5</v>
       </c>
       <c r="T79">
         <v>1.975</v>
@@ -7271,25 +7268,25 @@
         <v>1.825</v>
       </c>
       <c r="V79">
-        <v>-1</v>
+        <v>1.9</v>
       </c>
       <c r="W79">
         <v>-1</v>
       </c>
       <c r="X79">
-        <v>5</v>
+        <v>-1</v>
       </c>
       <c r="Y79">
-        <v>-1</v>
+        <v>0.875</v>
       </c>
       <c r="Z79">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
       <c r="AA79">
-        <v>-0.5</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AB79">
-        <v>0.4125</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="80" spans="1:28">
@@ -7300,16 +7297,16 @@
         <v>6227881</v>
       </c>
       <c r="C80" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D80" s="2">
         <v>45200.58333333334</v>
       </c>
       <c r="E80" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F80" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G80">
         <v>1</v>
@@ -7318,7 +7315,7 @@
         <v>0</v>
       </c>
       <c r="I80" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J80">
         <v>2.375</v>
@@ -7383,64 +7380,64 @@
         <v>79</v>
       </c>
       <c r="B81">
-        <v>6227882</v>
+        <v>6240262</v>
       </c>
       <c r="C81" t="s">
+        <v>27</v>
+      </c>
+      <c r="D81" s="2">
+        <v>45205.97916666666</v>
+      </c>
+      <c r="E81" t="s">
         <v>28</v>
       </c>
-      <c r="D81" s="2">
-        <v>45205.85416666666</v>
-      </c>
-      <c r="E81" t="s">
+      <c r="F81" t="s">
         <v>32</v>
       </c>
-      <c r="F81" t="s">
-        <v>34</v>
-      </c>
       <c r="G81">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H81">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I81" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J81">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="K81">
-        <v>3.2</v>
+        <v>3.4</v>
       </c>
       <c r="L81">
-        <v>2.3</v>
+        <v>2.05</v>
       </c>
       <c r="M81">
-        <v>2.7</v>
+        <v>3.1</v>
       </c>
       <c r="N81">
+        <v>3.6</v>
+      </c>
+      <c r="O81">
+        <v>1.95</v>
+      </c>
+      <c r="P81">
+        <v>0.5</v>
+      </c>
+      <c r="Q81">
+        <v>1.825</v>
+      </c>
+      <c r="R81">
+        <v>1.975</v>
+      </c>
+      <c r="S81">
         <v>3.25</v>
       </c>
-      <c r="O81">
-        <v>2.3</v>
-      </c>
-      <c r="P81">
-        <v>0.25</v>
-      </c>
-      <c r="Q81">
-        <v>1.75</v>
-      </c>
-      <c r="R81">
-        <v>2.05</v>
-      </c>
-      <c r="S81">
-        <v>2.5</v>
-      </c>
       <c r="T81">
-        <v>1.825</v>
+        <v>1.95</v>
       </c>
       <c r="U81">
-        <v>1.975</v>
+        <v>1.85</v>
       </c>
       <c r="V81">
         <v>-1</v>
@@ -7449,19 +7446,19 @@
         <v>-1</v>
       </c>
       <c r="X81">
-        <v>1.3</v>
+        <v>0.95</v>
       </c>
       <c r="Y81">
         <v>-1</v>
       </c>
       <c r="Z81">
-        <v>1.05</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AA81">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="AB81">
-        <v>0.9750000000000001</v>
+        <v>0.425</v>
       </c>
     </row>
     <row r="82" spans="1:28">
@@ -7469,65 +7466,65 @@
         <v>80</v>
       </c>
       <c r="B82">
-        <v>6240262</v>
+        <v>6227882</v>
       </c>
       <c r="C82" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D82" s="2">
-        <v>45205.97916666666</v>
+        <v>45205.85416666666</v>
       </c>
       <c r="E82" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F82" t="s">
         <v>33</v>
       </c>
       <c r="G82">
+        <v>0</v>
+      </c>
+      <c r="H82">
         <v>1</v>
       </c>
-      <c r="H82">
-        <v>2</v>
-      </c>
       <c r="I82" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J82">
-        <v>3</v>
+        <v>2.75</v>
       </c>
       <c r="K82">
-        <v>3.4</v>
+        <v>3.2</v>
       </c>
       <c r="L82">
+        <v>2.3</v>
+      </c>
+      <c r="M82">
+        <v>2.7</v>
+      </c>
+      <c r="N82">
+        <v>3.25</v>
+      </c>
+      <c r="O82">
+        <v>2.3</v>
+      </c>
+      <c r="P82">
+        <v>0.25</v>
+      </c>
+      <c r="Q82">
+        <v>1.75</v>
+      </c>
+      <c r="R82">
         <v>2.05</v>
       </c>
-      <c r="M82">
-        <v>3.1</v>
-      </c>
-      <c r="N82">
-        <v>3.6</v>
-      </c>
-      <c r="O82">
-        <v>1.95</v>
-      </c>
-      <c r="P82">
-        <v>0.5</v>
-      </c>
-      <c r="Q82">
+      <c r="S82">
+        <v>2.5</v>
+      </c>
+      <c r="T82">
         <v>1.825</v>
       </c>
-      <c r="R82">
+      <c r="U82">
         <v>1.975</v>
       </c>
-      <c r="S82">
-        <v>3.25</v>
-      </c>
-      <c r="T82">
-        <v>1.95</v>
-      </c>
-      <c r="U82">
-        <v>1.85</v>
-      </c>
       <c r="V82">
         <v>-1</v>
       </c>
@@ -7535,19 +7532,19 @@
         <v>-1</v>
       </c>
       <c r="X82">
-        <v>0.95</v>
+        <v>1.3</v>
       </c>
       <c r="Y82">
         <v>-1</v>
       </c>
       <c r="Z82">
+        <v>1.05</v>
+      </c>
+      <c r="AA82">
+        <v>-1</v>
+      </c>
+      <c r="AB82">
         <v>0.9750000000000001</v>
-      </c>
-      <c r="AA82">
-        <v>-0.5</v>
-      </c>
-      <c r="AB82">
-        <v>0.425</v>
       </c>
     </row>
     <row r="83" spans="1:28">
@@ -7558,16 +7555,16 @@
         <v>6227884</v>
       </c>
       <c r="C83" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D83" s="2">
         <v>45206.75</v>
       </c>
       <c r="E83" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F83" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G83">
         <v>3</v>
@@ -7576,7 +7573,7 @@
         <v>0</v>
       </c>
       <c r="I83" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J83">
         <v>2.25</v>
@@ -7644,16 +7641,16 @@
         <v>7301364</v>
       </c>
       <c r="C84" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D84" s="2">
         <v>45206.75</v>
       </c>
       <c r="E84" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F84" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G84">
         <v>0</v>
@@ -7662,7 +7659,7 @@
         <v>1</v>
       </c>
       <c r="I84" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J84">
         <v>1.8</v>
@@ -7730,16 +7727,16 @@
         <v>7314312</v>
       </c>
       <c r="C85" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D85" s="2">
         <v>45210.95833333334</v>
       </c>
       <c r="E85" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F85" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G85">
         <v>1</v>
@@ -7748,7 +7745,7 @@
         <v>0</v>
       </c>
       <c r="I85" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J85">
         <v>1.727</v>
@@ -7813,55 +7810,55 @@
         <v>84</v>
       </c>
       <c r="B86">
-        <v>7334555</v>
+        <v>7314311</v>
       </c>
       <c r="C86" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D86" s="2">
-        <v>45213.625</v>
+        <v>45213.75</v>
       </c>
       <c r="E86" t="s">
+        <v>29</v>
+      </c>
+      <c r="F86" t="s">
         <v>34</v>
       </c>
-      <c r="F86" t="s">
+      <c r="G86">
+        <v>1</v>
+      </c>
+      <c r="H86">
+        <v>2</v>
+      </c>
+      <c r="I86" t="s">
         <v>36</v>
       </c>
-      <c r="G86">
-        <v>0</v>
-      </c>
-      <c r="H86">
-        <v>1</v>
-      </c>
-      <c r="I86" t="s">
-        <v>37</v>
-      </c>
       <c r="J86">
-        <v>2.6</v>
+        <v>2.3</v>
       </c>
       <c r="K86">
         <v>3.2</v>
       </c>
       <c r="L86">
-        <v>2.375</v>
+        <v>2.7</v>
       </c>
       <c r="M86">
-        <v>2.6</v>
+        <v>2.1</v>
       </c>
       <c r="N86">
         <v>3.2</v>
       </c>
       <c r="O86">
-        <v>2.375</v>
+        <v>3.1</v>
       </c>
       <c r="P86">
-        <v>0</v>
+        <v>-0.25</v>
       </c>
       <c r="Q86">
-        <v>2</v>
+        <v>1.875</v>
       </c>
       <c r="R86">
-        <v>1.8</v>
+        <v>1.925</v>
       </c>
       <c r="S86">
         <v>2.5</v>
@@ -7879,19 +7876,19 @@
         <v>-1</v>
       </c>
       <c r="X86">
-        <v>1.375</v>
+        <v>2.1</v>
       </c>
       <c r="Y86">
         <v>-1</v>
       </c>
       <c r="Z86">
-        <v>0.8</v>
+        <v>0.925</v>
       </c>
       <c r="AA86">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="AB86">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="87" spans="1:28">
@@ -7899,55 +7896,55 @@
         <v>85</v>
       </c>
       <c r="B87">
-        <v>7314311</v>
+        <v>7334555</v>
       </c>
       <c r="C87" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D87" s="2">
-        <v>45213.75</v>
+        <v>45213.625</v>
       </c>
       <c r="E87" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F87" t="s">
         <v>35</v>
       </c>
       <c r="G87">
+        <v>0</v>
+      </c>
+      <c r="H87">
         <v>1</v>
       </c>
-      <c r="H87">
-        <v>2</v>
-      </c>
       <c r="I87" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J87">
-        <v>2.3</v>
+        <v>2.6</v>
       </c>
       <c r="K87">
         <v>3.2</v>
       </c>
       <c r="L87">
-        <v>2.7</v>
+        <v>2.375</v>
       </c>
       <c r="M87">
-        <v>2.1</v>
+        <v>2.6</v>
       </c>
       <c r="N87">
         <v>3.2</v>
       </c>
       <c r="O87">
-        <v>3.1</v>
+        <v>2.375</v>
       </c>
       <c r="P87">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
       <c r="Q87">
-        <v>1.875</v>
+        <v>2</v>
       </c>
       <c r="R87">
-        <v>1.925</v>
+        <v>1.8</v>
       </c>
       <c r="S87">
         <v>2.5</v>
@@ -7965,19 +7962,19 @@
         <v>-1</v>
       </c>
       <c r="X87">
-        <v>2.1</v>
+        <v>1.375</v>
       </c>
       <c r="Y87">
         <v>-1</v>
       </c>
       <c r="Z87">
-        <v>0.925</v>
+        <v>0.8</v>
       </c>
       <c r="AA87">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AB87">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
     </row>
     <row r="88" spans="1:28">
@@ -7988,16 +7985,16 @@
         <v>7373916</v>
       </c>
       <c r="C88" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D88" s="2">
         <v>45227.79166666666</v>
       </c>
       <c r="E88" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F88" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G88">
         <v>2</v>
@@ -8006,7 +8003,7 @@
         <v>1</v>
       </c>
       <c r="I88" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J88">
         <v>2.2</v>
@@ -8071,67 +8068,67 @@
         <v>87</v>
       </c>
       <c r="B89">
-        <v>7802934</v>
+        <v>7803361</v>
       </c>
       <c r="C89" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D89" s="2">
-        <v>45395.58333333334</v>
+        <v>45395.83333333334</v>
       </c>
       <c r="E89" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="F89" t="s">
         <v>33</v>
       </c>
       <c r="G89">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H89">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I89" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J89">
-        <v>2.875</v>
+        <v>1.833</v>
       </c>
       <c r="K89">
+        <v>3.5</v>
+      </c>
+      <c r="L89">
+        <v>3.5</v>
+      </c>
+      <c r="M89">
+        <v>1.95</v>
+      </c>
+      <c r="N89">
+        <v>3.25</v>
+      </c>
+      <c r="O89">
         <v>3.4</v>
       </c>
-      <c r="L89">
-        <v>2.1</v>
-      </c>
-      <c r="M89">
-        <v>2.4</v>
-      </c>
-      <c r="N89">
-        <v>3.4</v>
-      </c>
-      <c r="O89">
-        <v>2.5</v>
-      </c>
       <c r="P89">
-        <v>0</v>
+        <v>-0.25</v>
       </c>
       <c r="Q89">
-        <v>1.85</v>
+        <v>1.775</v>
       </c>
       <c r="R89">
-        <v>1.95</v>
+        <v>2.025</v>
       </c>
       <c r="S89">
-        <v>2.5</v>
+        <v>2.25</v>
       </c>
       <c r="T89">
-        <v>2</v>
+        <v>1.875</v>
       </c>
       <c r="U89">
-        <v>1.8</v>
+        <v>1.925</v>
       </c>
       <c r="V89">
-        <v>1.4</v>
+        <v>0.95</v>
       </c>
       <c r="W89">
         <v>-1</v>
@@ -8140,16 +8137,16 @@
         <v>-1</v>
       </c>
       <c r="Y89">
-        <v>0.8500000000000001</v>
+        <v>0.7749999999999999</v>
       </c>
       <c r="Z89">
         <v>-1</v>
       </c>
       <c r="AA89">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AB89">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="90" spans="1:28">
@@ -8160,16 +8157,16 @@
         <v>7802874</v>
       </c>
       <c r="C90" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D90" s="2">
         <v>45395.70833333334</v>
       </c>
       <c r="E90" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F90" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G90">
         <v>2</v>
@@ -8178,7 +8175,7 @@
         <v>1</v>
       </c>
       <c r="I90" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J90">
         <v>2.2</v>
@@ -8243,67 +8240,67 @@
         <v>89</v>
       </c>
       <c r="B91">
-        <v>7803361</v>
+        <v>7802934</v>
       </c>
       <c r="C91" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D91" s="2">
-        <v>45395.83333333334</v>
+        <v>45395.58333333334</v>
       </c>
       <c r="E91" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="F91" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G91">
+        <v>2</v>
+      </c>
+      <c r="H91">
         <v>1</v>
       </c>
-      <c r="H91">
-        <v>0</v>
-      </c>
       <c r="I91" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J91">
-        <v>1.833</v>
+        <v>2.875</v>
       </c>
       <c r="K91">
-        <v>3.5</v>
+        <v>3.4</v>
       </c>
       <c r="L91">
-        <v>3.5</v>
+        <v>2.1</v>
       </c>
       <c r="M91">
+        <v>2.4</v>
+      </c>
+      <c r="N91">
+        <v>3.4</v>
+      </c>
+      <c r="O91">
+        <v>2.5</v>
+      </c>
+      <c r="P91">
+        <v>0</v>
+      </c>
+      <c r="Q91">
+        <v>1.85</v>
+      </c>
+      <c r="R91">
         <v>1.95</v>
       </c>
-      <c r="N91">
-        <v>3.25</v>
-      </c>
-      <c r="O91">
-        <v>3.4</v>
-      </c>
-      <c r="P91">
-        <v>-0.25</v>
-      </c>
-      <c r="Q91">
-        <v>1.775</v>
-      </c>
-      <c r="R91">
-        <v>2.025</v>
-      </c>
       <c r="S91">
-        <v>2.25</v>
+        <v>2.5</v>
       </c>
       <c r="T91">
-        <v>1.875</v>
+        <v>2</v>
       </c>
       <c r="U91">
-        <v>1.925</v>
+        <v>1.8</v>
       </c>
       <c r="V91">
-        <v>0.95</v>
+        <v>1.4</v>
       </c>
       <c r="W91">
         <v>-1</v>
@@ -8312,16 +8309,16 @@
         <v>-1</v>
       </c>
       <c r="Y91">
-        <v>0.7749999999999999</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="Z91">
         <v>-1</v>
       </c>
       <c r="AA91">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AB91">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="92" spans="1:28">
@@ -8332,16 +8329,16 @@
         <v>7803362</v>
       </c>
       <c r="C92" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D92" s="2">
         <v>45396.83333333334</v>
       </c>
       <c r="E92" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F92" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G92">
         <v>4</v>
@@ -8350,7 +8347,7 @@
         <v>1</v>
       </c>
       <c r="I92" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J92">
         <v>2.4</v>
@@ -8418,16 +8415,16 @@
         <v>7803363</v>
       </c>
       <c r="C93" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D93" s="2">
         <v>45400.95833333334</v>
       </c>
       <c r="E93" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F93" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G93">
         <v>2</v>
@@ -8436,7 +8433,7 @@
         <v>0</v>
       </c>
       <c r="I93" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J93">
         <v>3.1</v>
@@ -8504,16 +8501,16 @@
         <v>7802935</v>
       </c>
       <c r="C94" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D94" s="2">
         <v>45401.95833333334</v>
       </c>
       <c r="E94" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F94" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G94">
         <v>2</v>
@@ -8522,7 +8519,7 @@
         <v>0</v>
       </c>
       <c r="I94" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J94">
         <v>1.727</v>
@@ -8590,16 +8587,16 @@
         <v>7802936</v>
       </c>
       <c r="C95" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D95" s="2">
         <v>45402.625</v>
       </c>
       <c r="E95" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F95" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G95">
         <v>1</v>
@@ -8608,7 +8605,7 @@
         <v>1</v>
       </c>
       <c r="I95" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J95">
         <v>3.1</v>
@@ -8676,16 +8673,16 @@
         <v>7802875</v>
       </c>
       <c r="C96" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D96" s="2">
         <v>45403.70833333334</v>
       </c>
       <c r="E96" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F96" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G96">
         <v>0</v>
@@ -8694,7 +8691,7 @@
         <v>3</v>
       </c>
       <c r="I96" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J96">
         <v>2.8</v>
@@ -8762,16 +8759,16 @@
         <v>7802937</v>
       </c>
       <c r="C97" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D97" s="2">
         <v>45408.83333333334</v>
       </c>
       <c r="E97" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F97" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G97">
         <v>3</v>
@@ -8780,7 +8777,7 @@
         <v>0</v>
       </c>
       <c r="I97" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J97">
         <v>2.2</v>
@@ -8844,65 +8841,172 @@
       <c r="A98" s="1">
         <v>96</v>
       </c>
-      <c r="B98" t="s">
-        <v>27</v>
+      <c r="B98">
+        <v>7802876</v>
       </c>
       <c r="C98" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D98" s="2">
-        <v>45410.75</v>
+        <v>45409.70833333334</v>
       </c>
       <c r="E98" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="F98" t="s">
-        <v>36</v>
+        <v>31</v>
+      </c>
+      <c r="G98">
+        <v>2</v>
+      </c>
+      <c r="H98">
+        <v>1</v>
+      </c>
+      <c r="I98" t="s">
+        <v>38</v>
       </c>
       <c r="J98">
-        <v>2</v>
+        <v>1.6</v>
       </c>
       <c r="K98">
-        <v>3.2</v>
+        <v>3.75</v>
       </c>
       <c r="L98">
-        <v>3.3</v>
+        <v>4.5</v>
       </c>
       <c r="M98">
-        <v>1.8</v>
+        <v>1.4</v>
       </c>
       <c r="N98">
-        <v>3.3</v>
+        <v>4</v>
       </c>
       <c r="O98">
-        <v>3.8</v>
+        <v>6.5</v>
       </c>
       <c r="P98">
-        <v>-0.5</v>
+        <v>-1.25</v>
       </c>
       <c r="Q98">
-        <v>1.875</v>
+        <v>1.9</v>
       </c>
       <c r="R98">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="S98">
         <v>2.5</v>
       </c>
       <c r="T98">
+        <v>1.8</v>
+      </c>
+      <c r="U98">
+        <v>2</v>
+      </c>
+      <c r="V98">
+        <v>0.3999999999999999</v>
+      </c>
+      <c r="W98">
+        <v>-1</v>
+      </c>
+      <c r="X98">
+        <v>-1</v>
+      </c>
+      <c r="Y98">
+        <v>-0.5</v>
+      </c>
+      <c r="Z98">
+        <v>0.45</v>
+      </c>
+      <c r="AA98">
+        <v>0.8</v>
+      </c>
+      <c r="AB98">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:28">
+      <c r="A99" s="1">
+        <v>97</v>
+      </c>
+      <c r="B99">
+        <v>7802938</v>
+      </c>
+      <c r="C99" t="s">
+        <v>27</v>
+      </c>
+      <c r="D99" s="2">
+        <v>45409.58333333334</v>
+      </c>
+      <c r="E99" t="s">
+        <v>33</v>
+      </c>
+      <c r="F99" t="s">
+        <v>30</v>
+      </c>
+      <c r="G99">
+        <v>1</v>
+      </c>
+      <c r="H99">
+        <v>3</v>
+      </c>
+      <c r="I99" t="s">
+        <v>36</v>
+      </c>
+      <c r="J99">
+        <v>2</v>
+      </c>
+      <c r="K99">
+        <v>3.3</v>
+      </c>
+      <c r="L99">
+        <v>3.2</v>
+      </c>
+      <c r="M99">
+        <v>2.25</v>
+      </c>
+      <c r="N99">
+        <v>3.1</v>
+      </c>
+      <c r="O99">
+        <v>2.875</v>
+      </c>
+      <c r="P99">
+        <v>-0.25</v>
+      </c>
+      <c r="Q99">
+        <v>2.025</v>
+      </c>
+      <c r="R99">
+        <v>1.775</v>
+      </c>
+      <c r="S99">
+        <v>2.25</v>
+      </c>
+      <c r="T99">
+        <v>1.95</v>
+      </c>
+      <c r="U99">
         <v>1.85</v>
       </c>
-      <c r="U98">
-        <v>1.95</v>
-      </c>
-      <c r="V98">
-        <v>0</v>
-      </c>
-      <c r="W98">
-        <v>0</v>
-      </c>
-      <c r="X98">
-        <v>0</v>
+      <c r="V99">
+        <v>-1</v>
+      </c>
+      <c r="W99">
+        <v>-1</v>
+      </c>
+      <c r="X99">
+        <v>1.875</v>
+      </c>
+      <c r="Y99">
+        <v>-1</v>
+      </c>
+      <c r="Z99">
+        <v>0.7749999999999999</v>
+      </c>
+      <c r="AA99">
+        <v>0.95</v>
+      </c>
+      <c r="AB99">
+        <v>-1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 30-04-2024 às 00:25
</commit_message>
<xml_diff>
--- a/Canada Premier League/Canada Premier League.xlsx
+++ b/Canada Premier League/Canada Premier League.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="39">
   <si>
     <t>id</t>
   </si>
@@ -492,7 +492,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AB99"/>
+  <dimension ref="A1:AB100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1704,49 +1704,49 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>6227818</v>
+        <v>6227817</v>
       </c>
       <c r="C15" t="s">
         <v>27</v>
       </c>
       <c r="D15" s="2">
-        <v>45098.95833333334</v>
+        <v>45098.83333333334</v>
       </c>
       <c r="E15" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F15" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H15">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J15">
-        <v>1.666</v>
+        <v>2.5</v>
       </c>
       <c r="K15">
-        <v>3.4</v>
+        <v>2.9</v>
       </c>
       <c r="L15">
-        <v>5</v>
+        <v>2.875</v>
       </c>
       <c r="M15">
-        <v>1.533</v>
+        <v>2.25</v>
       </c>
       <c r="N15">
-        <v>3.6</v>
+        <v>3.1</v>
       </c>
       <c r="O15">
-        <v>6</v>
+        <v>3.2</v>
       </c>
       <c r="P15">
-        <v>-1</v>
+        <v>-0.25</v>
       </c>
       <c r="Q15">
         <v>1.95</v>
@@ -1758,31 +1758,31 @@
         <v>2.25</v>
       </c>
       <c r="T15">
-        <v>1.8</v>
+        <v>1.875</v>
       </c>
       <c r="U15">
-        <v>2</v>
+        <v>1.925</v>
       </c>
       <c r="V15">
-        <v>0.5329999999999999</v>
+        <v>-1</v>
       </c>
       <c r="W15">
-        <v>-1</v>
+        <v>2.1</v>
       </c>
       <c r="X15">
         <v>-1</v>
       </c>
       <c r="Y15">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="Z15">
-        <v>0</v>
+        <v>0.425</v>
       </c>
       <c r="AA15">
-        <v>-1</v>
+        <v>0.875</v>
       </c>
       <c r="AB15">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="16" spans="1:28">
@@ -1790,49 +1790,49 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>6227817</v>
+        <v>6227818</v>
       </c>
       <c r="C16" t="s">
         <v>27</v>
       </c>
       <c r="D16" s="2">
-        <v>45098.83333333334</v>
+        <v>45098.95833333334</v>
       </c>
       <c r="E16" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J16">
-        <v>2.5</v>
+        <v>1.666</v>
       </c>
       <c r="K16">
-        <v>2.9</v>
+        <v>3.4</v>
       </c>
       <c r="L16">
-        <v>2.875</v>
+        <v>5</v>
       </c>
       <c r="M16">
-        <v>2.25</v>
+        <v>1.533</v>
       </c>
       <c r="N16">
-        <v>3.1</v>
+        <v>3.6</v>
       </c>
       <c r="O16">
-        <v>3.2</v>
+        <v>6</v>
       </c>
       <c r="P16">
-        <v>-0.25</v>
+        <v>-1</v>
       </c>
       <c r="Q16">
         <v>1.95</v>
@@ -1844,31 +1844,31 @@
         <v>2.25</v>
       </c>
       <c r="T16">
-        <v>1.875</v>
+        <v>1.8</v>
       </c>
       <c r="U16">
-        <v>1.925</v>
+        <v>2</v>
       </c>
       <c r="V16">
-        <v>-1</v>
+        <v>0.5329999999999999</v>
       </c>
       <c r="W16">
-        <v>2.1</v>
+        <v>-1</v>
       </c>
       <c r="X16">
         <v>-1</v>
       </c>
       <c r="Y16">
-        <v>-0.5</v>
+        <v>0</v>
       </c>
       <c r="Z16">
-        <v>0.425</v>
+        <v>0</v>
       </c>
       <c r="AA16">
-        <v>0.875</v>
+        <v>-1</v>
       </c>
       <c r="AB16">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:28">
@@ -2134,82 +2134,82 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>6227821</v>
+        <v>6227822</v>
       </c>
       <c r="C20" t="s">
         <v>27</v>
       </c>
       <c r="D20" s="2">
-        <v>45107.79166666666</v>
+        <v>45107.9375</v>
       </c>
       <c r="E20" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F20" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G20">
         <v>2</v>
       </c>
       <c r="H20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J20">
+        <v>1.727</v>
+      </c>
+      <c r="K20">
+        <v>3.4</v>
+      </c>
+      <c r="L20">
+        <v>4.333</v>
+      </c>
+      <c r="M20">
+        <v>1.833</v>
+      </c>
+      <c r="N20">
+        <v>3.4</v>
+      </c>
+      <c r="O20">
+        <v>4</v>
+      </c>
+      <c r="P20">
+        <v>-0.5</v>
+      </c>
+      <c r="Q20">
+        <v>1.85</v>
+      </c>
+      <c r="R20">
+        <v>1.95</v>
+      </c>
+      <c r="S20">
+        <v>2.5</v>
+      </c>
+      <c r="T20">
+        <v>2.075</v>
+      </c>
+      <c r="U20">
+        <v>1.725</v>
+      </c>
+      <c r="V20">
+        <v>-1</v>
+      </c>
+      <c r="W20">
         <v>2.4</v>
       </c>
-      <c r="K20">
-        <v>3</v>
-      </c>
-      <c r="L20">
-        <v>2.75</v>
-      </c>
-      <c r="M20">
-        <v>2.75</v>
-      </c>
-      <c r="N20">
-        <v>2.9</v>
-      </c>
-      <c r="O20">
-        <v>2.4</v>
-      </c>
-      <c r="P20">
-        <v>0</v>
-      </c>
-      <c r="Q20">
-        <v>2.025</v>
-      </c>
-      <c r="R20">
-        <v>1.775</v>
-      </c>
-      <c r="S20">
-        <v>2.25</v>
-      </c>
-      <c r="T20">
-        <v>1.8</v>
-      </c>
-      <c r="U20">
-        <v>2</v>
-      </c>
-      <c r="V20">
-        <v>1.75</v>
-      </c>
-      <c r="W20">
-        <v>-1</v>
-      </c>
       <c r="X20">
         <v>-1</v>
       </c>
       <c r="Y20">
-        <v>1.025</v>
+        <v>-1</v>
       </c>
       <c r="Z20">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="AA20">
-        <v>0.8</v>
+        <v>1.075</v>
       </c>
       <c r="AB20">
         <v>-1</v>
@@ -2220,82 +2220,82 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>6227822</v>
+        <v>6227821</v>
       </c>
       <c r="C21" t="s">
         <v>27</v>
       </c>
       <c r="D21" s="2">
-        <v>45107.9375</v>
+        <v>45107.79166666666</v>
       </c>
       <c r="E21" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F21" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="G21">
         <v>2</v>
       </c>
       <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21" t="s">
+        <v>38</v>
+      </c>
+      <c r="J21">
+        <v>2.4</v>
+      </c>
+      <c r="K21">
+        <v>3</v>
+      </c>
+      <c r="L21">
+        <v>2.75</v>
+      </c>
+      <c r="M21">
+        <v>2.75</v>
+      </c>
+      <c r="N21">
+        <v>2.9</v>
+      </c>
+      <c r="O21">
+        <v>2.4</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>2.025</v>
+      </c>
+      <c r="R21">
+        <v>1.775</v>
+      </c>
+      <c r="S21">
+        <v>2.25</v>
+      </c>
+      <c r="T21">
+        <v>1.8</v>
+      </c>
+      <c r="U21">
         <v>2</v>
       </c>
-      <c r="I21" t="s">
-        <v>37</v>
-      </c>
-      <c r="J21">
-        <v>1.727</v>
-      </c>
-      <c r="K21">
-        <v>3.4</v>
-      </c>
-      <c r="L21">
-        <v>4.333</v>
-      </c>
-      <c r="M21">
-        <v>1.833</v>
-      </c>
-      <c r="N21">
-        <v>3.4</v>
-      </c>
-      <c r="O21">
-        <v>4</v>
-      </c>
-      <c r="P21">
-        <v>-0.5</v>
-      </c>
-      <c r="Q21">
-        <v>1.85</v>
-      </c>
-      <c r="R21">
-        <v>1.95</v>
-      </c>
-      <c r="S21">
-        <v>2.5</v>
-      </c>
-      <c r="T21">
-        <v>2.075</v>
-      </c>
-      <c r="U21">
-        <v>1.725</v>
-      </c>
       <c r="V21">
-        <v>-1</v>
+        <v>1.75</v>
       </c>
       <c r="W21">
-        <v>2.4</v>
+        <v>-1</v>
       </c>
       <c r="X21">
         <v>-1</v>
       </c>
       <c r="Y21">
-        <v>-1</v>
+        <v>1.025</v>
       </c>
       <c r="Z21">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AA21">
-        <v>1.075</v>
+        <v>0.8</v>
       </c>
       <c r="AB21">
         <v>-1</v>
@@ -3080,85 +3080,85 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>6227830</v>
+        <v>6227831</v>
       </c>
       <c r="C31" t="s">
         <v>27</v>
       </c>
       <c r="D31" s="2">
-        <v>45122.70833333334</v>
+        <v>45122.83333333334</v>
       </c>
       <c r="E31" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="F31" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G31">
         <v>1</v>
       </c>
       <c r="H31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I31" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J31">
-        <v>2.1</v>
+        <v>1.909</v>
       </c>
       <c r="K31">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="L31">
-        <v>3.25</v>
+        <v>3.5</v>
       </c>
       <c r="M31">
+        <v>1.7</v>
+      </c>
+      <c r="N31">
+        <v>3.5</v>
+      </c>
+      <c r="O31">
+        <v>4.2</v>
+      </c>
+      <c r="P31">
+        <v>-0.75</v>
+      </c>
+      <c r="Q31">
+        <v>1.85</v>
+      </c>
+      <c r="R31">
         <v>1.95</v>
       </c>
-      <c r="N31">
-        <v>3</v>
-      </c>
-      <c r="O31">
-        <v>3.75</v>
-      </c>
-      <c r="P31">
-        <v>-0.5</v>
-      </c>
-      <c r="Q31">
-        <v>1.975</v>
-      </c>
-      <c r="R31">
-        <v>1.825</v>
-      </c>
       <c r="S31">
-        <v>2.25</v>
+        <v>2.5</v>
       </c>
       <c r="T31">
-        <v>1.85</v>
+        <v>1.9</v>
       </c>
       <c r="U31">
-        <v>1.95</v>
+        <v>1.9</v>
       </c>
       <c r="V31">
+        <v>-1</v>
+      </c>
+      <c r="W31">
+        <v>2.5</v>
+      </c>
+      <c r="X31">
+        <v>-1</v>
+      </c>
+      <c r="Y31">
+        <v>-1</v>
+      </c>
+      <c r="Z31">
         <v>0.95</v>
       </c>
-      <c r="W31">
-        <v>-1</v>
-      </c>
-      <c r="X31">
-        <v>-1</v>
-      </c>
-      <c r="Y31">
-        <v>0.9750000000000001</v>
-      </c>
-      <c r="Z31">
-        <v>-1</v>
-      </c>
       <c r="AA31">
         <v>-1</v>
       </c>
       <c r="AB31">
-        <v>0.95</v>
+        <v>0.8999999999999999</v>
       </c>
     </row>
     <row r="32" spans="1:28">
@@ -3166,85 +3166,85 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>6227831</v>
+        <v>6227830</v>
       </c>
       <c r="C32" t="s">
         <v>27</v>
       </c>
       <c r="D32" s="2">
-        <v>45122.83333333334</v>
+        <v>45122.70833333334</v>
       </c>
       <c r="E32" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="F32" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G32">
         <v>1</v>
       </c>
       <c r="H32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I32" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J32">
-        <v>1.909</v>
+        <v>2.1</v>
       </c>
       <c r="K32">
+        <v>3</v>
+      </c>
+      <c r="L32">
         <v>3.25</v>
       </c>
-      <c r="L32">
-        <v>3.5</v>
-      </c>
       <c r="M32">
-        <v>1.7</v>
+        <v>1.95</v>
       </c>
       <c r="N32">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="O32">
-        <v>4.2</v>
+        <v>3.75</v>
       </c>
       <c r="P32">
-        <v>-0.75</v>
+        <v>-0.5</v>
       </c>
       <c r="Q32">
+        <v>1.975</v>
+      </c>
+      <c r="R32">
+        <v>1.825</v>
+      </c>
+      <c r="S32">
+        <v>2.25</v>
+      </c>
+      <c r="T32">
         <v>1.85</v>
       </c>
-      <c r="R32">
+      <c r="U32">
         <v>1.95</v>
       </c>
-      <c r="S32">
-        <v>2.5</v>
-      </c>
-      <c r="T32">
-        <v>1.9</v>
-      </c>
-      <c r="U32">
-        <v>1.9</v>
-      </c>
       <c r="V32">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="W32">
-        <v>2.5</v>
+        <v>-1</v>
       </c>
       <c r="X32">
         <v>-1</v>
       </c>
       <c r="Y32">
-        <v>-1</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="Z32">
+        <v>-1</v>
+      </c>
+      <c r="AA32">
+        <v>-1</v>
+      </c>
+      <c r="AB32">
         <v>0.95</v>
-      </c>
-      <c r="AA32">
-        <v>-1</v>
-      </c>
-      <c r="AB32">
-        <v>0.8999999999999999</v>
       </c>
     </row>
     <row r="33" spans="1:28">
@@ -5918,85 +5918,85 @@
         <v>62</v>
       </c>
       <c r="B64">
-        <v>6227870</v>
+        <v>6240267</v>
       </c>
       <c r="C64" t="s">
         <v>27</v>
       </c>
       <c r="D64" s="2">
-        <v>45178.83333333334</v>
+        <v>45178.95833333334</v>
       </c>
       <c r="E64" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F64" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G64">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H64">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I64" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J64">
+        <v>3.5</v>
+      </c>
+      <c r="K64">
+        <v>3.5</v>
+      </c>
+      <c r="L64">
+        <v>1.85</v>
+      </c>
+      <c r="M64">
+        <v>3.3</v>
+      </c>
+      <c r="N64">
+        <v>3.6</v>
+      </c>
+      <c r="O64">
         <v>1.909</v>
       </c>
-      <c r="K64">
-        <v>3.4</v>
-      </c>
-      <c r="L64">
-        <v>3.4</v>
-      </c>
-      <c r="M64">
-        <v>2.15</v>
-      </c>
-      <c r="N64">
-        <v>3.4</v>
-      </c>
-      <c r="O64">
-        <v>2.8</v>
-      </c>
       <c r="P64">
-        <v>-0.25</v>
+        <v>0.5</v>
       </c>
       <c r="Q64">
-        <v>1.825</v>
+        <v>1.9</v>
       </c>
       <c r="R64">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="S64">
         <v>2.5</v>
       </c>
       <c r="T64">
+        <v>1.75</v>
+      </c>
+      <c r="U64">
         <v>1.95</v>
       </c>
-      <c r="U64">
-        <v>1.85</v>
-      </c>
       <c r="V64">
-        <v>-1</v>
+        <v>2.3</v>
       </c>
       <c r="W64">
-        <v>2.4</v>
+        <v>-1</v>
       </c>
       <c r="X64">
         <v>-1</v>
       </c>
       <c r="Y64">
-        <v>-0.5</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="Z64">
-        <v>0.4875</v>
+        <v>-1</v>
       </c>
       <c r="AA64">
-        <v>-1</v>
+        <v>0.75</v>
       </c>
       <c r="AB64">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="65" spans="1:28">
@@ -6004,85 +6004,85 @@
         <v>63</v>
       </c>
       <c r="B65">
-        <v>6240267</v>
+        <v>6227870</v>
       </c>
       <c r="C65" t="s">
         <v>27</v>
       </c>
       <c r="D65" s="2">
-        <v>45178.95833333334</v>
+        <v>45178.83333333334</v>
       </c>
       <c r="E65" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F65" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G65">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H65">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I65" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J65">
-        <v>3.5</v>
+        <v>1.909</v>
       </c>
       <c r="K65">
-        <v>3.5</v>
+        <v>3.4</v>
       </c>
       <c r="L65">
-        <v>1.85</v>
+        <v>3.4</v>
       </c>
       <c r="M65">
-        <v>3.3</v>
+        <v>2.15</v>
       </c>
       <c r="N65">
-        <v>3.6</v>
+        <v>3.4</v>
       </c>
       <c r="O65">
-        <v>1.909</v>
+        <v>2.8</v>
       </c>
       <c r="P65">
-        <v>0.5</v>
+        <v>-0.25</v>
       </c>
       <c r="Q65">
-        <v>1.9</v>
+        <v>1.825</v>
       </c>
       <c r="R65">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="S65">
         <v>2.5</v>
       </c>
       <c r="T65">
-        <v>1.75</v>
+        <v>1.95</v>
       </c>
       <c r="U65">
-        <v>1.95</v>
+        <v>1.85</v>
       </c>
       <c r="V65">
-        <v>2.3</v>
+        <v>-1</v>
       </c>
       <c r="W65">
-        <v>-1</v>
+        <v>2.4</v>
       </c>
       <c r="X65">
         <v>-1</v>
       </c>
       <c r="Y65">
-        <v>0.8999999999999999</v>
+        <v>-0.5</v>
       </c>
       <c r="Z65">
-        <v>-1</v>
+        <v>0.4875</v>
       </c>
       <c r="AA65">
-        <v>0.75</v>
+        <v>-1</v>
       </c>
       <c r="AB65">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
     </row>
     <row r="66" spans="1:28">
@@ -6778,43 +6778,43 @@
         <v>72</v>
       </c>
       <c r="B74">
-        <v>6227876</v>
+        <v>6240264</v>
       </c>
       <c r="C74" t="s">
         <v>27</v>
       </c>
       <c r="D74" s="2">
-        <v>45192.58333333334</v>
+        <v>45192.70833333334</v>
       </c>
       <c r="E74" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F74" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="G74">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H74">
         <v>1</v>
       </c>
       <c r="I74" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="J74">
-        <v>3.6</v>
+        <v>3.75</v>
       </c>
       <c r="K74">
         <v>3.4</v>
       </c>
       <c r="L74">
-        <v>1.909</v>
+        <v>1.8</v>
       </c>
       <c r="M74">
-        <v>3.75</v>
+        <v>3.6</v>
       </c>
       <c r="N74">
-        <v>3.5</v>
+        <v>3.4</v>
       </c>
       <c r="O74">
         <v>1.833</v>
@@ -6823,40 +6823,40 @@
         <v>0.5</v>
       </c>
       <c r="Q74">
-        <v>1.9</v>
+        <v>1.925</v>
       </c>
       <c r="R74">
-        <v>1.9</v>
+        <v>1.875</v>
       </c>
       <c r="S74">
         <v>2.75</v>
       </c>
       <c r="T74">
-        <v>1.9</v>
+        <v>1.95</v>
       </c>
       <c r="U74">
-        <v>1.9</v>
+        <v>1.85</v>
       </c>
       <c r="V74">
-        <v>-1</v>
+        <v>2.6</v>
       </c>
       <c r="W74">
         <v>-1</v>
       </c>
       <c r="X74">
-        <v>0.833</v>
+        <v>-1</v>
       </c>
       <c r="Y74">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
       <c r="Z74">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AA74">
-        <v>-1</v>
+        <v>0.475</v>
       </c>
       <c r="AB74">
-        <v>0.8999999999999999</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="75" spans="1:28">
@@ -6864,43 +6864,43 @@
         <v>73</v>
       </c>
       <c r="B75">
-        <v>6240264</v>
+        <v>6227876</v>
       </c>
       <c r="C75" t="s">
         <v>27</v>
       </c>
       <c r="D75" s="2">
-        <v>45192.70833333334</v>
+        <v>45192.58333333334</v>
       </c>
       <c r="E75" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="F75" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="G75">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H75">
         <v>1</v>
       </c>
       <c r="I75" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J75">
-        <v>3.75</v>
+        <v>3.6</v>
       </c>
       <c r="K75">
         <v>3.4</v>
       </c>
       <c r="L75">
-        <v>1.8</v>
+        <v>1.909</v>
       </c>
       <c r="M75">
-        <v>3.6</v>
+        <v>3.75</v>
       </c>
       <c r="N75">
-        <v>3.4</v>
+        <v>3.5</v>
       </c>
       <c r="O75">
         <v>1.833</v>
@@ -6909,40 +6909,40 @@
         <v>0.5</v>
       </c>
       <c r="Q75">
-        <v>1.925</v>
+        <v>1.9</v>
       </c>
       <c r="R75">
-        <v>1.875</v>
+        <v>1.9</v>
       </c>
       <c r="S75">
         <v>2.75</v>
       </c>
       <c r="T75">
-        <v>1.95</v>
+        <v>1.9</v>
       </c>
       <c r="U75">
-        <v>1.85</v>
+        <v>1.9</v>
       </c>
       <c r="V75">
-        <v>2.6</v>
+        <v>-1</v>
       </c>
       <c r="W75">
         <v>-1</v>
       </c>
       <c r="X75">
-        <v>-1</v>
+        <v>0.833</v>
       </c>
       <c r="Y75">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
       <c r="Z75">
-        <v>-1</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AA75">
-        <v>0.475</v>
+        <v>-1</v>
       </c>
       <c r="AB75">
-        <v>-0.5</v>
+        <v>0.8999999999999999</v>
       </c>
     </row>
     <row r="76" spans="1:28">
@@ -7380,65 +7380,65 @@
         <v>79</v>
       </c>
       <c r="B81">
-        <v>6240262</v>
+        <v>6227882</v>
       </c>
       <c r="C81" t="s">
         <v>27</v>
       </c>
       <c r="D81" s="2">
-        <v>45205.97916666666</v>
+        <v>45205.85416666666</v>
       </c>
       <c r="E81" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F81" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G81">
+        <v>0</v>
+      </c>
+      <c r="H81">
         <v>1</v>
-      </c>
-      <c r="H81">
-        <v>2</v>
       </c>
       <c r="I81" t="s">
         <v>36</v>
       </c>
       <c r="J81">
-        <v>3</v>
+        <v>2.75</v>
       </c>
       <c r="K81">
-        <v>3.4</v>
+        <v>3.2</v>
       </c>
       <c r="L81">
+        <v>2.3</v>
+      </c>
+      <c r="M81">
+        <v>2.7</v>
+      </c>
+      <c r="N81">
+        <v>3.25</v>
+      </c>
+      <c r="O81">
+        <v>2.3</v>
+      </c>
+      <c r="P81">
+        <v>0.25</v>
+      </c>
+      <c r="Q81">
+        <v>1.75</v>
+      </c>
+      <c r="R81">
         <v>2.05</v>
       </c>
-      <c r="M81">
-        <v>3.1</v>
-      </c>
-      <c r="N81">
-        <v>3.6</v>
-      </c>
-      <c r="O81">
-        <v>1.95</v>
-      </c>
-      <c r="P81">
-        <v>0.5</v>
-      </c>
-      <c r="Q81">
+      <c r="S81">
+        <v>2.5</v>
+      </c>
+      <c r="T81">
         <v>1.825</v>
       </c>
-      <c r="R81">
+      <c r="U81">
         <v>1.975</v>
       </c>
-      <c r="S81">
-        <v>3.25</v>
-      </c>
-      <c r="T81">
-        <v>1.95</v>
-      </c>
-      <c r="U81">
-        <v>1.85</v>
-      </c>
       <c r="V81">
         <v>-1</v>
       </c>
@@ -7446,19 +7446,19 @@
         <v>-1</v>
       </c>
       <c r="X81">
-        <v>0.95</v>
+        <v>1.3</v>
       </c>
       <c r="Y81">
         <v>-1</v>
       </c>
       <c r="Z81">
+        <v>1.05</v>
+      </c>
+      <c r="AA81">
+        <v>-1</v>
+      </c>
+      <c r="AB81">
         <v>0.9750000000000001</v>
-      </c>
-      <c r="AA81">
-        <v>-0.5</v>
-      </c>
-      <c r="AB81">
-        <v>0.425</v>
       </c>
     </row>
     <row r="82" spans="1:28">
@@ -7466,64 +7466,64 @@
         <v>80</v>
       </c>
       <c r="B82">
-        <v>6227882</v>
+        <v>6240262</v>
       </c>
       <c r="C82" t="s">
         <v>27</v>
       </c>
       <c r="D82" s="2">
-        <v>45205.85416666666</v>
+        <v>45205.97916666666</v>
       </c>
       <c r="E82" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F82" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G82">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H82">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I82" t="s">
         <v>36</v>
       </c>
       <c r="J82">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="K82">
-        <v>3.2</v>
+        <v>3.4</v>
       </c>
       <c r="L82">
-        <v>2.3</v>
+        <v>2.05</v>
       </c>
       <c r="M82">
-        <v>2.7</v>
+        <v>3.1</v>
       </c>
       <c r="N82">
+        <v>3.6</v>
+      </c>
+      <c r="O82">
+        <v>1.95</v>
+      </c>
+      <c r="P82">
+        <v>0.5</v>
+      </c>
+      <c r="Q82">
+        <v>1.825</v>
+      </c>
+      <c r="R82">
+        <v>1.975</v>
+      </c>
+      <c r="S82">
         <v>3.25</v>
       </c>
-      <c r="O82">
-        <v>2.3</v>
-      </c>
-      <c r="P82">
-        <v>0.25</v>
-      </c>
-      <c r="Q82">
-        <v>1.75</v>
-      </c>
-      <c r="R82">
-        <v>2.05</v>
-      </c>
-      <c r="S82">
-        <v>2.5</v>
-      </c>
       <c r="T82">
-        <v>1.825</v>
+        <v>1.95</v>
       </c>
       <c r="U82">
-        <v>1.975</v>
+        <v>1.85</v>
       </c>
       <c r="V82">
         <v>-1</v>
@@ -7532,19 +7532,19 @@
         <v>-1</v>
       </c>
       <c r="X82">
-        <v>1.3</v>
+        <v>0.95</v>
       </c>
       <c r="Y82">
         <v>-1</v>
       </c>
       <c r="Z82">
-        <v>1.05</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AA82">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="AB82">
-        <v>0.9750000000000001</v>
+        <v>0.425</v>
       </c>
     </row>
     <row r="83" spans="1:28">
@@ -8068,67 +8068,67 @@
         <v>87</v>
       </c>
       <c r="B89">
-        <v>7803361</v>
+        <v>7802934</v>
       </c>
       <c r="C89" t="s">
         <v>27</v>
       </c>
       <c r="D89" s="2">
-        <v>45395.83333333334</v>
+        <v>45395.58333333334</v>
       </c>
       <c r="E89" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F89" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G89">
+        <v>2</v>
+      </c>
+      <c r="H89">
         <v>1</v>
-      </c>
-      <c r="H89">
-        <v>0</v>
       </c>
       <c r="I89" t="s">
         <v>38</v>
       </c>
       <c r="J89">
-        <v>1.833</v>
+        <v>2.875</v>
       </c>
       <c r="K89">
-        <v>3.5</v>
+        <v>3.4</v>
       </c>
       <c r="L89">
-        <v>3.5</v>
+        <v>2.1</v>
       </c>
       <c r="M89">
+        <v>2.4</v>
+      </c>
+      <c r="N89">
+        <v>3.4</v>
+      </c>
+      <c r="O89">
+        <v>2.5</v>
+      </c>
+      <c r="P89">
+        <v>0</v>
+      </c>
+      <c r="Q89">
+        <v>1.85</v>
+      </c>
+      <c r="R89">
         <v>1.95</v>
       </c>
-      <c r="N89">
-        <v>3.25</v>
-      </c>
-      <c r="O89">
-        <v>3.4</v>
-      </c>
-      <c r="P89">
-        <v>-0.25</v>
-      </c>
-      <c r="Q89">
-        <v>1.775</v>
-      </c>
-      <c r="R89">
-        <v>2.025</v>
-      </c>
       <c r="S89">
-        <v>2.25</v>
+        <v>2.5</v>
       </c>
       <c r="T89">
-        <v>1.875</v>
+        <v>2</v>
       </c>
       <c r="U89">
-        <v>1.925</v>
+        <v>1.8</v>
       </c>
       <c r="V89">
-        <v>0.95</v>
+        <v>1.4</v>
       </c>
       <c r="W89">
         <v>-1</v>
@@ -8137,16 +8137,16 @@
         <v>-1</v>
       </c>
       <c r="Y89">
-        <v>0.7749999999999999</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="Z89">
         <v>-1</v>
       </c>
       <c r="AA89">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="AB89">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="90" spans="1:28">
@@ -8240,67 +8240,67 @@
         <v>89</v>
       </c>
       <c r="B91">
-        <v>7802934</v>
+        <v>7803361</v>
       </c>
       <c r="C91" t="s">
         <v>27</v>
       </c>
       <c r="D91" s="2">
-        <v>45395.58333333334</v>
+        <v>45395.83333333334</v>
       </c>
       <c r="E91" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="F91" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G91">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H91">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I91" t="s">
         <v>38</v>
       </c>
       <c r="J91">
-        <v>2.875</v>
+        <v>1.833</v>
       </c>
       <c r="K91">
+        <v>3.5</v>
+      </c>
+      <c r="L91">
+        <v>3.5</v>
+      </c>
+      <c r="M91">
+        <v>1.95</v>
+      </c>
+      <c r="N91">
+        <v>3.25</v>
+      </c>
+      <c r="O91">
         <v>3.4</v>
       </c>
-      <c r="L91">
-        <v>2.1</v>
-      </c>
-      <c r="M91">
-        <v>2.4</v>
-      </c>
-      <c r="N91">
-        <v>3.4</v>
-      </c>
-      <c r="O91">
-        <v>2.5</v>
-      </c>
       <c r="P91">
-        <v>0</v>
+        <v>-0.25</v>
       </c>
       <c r="Q91">
-        <v>1.85</v>
+        <v>1.775</v>
       </c>
       <c r="R91">
-        <v>1.95</v>
+        <v>2.025</v>
       </c>
       <c r="S91">
-        <v>2.5</v>
+        <v>2.25</v>
       </c>
       <c r="T91">
-        <v>2</v>
+        <v>1.875</v>
       </c>
       <c r="U91">
-        <v>1.8</v>
+        <v>1.925</v>
       </c>
       <c r="V91">
-        <v>1.4</v>
+        <v>0.95</v>
       </c>
       <c r="W91">
         <v>-1</v>
@@ -8309,16 +8309,16 @@
         <v>-1</v>
       </c>
       <c r="Y91">
-        <v>0.8500000000000001</v>
+        <v>0.7749999999999999</v>
       </c>
       <c r="Z91">
         <v>-1</v>
       </c>
       <c r="AA91">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AB91">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
     </row>
     <row r="92" spans="1:28">
@@ -8842,82 +8842,82 @@
         <v>96</v>
       </c>
       <c r="B98">
-        <v>7802876</v>
+        <v>7802938</v>
       </c>
       <c r="C98" t="s">
         <v>27</v>
       </c>
       <c r="D98" s="2">
-        <v>45409.70833333334</v>
+        <v>45409.58333333334</v>
       </c>
       <c r="E98" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F98" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G98">
+        <v>1</v>
+      </c>
+      <c r="H98">
+        <v>3</v>
+      </c>
+      <c r="I98" t="s">
+        <v>36</v>
+      </c>
+      <c r="J98">
         <v>2</v>
       </c>
-      <c r="H98">
-        <v>1</v>
-      </c>
-      <c r="I98" t="s">
-        <v>38</v>
-      </c>
-      <c r="J98">
-        <v>1.6</v>
-      </c>
       <c r="K98">
-        <v>3.75</v>
+        <v>3.3</v>
       </c>
       <c r="L98">
-        <v>4.5</v>
+        <v>3.2</v>
       </c>
       <c r="M98">
-        <v>1.4</v>
+        <v>2.25</v>
       </c>
       <c r="N98">
-        <v>4</v>
+        <v>3.1</v>
       </c>
       <c r="O98">
-        <v>6.5</v>
+        <v>2.875</v>
       </c>
       <c r="P98">
-        <v>-1.25</v>
+        <v>-0.25</v>
       </c>
       <c r="Q98">
-        <v>1.9</v>
+        <v>2.025</v>
       </c>
       <c r="R98">
-        <v>1.9</v>
+        <v>1.775</v>
       </c>
       <c r="S98">
-        <v>2.5</v>
+        <v>2.25</v>
       </c>
       <c r="T98">
-        <v>1.8</v>
+        <v>1.95</v>
       </c>
       <c r="U98">
-        <v>2</v>
+        <v>1.85</v>
       </c>
       <c r="V98">
-        <v>0.3999999999999999</v>
+        <v>-1</v>
       </c>
       <c r="W98">
         <v>-1</v>
       </c>
       <c r="X98">
-        <v>-1</v>
+        <v>1.875</v>
       </c>
       <c r="Y98">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
       <c r="Z98">
-        <v>0.45</v>
+        <v>0.7749999999999999</v>
       </c>
       <c r="AA98">
-        <v>0.8</v>
+        <v>0.95</v>
       </c>
       <c r="AB98">
         <v>-1</v>
@@ -8928,85 +8928,171 @@
         <v>97</v>
       </c>
       <c r="B99">
-        <v>7802938</v>
+        <v>7802876</v>
       </c>
       <c r="C99" t="s">
         <v>27</v>
       </c>
       <c r="D99" s="2">
-        <v>45409.58333333334</v>
+        <v>45409.70833333334</v>
       </c>
       <c r="E99" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F99" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G99">
+        <v>2</v>
+      </c>
+      <c r="H99">
         <v>1</v>
       </c>
-      <c r="H99">
-        <v>3</v>
-      </c>
       <c r="I99" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="J99">
+        <v>1.6</v>
+      </c>
+      <c r="K99">
+        <v>3.75</v>
+      </c>
+      <c r="L99">
+        <v>4.5</v>
+      </c>
+      <c r="M99">
+        <v>1.4</v>
+      </c>
+      <c r="N99">
+        <v>4</v>
+      </c>
+      <c r="O99">
+        <v>6.5</v>
+      </c>
+      <c r="P99">
+        <v>-1.25</v>
+      </c>
+      <c r="Q99">
+        <v>1.9</v>
+      </c>
+      <c r="R99">
+        <v>1.9</v>
+      </c>
+      <c r="S99">
+        <v>2.5</v>
+      </c>
+      <c r="T99">
+        <v>1.8</v>
+      </c>
+      <c r="U99">
         <v>2</v>
       </c>
-      <c r="K99">
+      <c r="V99">
+        <v>0.3999999999999999</v>
+      </c>
+      <c r="W99">
+        <v>-1</v>
+      </c>
+      <c r="X99">
+        <v>-1</v>
+      </c>
+      <c r="Y99">
+        <v>-0.5</v>
+      </c>
+      <c r="Z99">
+        <v>0.45</v>
+      </c>
+      <c r="AA99">
+        <v>0.8</v>
+      </c>
+      <c r="AB99">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:28">
+      <c r="A100" s="1">
+        <v>98</v>
+      </c>
+      <c r="B100">
+        <v>7803364</v>
+      </c>
+      <c r="C100" t="s">
+        <v>27</v>
+      </c>
+      <c r="D100" s="2">
+        <v>45410.75</v>
+      </c>
+      <c r="E100" t="s">
+        <v>29</v>
+      </c>
+      <c r="F100" t="s">
+        <v>35</v>
+      </c>
+      <c r="G100">
+        <v>0</v>
+      </c>
+      <c r="H100">
+        <v>0</v>
+      </c>
+      <c r="I100" t="s">
+        <v>37</v>
+      </c>
+      <c r="J100">
+        <v>2</v>
+      </c>
+      <c r="K100">
+        <v>3.2</v>
+      </c>
+      <c r="L100">
         <v>3.3</v>
       </c>
-      <c r="L99">
-        <v>3.2</v>
-      </c>
-      <c r="M99">
+      <c r="M100">
+        <v>1.8</v>
+      </c>
+      <c r="N100">
+        <v>3.1</v>
+      </c>
+      <c r="O100">
+        <v>4.2</v>
+      </c>
+      <c r="P100">
+        <v>-0.5</v>
+      </c>
+      <c r="Q100">
+        <v>1.825</v>
+      </c>
+      <c r="R100">
+        <v>1.975</v>
+      </c>
+      <c r="S100">
         <v>2.25</v>
       </c>
-      <c r="N99">
-        <v>3.1</v>
-      </c>
-      <c r="O99">
-        <v>2.875</v>
-      </c>
-      <c r="P99">
-        <v>-0.25</v>
-      </c>
-      <c r="Q99">
-        <v>2.025</v>
-      </c>
-      <c r="R99">
-        <v>1.775</v>
-      </c>
-      <c r="S99">
-        <v>2.25</v>
-      </c>
-      <c r="T99">
+      <c r="T100">
         <v>1.95</v>
       </c>
-      <c r="U99">
+      <c r="U100">
         <v>1.85</v>
       </c>
-      <c r="V99">
-        <v>-1</v>
-      </c>
-      <c r="W99">
-        <v>-1</v>
-      </c>
-      <c r="X99">
-        <v>1.875</v>
-      </c>
-      <c r="Y99">
-        <v>-1</v>
-      </c>
-      <c r="Z99">
-        <v>0.7749999999999999</v>
-      </c>
-      <c r="AA99">
-        <v>0.95</v>
-      </c>
-      <c r="AB99">
-        <v>-1</v>
+      <c r="V100">
+        <v>-1</v>
+      </c>
+      <c r="W100">
+        <v>2.1</v>
+      </c>
+      <c r="X100">
+        <v>-1</v>
+      </c>
+      <c r="Y100">
+        <v>-1</v>
+      </c>
+      <c r="Z100">
+        <v>0.9750000000000001</v>
+      </c>
+      <c r="AA100">
+        <v>-1</v>
+      </c>
+      <c r="AB100">
+        <v>0.8500000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 30-04-2024 às 19:33
</commit_message>
<xml_diff>
--- a/Canada Premier League/Canada Premier League.xlsx
+++ b/Canada Premier League/Canada Premier League.xlsx
@@ -103,10 +103,10 @@
     <t>Vancouver FC</t>
   </si>
   <si>
-    <t>Cavalry FC</t>
+    <t>Atletico Ottawa</t>
   </si>
   <si>
-    <t>Atletico Ottawa</t>
+    <t>Cavalry FC</t>
   </si>
   <si>
     <t>Valour FC</t>
@@ -127,10 +127,10 @@
     <t>A</t>
   </si>
   <si>
-    <t>D</t>
+    <t>H</t>
   </si>
   <si>
-    <t>H</t>
+    <t>D</t>
   </si>
 </sst>
 </file>
@@ -672,85 +672,85 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>6227808</v>
+        <v>6227809</v>
       </c>
       <c r="C3" t="s">
         <v>27</v>
       </c>
       <c r="D3" s="2">
-        <v>45080.70833333334</v>
+        <v>45080.83333333334</v>
       </c>
       <c r="E3" t="s">
         <v>29</v>
       </c>
       <c r="F3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I3" t="s">
         <v>37</v>
       </c>
       <c r="J3">
+        <v>2.1</v>
+      </c>
+      <c r="K3">
+        <v>3.1</v>
+      </c>
+      <c r="L3">
         <v>3.2</v>
       </c>
-      <c r="K3">
-        <v>2.75</v>
-      </c>
-      <c r="L3">
-        <v>2.3</v>
-      </c>
       <c r="M3">
-        <v>2.55</v>
+        <v>2.5</v>
       </c>
       <c r="N3">
-        <v>3</v>
+        <v>2.875</v>
       </c>
       <c r="O3">
-        <v>2.625</v>
+        <v>2.7</v>
       </c>
       <c r="P3">
         <v>0</v>
       </c>
       <c r="Q3">
-        <v>1.8</v>
+        <v>1.825</v>
       </c>
       <c r="R3">
+        <v>1.975</v>
+      </c>
+      <c r="S3">
         <v>2</v>
       </c>
-      <c r="S3">
-        <v>2.25</v>
-      </c>
       <c r="T3">
-        <v>1.925</v>
+        <v>1.775</v>
       </c>
       <c r="U3">
-        <v>1.875</v>
+        <v>2.025</v>
       </c>
       <c r="V3">
-        <v>-1</v>
+        <v>1.5</v>
       </c>
       <c r="W3">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="X3">
         <v>-1</v>
       </c>
       <c r="Y3">
-        <v>0</v>
+        <v>0.825</v>
       </c>
       <c r="Z3">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AA3">
-        <v>-0.5</v>
+        <v>0</v>
       </c>
       <c r="AB3">
-        <v>0.4375</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:28">
@@ -758,85 +758,85 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>6227809</v>
+        <v>6227808</v>
       </c>
       <c r="C4" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="2">
-        <v>45080.83333333334</v>
+        <v>45080.70833333334</v>
       </c>
       <c r="E4" t="s">
         <v>30</v>
       </c>
       <c r="F4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4" t="s">
         <v>38</v>
       </c>
       <c r="J4">
-        <v>2.1</v>
+        <v>3.2</v>
       </c>
       <c r="K4">
-        <v>3.1</v>
+        <v>2.75</v>
       </c>
       <c r="L4">
-        <v>3.2</v>
+        <v>2.3</v>
       </c>
       <c r="M4">
-        <v>2.5</v>
+        <v>2.55</v>
       </c>
       <c r="N4">
-        <v>2.875</v>
+        <v>3</v>
       </c>
       <c r="O4">
-        <v>2.7</v>
+        <v>2.625</v>
       </c>
       <c r="P4">
         <v>0</v>
       </c>
       <c r="Q4">
-        <v>1.825</v>
+        <v>1.8</v>
       </c>
       <c r="R4">
-        <v>1.975</v>
+        <v>2</v>
       </c>
       <c r="S4">
+        <v>2.25</v>
+      </c>
+      <c r="T4">
+        <v>1.925</v>
+      </c>
+      <c r="U4">
+        <v>1.875</v>
+      </c>
+      <c r="V4">
+        <v>-1</v>
+      </c>
+      <c r="W4">
         <v>2</v>
       </c>
-      <c r="T4">
-        <v>1.775</v>
-      </c>
-      <c r="U4">
-        <v>2.025</v>
-      </c>
-      <c r="V4">
-        <v>1.5</v>
-      </c>
-      <c r="W4">
-        <v>-1</v>
-      </c>
       <c r="X4">
         <v>-1</v>
       </c>
       <c r="Y4">
-        <v>0.825</v>
+        <v>0</v>
       </c>
       <c r="Z4">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AA4">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="AB4">
-        <v>0</v>
+        <v>0.4375</v>
       </c>
     </row>
     <row r="5" spans="1:28">
@@ -865,7 +865,7 @@
         <v>1</v>
       </c>
       <c r="I5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J5">
         <v>3.25</v>
@@ -942,7 +942,7 @@
         <v>32</v>
       </c>
       <c r="F6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G6">
         <v>2</v>
@@ -951,7 +951,7 @@
         <v>1</v>
       </c>
       <c r="I6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J6">
         <v>2.45</v>
@@ -1037,7 +1037,7 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J7">
         <v>2.7</v>
@@ -1197,7 +1197,7 @@
         <v>45088.75</v>
       </c>
       <c r="E9" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F9" t="s">
         <v>28</v>
@@ -1209,7 +1209,7 @@
         <v>1</v>
       </c>
       <c r="I9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J9">
         <v>1.909</v>
@@ -1295,7 +1295,7 @@
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J10">
         <v>2.1</v>
@@ -1369,7 +1369,7 @@
         <v>45094.625</v>
       </c>
       <c r="E11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F11" t="s">
         <v>28</v>
@@ -1381,7 +1381,7 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J11">
         <v>1.571</v>
@@ -1458,7 +1458,7 @@
         <v>33</v>
       </c>
       <c r="F12" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G12">
         <v>3</v>
@@ -1467,7 +1467,7 @@
         <v>1</v>
       </c>
       <c r="I12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J12">
         <v>2.6</v>
@@ -1553,7 +1553,7 @@
         <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J13">
         <v>1.615</v>
@@ -1639,7 +1639,7 @@
         <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J14">
         <v>5.2</v>
@@ -1725,7 +1725,7 @@
         <v>2</v>
       </c>
       <c r="I15" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J15">
         <v>2.5</v>
@@ -1811,7 +1811,7 @@
         <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J16">
         <v>1.666</v>
@@ -1885,7 +1885,7 @@
         <v>45101.75</v>
       </c>
       <c r="E17" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F17" t="s">
         <v>32</v>
@@ -1897,7 +1897,7 @@
         <v>1</v>
       </c>
       <c r="I17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J17">
         <v>1.8</v>
@@ -1983,7 +1983,7 @@
         <v>0</v>
       </c>
       <c r="I18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J18">
         <v>1.571</v>
@@ -2060,7 +2060,7 @@
         <v>34</v>
       </c>
       <c r="F19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G19">
         <v>4</v>
@@ -2069,7 +2069,7 @@
         <v>3</v>
       </c>
       <c r="I19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J19">
         <v>1.909</v>
@@ -2146,7 +2146,7 @@
         <v>35</v>
       </c>
       <c r="F20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G20">
         <v>2</v>
@@ -2155,7 +2155,7 @@
         <v>2</v>
       </c>
       <c r="I20" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J20">
         <v>1.727</v>
@@ -2241,7 +2241,7 @@
         <v>1</v>
       </c>
       <c r="I21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J21">
         <v>2.4</v>
@@ -2318,7 +2318,7 @@
         <v>31</v>
       </c>
       <c r="F22" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G22">
         <v>0</v>
@@ -2499,7 +2499,7 @@
         <v>1</v>
       </c>
       <c r="I24" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J24">
         <v>4.5</v>
@@ -2576,7 +2576,7 @@
         <v>35</v>
       </c>
       <c r="F25" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G25">
         <v>1</v>
@@ -2650,58 +2650,58 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>6227825</v>
+        <v>6227826</v>
       </c>
       <c r="C26" t="s">
         <v>27</v>
       </c>
       <c r="D26" s="2">
-        <v>45116.66666666666</v>
+        <v>45116.85416666666</v>
       </c>
       <c r="E26" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F26" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G26">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H26">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I26" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J26">
-        <v>2.25</v>
+        <v>2.6</v>
       </c>
       <c r="K26">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="L26">
+        <v>2.5</v>
+      </c>
+      <c r="M26">
+        <v>3.1</v>
+      </c>
+      <c r="N26">
+        <v>3.2</v>
+      </c>
+      <c r="O26">
+        <v>2.1</v>
+      </c>
+      <c r="P26">
+        <v>0.25</v>
+      </c>
+      <c r="Q26">
+        <v>1.9</v>
+      </c>
+      <c r="R26">
+        <v>1.9</v>
+      </c>
+      <c r="S26">
         <v>2.75</v>
-      </c>
-      <c r="M26">
-        <v>2.45</v>
-      </c>
-      <c r="N26">
-        <v>3.1</v>
-      </c>
-      <c r="O26">
-        <v>2.55</v>
-      </c>
-      <c r="P26">
-        <v>0</v>
-      </c>
-      <c r="Q26">
-        <v>1.85</v>
-      </c>
-      <c r="R26">
-        <v>1.95</v>
-      </c>
-      <c r="S26">
-        <v>2.25</v>
       </c>
       <c r="T26">
         <v>1.975</v>
@@ -2710,25 +2710,25 @@
         <v>1.825</v>
       </c>
       <c r="V26">
-        <v>1.45</v>
+        <v>-1</v>
       </c>
       <c r="W26">
         <v>-1</v>
       </c>
       <c r="X26">
-        <v>-1</v>
+        <v>1.1</v>
       </c>
       <c r="Y26">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="Z26">
-        <v>-1</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AA26">
-        <v>-0.5</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AB26">
-        <v>0.4125</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="27" spans="1:28">
@@ -2736,58 +2736,58 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>6227826</v>
+        <v>6227825</v>
       </c>
       <c r="C27" t="s">
         <v>27</v>
       </c>
       <c r="D27" s="2">
-        <v>45116.85416666666</v>
+        <v>45116.66666666666</v>
       </c>
       <c r="E27" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="F27" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G27">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H27">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I27" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J27">
-        <v>2.6</v>
+        <v>2.25</v>
       </c>
       <c r="K27">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="L27">
-        <v>2.5</v>
+        <v>2.75</v>
       </c>
       <c r="M27">
+        <v>2.45</v>
+      </c>
+      <c r="N27">
         <v>3.1</v>
       </c>
-      <c r="N27">
-        <v>3.2</v>
-      </c>
       <c r="O27">
-        <v>2.1</v>
+        <v>2.55</v>
       </c>
       <c r="P27">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="Q27">
-        <v>1.9</v>
+        <v>1.85</v>
       </c>
       <c r="R27">
-        <v>1.9</v>
+        <v>1.95</v>
       </c>
       <c r="S27">
-        <v>2.75</v>
+        <v>2.25</v>
       </c>
       <c r="T27">
         <v>1.975</v>
@@ -2796,25 +2796,25 @@
         <v>1.825</v>
       </c>
       <c r="V27">
-        <v>-1</v>
+        <v>1.45</v>
       </c>
       <c r="W27">
         <v>-1</v>
       </c>
       <c r="X27">
-        <v>1.1</v>
+        <v>-1</v>
       </c>
       <c r="Y27">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="Z27">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AA27">
-        <v>0.9750000000000001</v>
+        <v>-0.5</v>
       </c>
       <c r="AB27">
-        <v>-1</v>
+        <v>0.4125</v>
       </c>
     </row>
     <row r="28" spans="1:28">
@@ -2843,7 +2843,7 @@
         <v>1</v>
       </c>
       <c r="I28" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J28">
         <v>2.75</v>
@@ -2917,10 +2917,10 @@
         <v>45119.89583333334</v>
       </c>
       <c r="E29" t="s">
+        <v>30</v>
+      </c>
+      <c r="F29" t="s">
         <v>29</v>
-      </c>
-      <c r="F29" t="s">
-        <v>30</v>
       </c>
       <c r="G29">
         <v>0</v>
@@ -3015,7 +3015,7 @@
         <v>0</v>
       </c>
       <c r="I30" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J30">
         <v>3.5</v>
@@ -3101,7 +3101,7 @@
         <v>1</v>
       </c>
       <c r="I31" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J31">
         <v>1.909</v>
@@ -3175,7 +3175,7 @@
         <v>45122.70833333334</v>
       </c>
       <c r="E32" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F32" t="s">
         <v>33</v>
@@ -3187,7 +3187,7 @@
         <v>0</v>
       </c>
       <c r="I32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J32">
         <v>2.1</v>
@@ -3261,7 +3261,7 @@
         <v>45123.625</v>
       </c>
       <c r="E33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F33" t="s">
         <v>28</v>
@@ -3273,7 +3273,7 @@
         <v>1</v>
       </c>
       <c r="I33" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J33">
         <v>1.5</v>
@@ -3436,7 +3436,7 @@
         <v>28</v>
       </c>
       <c r="F35" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G35">
         <v>1</v>
@@ -3608,7 +3608,7 @@
         <v>33</v>
       </c>
       <c r="F37" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G37">
         <v>1</v>
@@ -3617,7 +3617,7 @@
         <v>0</v>
       </c>
       <c r="I37" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J37">
         <v>2.5</v>
@@ -3703,7 +3703,7 @@
         <v>0</v>
       </c>
       <c r="I38" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J38">
         <v>1.3</v>
@@ -3863,10 +3863,10 @@
         <v>45136.83333333334</v>
       </c>
       <c r="E40" t="s">
+        <v>29</v>
+      </c>
+      <c r="F40" t="s">
         <v>30</v>
-      </c>
-      <c r="F40" t="s">
-        <v>29</v>
       </c>
       <c r="G40">
         <v>1</v>
@@ -3875,7 +3875,7 @@
         <v>0</v>
       </c>
       <c r="I40" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J40">
         <v>2.6</v>
@@ -4035,7 +4035,7 @@
         <v>45142.91666666666</v>
       </c>
       <c r="E42" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F42" t="s">
         <v>34</v>
@@ -4047,7 +4047,7 @@
         <v>0</v>
       </c>
       <c r="I42" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J42">
         <v>2.625</v>
@@ -4121,7 +4121,7 @@
         <v>45143.83333333334</v>
       </c>
       <c r="E43" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F43" t="s">
         <v>32</v>
@@ -4133,7 +4133,7 @@
         <v>3</v>
       </c>
       <c r="I43" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J43">
         <v>2</v>
@@ -4219,7 +4219,7 @@
         <v>0</v>
       </c>
       <c r="I44" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J44">
         <v>2.9</v>
@@ -4382,7 +4382,7 @@
         <v>31</v>
       </c>
       <c r="F46" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G46">
         <v>3</v>
@@ -4391,7 +4391,7 @@
         <v>2</v>
       </c>
       <c r="I46" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J46">
         <v>2.875</v>
@@ -4456,85 +4456,85 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>6240271</v>
+        <v>6227842</v>
       </c>
       <c r="C47" t="s">
         <v>27</v>
       </c>
       <c r="D47" s="2">
-        <v>45150.66666666666</v>
+        <v>45150.83333333334</v>
       </c>
       <c r="E47" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F47" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="G47">
         <v>3</v>
       </c>
       <c r="H47">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I47" t="s">
         <v>38</v>
       </c>
       <c r="J47">
-        <v>1.444</v>
+        <v>1.727</v>
       </c>
       <c r="K47">
+        <v>3.2</v>
+      </c>
+      <c r="L47">
+        <v>4.5</v>
+      </c>
+      <c r="M47">
+        <v>1.5</v>
+      </c>
+      <c r="N47">
         <v>3.6</v>
       </c>
-      <c r="L47">
-        <v>7</v>
-      </c>
-      <c r="M47">
-        <v>1.4</v>
-      </c>
-      <c r="N47">
-        <v>3.75</v>
-      </c>
       <c r="O47">
-        <v>7</v>
+        <v>5.75</v>
       </c>
       <c r="P47">
-        <v>-1.25</v>
+        <v>-1</v>
       </c>
       <c r="Q47">
-        <v>1.95</v>
+        <v>2</v>
       </c>
       <c r="R47">
-        <v>1.85</v>
+        <v>1.8</v>
       </c>
       <c r="S47">
         <v>2.75</v>
       </c>
       <c r="T47">
-        <v>1.975</v>
+        <v>1.85</v>
       </c>
       <c r="U47">
-        <v>1.825</v>
+        <v>1.95</v>
       </c>
       <c r="V47">
-        <v>0.3999999999999999</v>
+        <v>-1</v>
       </c>
       <c r="W47">
-        <v>-1</v>
+        <v>2.6</v>
       </c>
       <c r="X47">
         <v>-1</v>
       </c>
       <c r="Y47">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="Z47">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="AA47">
-        <v>0.4875</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AB47">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="48" spans="1:28">
@@ -4542,85 +4542,85 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>6227842</v>
+        <v>6240271</v>
       </c>
       <c r="C48" t="s">
         <v>27</v>
       </c>
       <c r="D48" s="2">
-        <v>45150.83333333334</v>
+        <v>45150.66666666666</v>
       </c>
       <c r="E48" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F48" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G48">
         <v>3</v>
       </c>
       <c r="H48">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I48" t="s">
         <v>37</v>
       </c>
       <c r="J48">
-        <v>1.727</v>
+        <v>1.444</v>
       </c>
       <c r="K48">
-        <v>3.2</v>
+        <v>3.6</v>
       </c>
       <c r="L48">
-        <v>4.5</v>
+        <v>7</v>
       </c>
       <c r="M48">
-        <v>1.5</v>
+        <v>1.4</v>
       </c>
       <c r="N48">
-        <v>3.6</v>
+        <v>3.75</v>
       </c>
       <c r="O48">
-        <v>5.75</v>
+        <v>7</v>
       </c>
       <c r="P48">
-        <v>-1</v>
+        <v>-1.25</v>
       </c>
       <c r="Q48">
-        <v>2</v>
+        <v>1.95</v>
       </c>
       <c r="R48">
-        <v>1.8</v>
+        <v>1.85</v>
       </c>
       <c r="S48">
         <v>2.75</v>
       </c>
       <c r="T48">
-        <v>1.85</v>
+        <v>1.975</v>
       </c>
       <c r="U48">
-        <v>1.95</v>
+        <v>1.825</v>
       </c>
       <c r="V48">
-        <v>-1</v>
+        <v>0.3999999999999999</v>
       </c>
       <c r="W48">
-        <v>2.6</v>
+        <v>-1</v>
       </c>
       <c r="X48">
         <v>-1</v>
       </c>
       <c r="Y48">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="Z48">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
       <c r="AA48">
-        <v>0.8500000000000001</v>
+        <v>0.4875</v>
       </c>
       <c r="AB48">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="49" spans="1:28">
@@ -4640,7 +4640,7 @@
         <v>35</v>
       </c>
       <c r="F49" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G49">
         <v>0</v>
@@ -4726,7 +4726,7 @@
         <v>31</v>
       </c>
       <c r="F50" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G50">
         <v>1</v>
@@ -4821,7 +4821,7 @@
         <v>2</v>
       </c>
       <c r="I51" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J51">
         <v>7</v>
@@ -4907,7 +4907,7 @@
         <v>1</v>
       </c>
       <c r="I52" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J52">
         <v>1.727</v>
@@ -4981,7 +4981,7 @@
         <v>45158.75</v>
       </c>
       <c r="E53" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F53" t="s">
         <v>32</v>
@@ -4993,7 +4993,7 @@
         <v>1</v>
       </c>
       <c r="I53" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J53">
         <v>1.571</v>
@@ -5079,7 +5079,7 @@
         <v>1</v>
       </c>
       <c r="I54" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J54">
         <v>1.8</v>
@@ -5144,22 +5144,22 @@
         <v>53</v>
       </c>
       <c r="B55">
-        <v>6227862</v>
+        <v>6227863</v>
       </c>
       <c r="C55" t="s">
         <v>27</v>
       </c>
       <c r="D55" s="2">
-        <v>45164.66666666666</v>
+        <v>45164.83333333334</v>
       </c>
       <c r="E55" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F55" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G55">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H55">
         <v>0</v>
@@ -5168,61 +5168,61 @@
         <v>38</v>
       </c>
       <c r="J55">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="K55">
         <v>3</v>
       </c>
       <c r="L55">
-        <v>3.6</v>
+        <v>2.6</v>
       </c>
       <c r="M55">
-        <v>1.85</v>
+        <v>2.6</v>
       </c>
       <c r="N55">
         <v>3.1</v>
       </c>
       <c r="O55">
-        <v>4</v>
+        <v>2.55</v>
       </c>
       <c r="P55">
-        <v>-0.5</v>
+        <v>0</v>
       </c>
       <c r="Q55">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="R55">
-        <v>1.85</v>
+        <v>1.875</v>
       </c>
       <c r="S55">
-        <v>2.25</v>
+        <v>2.5</v>
       </c>
       <c r="T55">
-        <v>1.825</v>
+        <v>1.925</v>
       </c>
       <c r="U55">
-        <v>1.975</v>
+        <v>1.875</v>
       </c>
       <c r="V55">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="W55">
-        <v>-1</v>
+        <v>2.1</v>
       </c>
       <c r="X55">
         <v>-1</v>
       </c>
       <c r="Y55">
-        <v>0.95</v>
+        <v>0</v>
       </c>
       <c r="Z55">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AA55">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
       <c r="AB55">
-        <v>-1</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="56" spans="1:28">
@@ -5230,22 +5230,22 @@
         <v>54</v>
       </c>
       <c r="B56">
-        <v>6227863</v>
+        <v>6227862</v>
       </c>
       <c r="C56" t="s">
         <v>27</v>
       </c>
       <c r="D56" s="2">
-        <v>45164.83333333334</v>
+        <v>45164.66666666666</v>
       </c>
       <c r="E56" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F56" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G56">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H56">
         <v>0</v>
@@ -5254,61 +5254,61 @@
         <v>37</v>
       </c>
       <c r="J56">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="K56">
         <v>3</v>
       </c>
       <c r="L56">
-        <v>2.6</v>
+        <v>3.6</v>
       </c>
       <c r="M56">
-        <v>2.6</v>
+        <v>1.85</v>
       </c>
       <c r="N56">
         <v>3.1</v>
       </c>
       <c r="O56">
-        <v>2.55</v>
+        <v>4</v>
       </c>
       <c r="P56">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="Q56">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="R56">
-        <v>1.875</v>
+        <v>1.85</v>
       </c>
       <c r="S56">
-        <v>2.5</v>
+        <v>2.25</v>
       </c>
       <c r="T56">
-        <v>1.925</v>
+        <v>1.825</v>
       </c>
       <c r="U56">
-        <v>1.875</v>
+        <v>1.975</v>
       </c>
       <c r="V56">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="W56">
-        <v>2.1</v>
+        <v>-1</v>
       </c>
       <c r="X56">
         <v>-1</v>
       </c>
       <c r="Y56">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="Z56">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AA56">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
       <c r="AB56">
-        <v>0.875</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="57" spans="1:28">
@@ -5325,7 +5325,7 @@
         <v>45165.75</v>
       </c>
       <c r="E57" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F57" t="s">
         <v>35</v>
@@ -5337,7 +5337,7 @@
         <v>0</v>
       </c>
       <c r="I57" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J57">
         <v>2.4</v>
@@ -5411,10 +5411,10 @@
         <v>45171.83333333334</v>
       </c>
       <c r="E58" t="s">
+        <v>29</v>
+      </c>
+      <c r="F58" t="s">
         <v>30</v>
-      </c>
-      <c r="F58" t="s">
-        <v>29</v>
       </c>
       <c r="G58">
         <v>1</v>
@@ -5509,7 +5509,7 @@
         <v>1</v>
       </c>
       <c r="I59" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J59">
         <v>1.7</v>
@@ -5767,7 +5767,7 @@
         <v>1</v>
       </c>
       <c r="I62" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J62">
         <v>1.75</v>
@@ -5930,7 +5930,7 @@
         <v>28</v>
       </c>
       <c r="F64" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G64">
         <v>2</v>
@@ -5939,7 +5939,7 @@
         <v>1</v>
       </c>
       <c r="I64" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J64">
         <v>3.5</v>
@@ -6016,7 +6016,7 @@
         <v>34</v>
       </c>
       <c r="F65" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G65">
         <v>0</v>
@@ -6025,7 +6025,7 @@
         <v>0</v>
       </c>
       <c r="I65" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J65">
         <v>1.909</v>
@@ -6102,7 +6102,7 @@
         <v>33</v>
       </c>
       <c r="F66" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G66">
         <v>1</v>
@@ -6185,7 +6185,7 @@
         <v>45182.77083333334</v>
       </c>
       <c r="E67" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F67" t="s">
         <v>35</v>
@@ -6197,7 +6197,7 @@
         <v>1</v>
       </c>
       <c r="I67" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J67">
         <v>2.5</v>
@@ -6271,7 +6271,7 @@
         <v>45185.75</v>
       </c>
       <c r="E68" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F68" t="s">
         <v>28</v>
@@ -6283,7 +6283,7 @@
         <v>1</v>
       </c>
       <c r="I68" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J68">
         <v>1.285</v>
@@ -6532,7 +6532,7 @@
         <v>33</v>
       </c>
       <c r="F71" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G71">
         <v>3</v>
@@ -6541,7 +6541,7 @@
         <v>2</v>
       </c>
       <c r="I71" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J71">
         <v>2.625</v>
@@ -6692,85 +6692,85 @@
         <v>71</v>
       </c>
       <c r="B73">
-        <v>6227877</v>
+        <v>6227876</v>
       </c>
       <c r="C73" t="s">
         <v>27</v>
       </c>
       <c r="D73" s="2">
-        <v>45192.83333333334</v>
+        <v>45192.58333333334</v>
       </c>
       <c r="E73" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F73" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="G73">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H73">
         <v>1</v>
       </c>
       <c r="I73" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J73">
-        <v>2</v>
+        <v>3.6</v>
       </c>
       <c r="K73">
-        <v>3.2</v>
+        <v>3.4</v>
       </c>
       <c r="L73">
-        <v>3.3</v>
+        <v>1.909</v>
       </c>
       <c r="M73">
-        <v>2.25</v>
+        <v>3.75</v>
       </c>
       <c r="N73">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="O73">
-        <v>2.875</v>
+        <v>1.833</v>
       </c>
       <c r="P73">
-        <v>-0.25</v>
+        <v>0.5</v>
       </c>
       <c r="Q73">
-        <v>2.025</v>
+        <v>1.9</v>
       </c>
       <c r="R73">
-        <v>1.775</v>
+        <v>1.9</v>
       </c>
       <c r="S73">
-        <v>2.25</v>
+        <v>2.75</v>
       </c>
       <c r="T73">
-        <v>1.825</v>
+        <v>1.9</v>
       </c>
       <c r="U73">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="V73">
-        <v>1.25</v>
+        <v>-1</v>
       </c>
       <c r="W73">
         <v>-1</v>
       </c>
       <c r="X73">
-        <v>-1</v>
+        <v>0.833</v>
       </c>
       <c r="Y73">
-        <v>1.025</v>
+        <v>-1</v>
       </c>
       <c r="Z73">
-        <v>-1</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AA73">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
       <c r="AB73">
-        <v>-1</v>
+        <v>0.8999999999999999</v>
       </c>
     </row>
     <row r="74" spans="1:28">
@@ -6799,7 +6799,7 @@
         <v>1</v>
       </c>
       <c r="I74" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J74">
         <v>3.75</v>
@@ -6864,85 +6864,85 @@
         <v>73</v>
       </c>
       <c r="B75">
-        <v>6227876</v>
+        <v>6227877</v>
       </c>
       <c r="C75" t="s">
         <v>27</v>
       </c>
       <c r="D75" s="2">
-        <v>45192.58333333334</v>
+        <v>45192.83333333334</v>
       </c>
       <c r="E75" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F75" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="G75">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H75">
         <v>1</v>
       </c>
       <c r="I75" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J75">
-        <v>3.6</v>
+        <v>2</v>
       </c>
       <c r="K75">
-        <v>3.4</v>
+        <v>3.2</v>
       </c>
       <c r="L75">
-        <v>1.909</v>
+        <v>3.3</v>
       </c>
       <c r="M75">
-        <v>3.75</v>
+        <v>2.25</v>
       </c>
       <c r="N75">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="O75">
-        <v>1.833</v>
+        <v>2.875</v>
       </c>
       <c r="P75">
-        <v>0.5</v>
+        <v>-0.25</v>
       </c>
       <c r="Q75">
-        <v>1.9</v>
+        <v>2.025</v>
       </c>
       <c r="R75">
-        <v>1.9</v>
+        <v>1.775</v>
       </c>
       <c r="S75">
-        <v>2.75</v>
+        <v>2.25</v>
       </c>
       <c r="T75">
-        <v>1.9</v>
+        <v>1.825</v>
       </c>
       <c r="U75">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="V75">
-        <v>-1</v>
+        <v>1.25</v>
       </c>
       <c r="W75">
         <v>-1</v>
       </c>
       <c r="X75">
-        <v>0.833</v>
+        <v>-1</v>
       </c>
       <c r="Y75">
-        <v>-1</v>
+        <v>1.025</v>
       </c>
       <c r="Z75">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AA75">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
       <c r="AB75">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="76" spans="1:28">
@@ -6959,7 +6959,7 @@
         <v>45193.625</v>
       </c>
       <c r="E76" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F76" t="s">
         <v>31</v>
@@ -7045,7 +7045,7 @@
         <v>45198.91666666666</v>
       </c>
       <c r="E77" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F77" t="s">
         <v>31</v>
@@ -7057,7 +7057,7 @@
         <v>1</v>
       </c>
       <c r="I77" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J77">
         <v>1.615</v>
@@ -7122,58 +7122,58 @@
         <v>76</v>
       </c>
       <c r="B78">
-        <v>6240263</v>
+        <v>6227880</v>
       </c>
       <c r="C78" t="s">
         <v>27</v>
       </c>
       <c r="D78" s="2">
-        <v>45199.75</v>
+        <v>45199.625</v>
       </c>
       <c r="E78" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F78" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="G78">
+        <v>2</v>
+      </c>
+      <c r="H78">
         <v>1</v>
       </c>
-      <c r="H78">
-        <v>2</v>
-      </c>
       <c r="I78" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J78">
-        <v>1.285</v>
+        <v>2.625</v>
       </c>
       <c r="K78">
-        <v>5</v>
+        <v>3.4</v>
       </c>
       <c r="L78">
-        <v>8.5</v>
+        <v>2.4</v>
       </c>
       <c r="M78">
-        <v>1.3</v>
+        <v>2.9</v>
       </c>
       <c r="N78">
-        <v>5.5</v>
+        <v>3.4</v>
       </c>
       <c r="O78">
-        <v>6</v>
+        <v>2.2</v>
       </c>
       <c r="P78">
-        <v>-1.5</v>
+        <v>0.25</v>
       </c>
       <c r="Q78">
-        <v>1.775</v>
+        <v>1.875</v>
       </c>
       <c r="R78">
         <v>1.925</v>
       </c>
       <c r="S78">
-        <v>3.25</v>
+        <v>2.5</v>
       </c>
       <c r="T78">
         <v>1.975</v>
@@ -7182,25 +7182,25 @@
         <v>1.825</v>
       </c>
       <c r="V78">
-        <v>-1</v>
+        <v>1.9</v>
       </c>
       <c r="W78">
         <v>-1</v>
       </c>
       <c r="X78">
-        <v>5</v>
+        <v>-1</v>
       </c>
       <c r="Y78">
-        <v>-1</v>
+        <v>0.875</v>
       </c>
       <c r="Z78">
-        <v>0.925</v>
+        <v>-1</v>
       </c>
       <c r="AA78">
-        <v>-0.5</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AB78">
-        <v>0.4125</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="79" spans="1:28">
@@ -7208,58 +7208,58 @@
         <v>77</v>
       </c>
       <c r="B79">
-        <v>6227880</v>
+        <v>6240263</v>
       </c>
       <c r="C79" t="s">
         <v>27</v>
       </c>
       <c r="D79" s="2">
-        <v>45199.625</v>
+        <v>45199.75</v>
       </c>
       <c r="E79" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F79" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="G79">
+        <v>1</v>
+      </c>
+      <c r="H79">
         <v>2</v>
       </c>
-      <c r="H79">
-        <v>1</v>
-      </c>
       <c r="I79" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J79">
-        <v>2.625</v>
+        <v>1.285</v>
       </c>
       <c r="K79">
-        <v>3.4</v>
+        <v>5</v>
       </c>
       <c r="L79">
-        <v>2.4</v>
+        <v>8.5</v>
       </c>
       <c r="M79">
-        <v>2.9</v>
+        <v>1.3</v>
       </c>
       <c r="N79">
-        <v>3.4</v>
+        <v>5.5</v>
       </c>
       <c r="O79">
-        <v>2.2</v>
+        <v>6</v>
       </c>
       <c r="P79">
-        <v>0.25</v>
+        <v>-1.5</v>
       </c>
       <c r="Q79">
-        <v>1.875</v>
+        <v>1.775</v>
       </c>
       <c r="R79">
         <v>1.925</v>
       </c>
       <c r="S79">
-        <v>2.5</v>
+        <v>3.25</v>
       </c>
       <c r="T79">
         <v>1.975</v>
@@ -7268,25 +7268,25 @@
         <v>1.825</v>
       </c>
       <c r="V79">
-        <v>1.9</v>
+        <v>-1</v>
       </c>
       <c r="W79">
         <v>-1</v>
       </c>
       <c r="X79">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="Y79">
-        <v>0.875</v>
+        <v>-1</v>
       </c>
       <c r="Z79">
-        <v>-1</v>
+        <v>0.925</v>
       </c>
       <c r="AA79">
-        <v>0.9750000000000001</v>
+        <v>-0.5</v>
       </c>
       <c r="AB79">
-        <v>-1</v>
+        <v>0.4125</v>
       </c>
     </row>
     <row r="80" spans="1:28">
@@ -7306,7 +7306,7 @@
         <v>32</v>
       </c>
       <c r="F80" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G80">
         <v>1</v>
@@ -7315,7 +7315,7 @@
         <v>0</v>
       </c>
       <c r="I80" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J80">
         <v>2.375</v>
@@ -7380,64 +7380,64 @@
         <v>79</v>
       </c>
       <c r="B81">
-        <v>6227882</v>
+        <v>6240262</v>
       </c>
       <c r="C81" t="s">
         <v>27</v>
       </c>
       <c r="D81" s="2">
-        <v>45205.85416666666</v>
+        <v>45205.97916666666</v>
       </c>
       <c r="E81" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F81" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G81">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H81">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I81" t="s">
         <v>36</v>
       </c>
       <c r="J81">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="K81">
-        <v>3.2</v>
+        <v>3.4</v>
       </c>
       <c r="L81">
-        <v>2.3</v>
+        <v>2.05</v>
       </c>
       <c r="M81">
-        <v>2.7</v>
+        <v>3.1</v>
       </c>
       <c r="N81">
+        <v>3.6</v>
+      </c>
+      <c r="O81">
+        <v>1.95</v>
+      </c>
+      <c r="P81">
+        <v>0.5</v>
+      </c>
+      <c r="Q81">
+        <v>1.825</v>
+      </c>
+      <c r="R81">
+        <v>1.975</v>
+      </c>
+      <c r="S81">
         <v>3.25</v>
       </c>
-      <c r="O81">
-        <v>2.3</v>
-      </c>
-      <c r="P81">
-        <v>0.25</v>
-      </c>
-      <c r="Q81">
-        <v>1.75</v>
-      </c>
-      <c r="R81">
-        <v>2.05</v>
-      </c>
-      <c r="S81">
-        <v>2.5</v>
-      </c>
       <c r="T81">
-        <v>1.825</v>
+        <v>1.95</v>
       </c>
       <c r="U81">
-        <v>1.975</v>
+        <v>1.85</v>
       </c>
       <c r="V81">
         <v>-1</v>
@@ -7446,19 +7446,19 @@
         <v>-1</v>
       </c>
       <c r="X81">
-        <v>1.3</v>
+        <v>0.95</v>
       </c>
       <c r="Y81">
         <v>-1</v>
       </c>
       <c r="Z81">
-        <v>1.05</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AA81">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="AB81">
-        <v>0.9750000000000001</v>
+        <v>0.425</v>
       </c>
     </row>
     <row r="82" spans="1:28">
@@ -7466,65 +7466,65 @@
         <v>80</v>
       </c>
       <c r="B82">
-        <v>6240262</v>
+        <v>6227882</v>
       </c>
       <c r="C82" t="s">
         <v>27</v>
       </c>
       <c r="D82" s="2">
-        <v>45205.97916666666</v>
+        <v>45205.85416666666</v>
       </c>
       <c r="E82" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F82" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G82">
+        <v>0</v>
+      </c>
+      <c r="H82">
         <v>1</v>
-      </c>
-      <c r="H82">
-        <v>2</v>
       </c>
       <c r="I82" t="s">
         <v>36</v>
       </c>
       <c r="J82">
-        <v>3</v>
+        <v>2.75</v>
       </c>
       <c r="K82">
-        <v>3.4</v>
+        <v>3.2</v>
       </c>
       <c r="L82">
+        <v>2.3</v>
+      </c>
+      <c r="M82">
+        <v>2.7</v>
+      </c>
+      <c r="N82">
+        <v>3.25</v>
+      </c>
+      <c r="O82">
+        <v>2.3</v>
+      </c>
+      <c r="P82">
+        <v>0.25</v>
+      </c>
+      <c r="Q82">
+        <v>1.75</v>
+      </c>
+      <c r="R82">
         <v>2.05</v>
       </c>
-      <c r="M82">
-        <v>3.1</v>
-      </c>
-      <c r="N82">
-        <v>3.6</v>
-      </c>
-      <c r="O82">
-        <v>1.95</v>
-      </c>
-      <c r="P82">
-        <v>0.5</v>
-      </c>
-      <c r="Q82">
+      <c r="S82">
+        <v>2.5</v>
+      </c>
+      <c r="T82">
         <v>1.825</v>
       </c>
-      <c r="R82">
+      <c r="U82">
         <v>1.975</v>
       </c>
-      <c r="S82">
-        <v>3.25</v>
-      </c>
-      <c r="T82">
-        <v>1.95</v>
-      </c>
-      <c r="U82">
-        <v>1.85</v>
-      </c>
       <c r="V82">
         <v>-1</v>
       </c>
@@ -7532,19 +7532,19 @@
         <v>-1</v>
       </c>
       <c r="X82">
-        <v>0.95</v>
+        <v>1.3</v>
       </c>
       <c r="Y82">
         <v>-1</v>
       </c>
       <c r="Z82">
+        <v>1.05</v>
+      </c>
+      <c r="AA82">
+        <v>-1</v>
+      </c>
+      <c r="AB82">
         <v>0.9750000000000001</v>
-      </c>
-      <c r="AA82">
-        <v>-0.5</v>
-      </c>
-      <c r="AB82">
-        <v>0.425</v>
       </c>
     </row>
     <row r="83" spans="1:28">
@@ -7552,7 +7552,7 @@
         <v>81</v>
       </c>
       <c r="B83">
-        <v>6227884</v>
+        <v>7301364</v>
       </c>
       <c r="C83" t="s">
         <v>27</v>
@@ -7561,76 +7561,76 @@
         <v>45206.75</v>
       </c>
       <c r="E83" t="s">
+        <v>34</v>
+      </c>
+      <c r="F83" t="s">
         <v>29</v>
       </c>
-      <c r="F83" t="s">
-        <v>35</v>
-      </c>
       <c r="G83">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H83">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I83" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J83">
-        <v>2.25</v>
+        <v>1.8</v>
       </c>
       <c r="K83">
-        <v>3.1</v>
+        <v>3.6</v>
       </c>
       <c r="L83">
-        <v>2.875</v>
+        <v>3.5</v>
       </c>
       <c r="M83">
-        <v>2.05</v>
+        <v>1.533</v>
       </c>
       <c r="N83">
-        <v>3.2</v>
+        <v>3.8</v>
       </c>
       <c r="O83">
-        <v>3.2</v>
+        <v>5</v>
       </c>
       <c r="P83">
-        <v>-0.25</v>
+        <v>-1</v>
       </c>
       <c r="Q83">
+        <v>1.975</v>
+      </c>
+      <c r="R83">
         <v>1.825</v>
-      </c>
-      <c r="R83">
-        <v>1.975</v>
       </c>
       <c r="S83">
         <v>2.5</v>
       </c>
       <c r="T83">
-        <v>1.825</v>
+        <v>1.9</v>
       </c>
       <c r="U83">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="V83">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="W83">
         <v>-1</v>
       </c>
       <c r="X83">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="Y83">
+        <v>-1</v>
+      </c>
+      <c r="Z83">
         <v>0.825</v>
       </c>
-      <c r="Z83">
-        <v>-1</v>
-      </c>
       <c r="AA83">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
       <c r="AB83">
-        <v>-1</v>
+        <v>0.8999999999999999</v>
       </c>
     </row>
     <row r="84" spans="1:28">
@@ -7638,7 +7638,7 @@
         <v>82</v>
       </c>
       <c r="B84">
-        <v>7301364</v>
+        <v>6227884</v>
       </c>
       <c r="C84" t="s">
         <v>27</v>
@@ -7647,76 +7647,76 @@
         <v>45206.75</v>
       </c>
       <c r="E84" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F84" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="G84">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H84">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I84" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J84">
-        <v>1.8</v>
+        <v>2.25</v>
       </c>
       <c r="K84">
-        <v>3.6</v>
+        <v>3.1</v>
       </c>
       <c r="L84">
-        <v>3.5</v>
+        <v>2.875</v>
       </c>
       <c r="M84">
-        <v>1.533</v>
+        <v>2.05</v>
       </c>
       <c r="N84">
-        <v>3.8</v>
+        <v>3.2</v>
       </c>
       <c r="O84">
-        <v>5</v>
+        <v>3.2</v>
       </c>
       <c r="P84">
-        <v>-1</v>
+        <v>-0.25</v>
       </c>
       <c r="Q84">
+        <v>1.825</v>
+      </c>
+      <c r="R84">
         <v>1.975</v>
-      </c>
-      <c r="R84">
-        <v>1.825</v>
       </c>
       <c r="S84">
         <v>2.5</v>
       </c>
       <c r="T84">
-        <v>1.9</v>
+        <v>1.825</v>
       </c>
       <c r="U84">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="V84">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="W84">
         <v>-1</v>
       </c>
       <c r="X84">
-        <v>4</v>
+        <v>-1</v>
       </c>
       <c r="Y84">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
       <c r="Z84">
+        <v>-1</v>
+      </c>
+      <c r="AA84">
         <v>0.825</v>
       </c>
-      <c r="AA84">
-        <v>-1</v>
-      </c>
       <c r="AB84">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="85" spans="1:28">
@@ -7745,7 +7745,7 @@
         <v>0</v>
       </c>
       <c r="I85" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J85">
         <v>1.727</v>
@@ -7819,7 +7819,7 @@
         <v>45213.75</v>
       </c>
       <c r="E86" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F86" t="s">
         <v>34</v>
@@ -7994,7 +7994,7 @@
         <v>34</v>
       </c>
       <c r="F88" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G88">
         <v>2</v>
@@ -8003,7 +8003,7 @@
         <v>1</v>
       </c>
       <c r="I88" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J88">
         <v>2.2</v>
@@ -8077,7 +8077,7 @@
         <v>45395.58333333334</v>
       </c>
       <c r="E89" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F89" t="s">
         <v>32</v>
@@ -8089,7 +8089,7 @@
         <v>1</v>
       </c>
       <c r="I89" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J89">
         <v>2.875</v>
@@ -8166,7 +8166,7 @@
         <v>34</v>
       </c>
       <c r="F90" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G90">
         <v>2</v>
@@ -8175,7 +8175,7 @@
         <v>1</v>
       </c>
       <c r="I90" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J90">
         <v>2.2</v>
@@ -8261,7 +8261,7 @@
         <v>0</v>
       </c>
       <c r="I91" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J91">
         <v>1.833</v>
@@ -8347,7 +8347,7 @@
         <v>1</v>
       </c>
       <c r="I92" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J92">
         <v>2.4</v>
@@ -8433,7 +8433,7 @@
         <v>0</v>
       </c>
       <c r="I93" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J93">
         <v>3.1</v>
@@ -8519,7 +8519,7 @@
         <v>0</v>
       </c>
       <c r="I94" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J94">
         <v>1.727</v>
@@ -8593,10 +8593,10 @@
         <v>45402.625</v>
       </c>
       <c r="E95" t="s">
+        <v>29</v>
+      </c>
+      <c r="F95" t="s">
         <v>30</v>
-      </c>
-      <c r="F95" t="s">
-        <v>29</v>
       </c>
       <c r="G95">
         <v>1</v>
@@ -8605,7 +8605,7 @@
         <v>1</v>
       </c>
       <c r="I95" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J95">
         <v>3.1</v>
@@ -8777,7 +8777,7 @@
         <v>0</v>
       </c>
       <c r="I97" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J97">
         <v>2.2</v>
@@ -8842,82 +8842,82 @@
         <v>96</v>
       </c>
       <c r="B98">
-        <v>7802938</v>
+        <v>7802876</v>
       </c>
       <c r="C98" t="s">
         <v>27</v>
       </c>
       <c r="D98" s="2">
-        <v>45409.58333333334</v>
+        <v>45409.70833333334</v>
       </c>
       <c r="E98" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F98" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G98">
+        <v>2</v>
+      </c>
+      <c r="H98">
         <v>1</v>
       </c>
-      <c r="H98">
-        <v>3</v>
-      </c>
       <c r="I98" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J98">
+        <v>1.6</v>
+      </c>
+      <c r="K98">
+        <v>3.75</v>
+      </c>
+      <c r="L98">
+        <v>4.5</v>
+      </c>
+      <c r="M98">
+        <v>1.4</v>
+      </c>
+      <c r="N98">
+        <v>4</v>
+      </c>
+      <c r="O98">
+        <v>6.5</v>
+      </c>
+      <c r="P98">
+        <v>-1.25</v>
+      </c>
+      <c r="Q98">
+        <v>1.9</v>
+      </c>
+      <c r="R98">
+        <v>1.9</v>
+      </c>
+      <c r="S98">
+        <v>2.5</v>
+      </c>
+      <c r="T98">
+        <v>1.8</v>
+      </c>
+      <c r="U98">
         <v>2</v>
       </c>
-      <c r="K98">
-        <v>3.3</v>
-      </c>
-      <c r="L98">
-        <v>3.2</v>
-      </c>
-      <c r="M98">
-        <v>2.25</v>
-      </c>
-      <c r="N98">
-        <v>3.1</v>
-      </c>
-      <c r="O98">
-        <v>2.875</v>
-      </c>
-      <c r="P98">
-        <v>-0.25</v>
-      </c>
-      <c r="Q98">
-        <v>2.025</v>
-      </c>
-      <c r="R98">
-        <v>1.775</v>
-      </c>
-      <c r="S98">
-        <v>2.25</v>
-      </c>
-      <c r="T98">
-        <v>1.95</v>
-      </c>
-      <c r="U98">
-        <v>1.85</v>
-      </c>
       <c r="V98">
-        <v>-1</v>
+        <v>0.3999999999999999</v>
       </c>
       <c r="W98">
         <v>-1</v>
       </c>
       <c r="X98">
-        <v>1.875</v>
+        <v>-1</v>
       </c>
       <c r="Y98">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="Z98">
-        <v>0.7749999999999999</v>
+        <v>0.45</v>
       </c>
       <c r="AA98">
-        <v>0.95</v>
+        <v>0.8</v>
       </c>
       <c r="AB98">
         <v>-1</v>
@@ -8928,82 +8928,82 @@
         <v>97</v>
       </c>
       <c r="B99">
-        <v>7802876</v>
+        <v>7802938</v>
       </c>
       <c r="C99" t="s">
         <v>27</v>
       </c>
       <c r="D99" s="2">
-        <v>45409.70833333334</v>
+        <v>45409.58333333334</v>
       </c>
       <c r="E99" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F99" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G99">
+        <v>1</v>
+      </c>
+      <c r="H99">
+        <v>3</v>
+      </c>
+      <c r="I99" t="s">
+        <v>36</v>
+      </c>
+      <c r="J99">
         <v>2</v>
       </c>
-      <c r="H99">
-        <v>1</v>
-      </c>
-      <c r="I99" t="s">
-        <v>38</v>
-      </c>
-      <c r="J99">
-        <v>1.6</v>
-      </c>
       <c r="K99">
-        <v>3.75</v>
+        <v>3.3</v>
       </c>
       <c r="L99">
-        <v>4.5</v>
+        <v>3.2</v>
       </c>
       <c r="M99">
-        <v>1.4</v>
+        <v>2.25</v>
       </c>
       <c r="N99">
-        <v>4</v>
+        <v>3.1</v>
       </c>
       <c r="O99">
-        <v>6.5</v>
+        <v>2.875</v>
       </c>
       <c r="P99">
-        <v>-1.25</v>
+        <v>-0.25</v>
       </c>
       <c r="Q99">
-        <v>1.9</v>
+        <v>2.025</v>
       </c>
       <c r="R99">
-        <v>1.9</v>
+        <v>1.775</v>
       </c>
       <c r="S99">
-        <v>2.5</v>
+        <v>2.25</v>
       </c>
       <c r="T99">
-        <v>1.8</v>
+        <v>1.95</v>
       </c>
       <c r="U99">
-        <v>2</v>
+        <v>1.85</v>
       </c>
       <c r="V99">
-        <v>0.3999999999999999</v>
+        <v>-1</v>
       </c>
       <c r="W99">
         <v>-1</v>
       </c>
       <c r="X99">
-        <v>-1</v>
+        <v>1.875</v>
       </c>
       <c r="Y99">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
       <c r="Z99">
-        <v>0.45</v>
+        <v>0.7749999999999999</v>
       </c>
       <c r="AA99">
-        <v>0.8</v>
+        <v>0.95</v>
       </c>
       <c r="AB99">
         <v>-1</v>
@@ -9023,7 +9023,7 @@
         <v>45410.75</v>
       </c>
       <c r="E100" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F100" t="s">
         <v>35</v>
@@ -9035,7 +9035,7 @@
         <v>0</v>
       </c>
       <c r="I100" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J100">
         <v>2</v>

</xml_diff>

<commit_message>
Atualização de bases das ligas, do dia: 01-05-2024 às 16:15
</commit_message>
<xml_diff>
--- a/Canada Premier League/Canada Premier League.xlsx
+++ b/Canada Premier League/Canada Premier League.xlsx
@@ -103,10 +103,10 @@
     <t>Vancouver FC</t>
   </si>
   <si>
-    <t>Atletico Ottawa</t>
+    <t>Cavalry FC</t>
   </si>
   <si>
-    <t>Cavalry FC</t>
+    <t>Atletico Ottawa</t>
   </si>
   <si>
     <t>Valour FC</t>
@@ -127,10 +127,10 @@
     <t>A</t>
   </si>
   <si>
-    <t>H</t>
+    <t>D</t>
   </si>
   <si>
-    <t>D</t>
+    <t>H</t>
   </si>
 </sst>
 </file>
@@ -672,85 +672,85 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>6227809</v>
+        <v>6227808</v>
       </c>
       <c r="C3" t="s">
         <v>27</v>
       </c>
       <c r="D3" s="2">
-        <v>45080.83333333334</v>
+        <v>45080.70833333334</v>
       </c>
       <c r="E3" t="s">
         <v>29</v>
       </c>
       <c r="F3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I3" t="s">
         <v>37</v>
       </c>
       <c r="J3">
-        <v>2.1</v>
+        <v>3.2</v>
       </c>
       <c r="K3">
-        <v>3.1</v>
+        <v>2.75</v>
       </c>
       <c r="L3">
-        <v>3.2</v>
+        <v>2.3</v>
       </c>
       <c r="M3">
-        <v>2.5</v>
+        <v>2.55</v>
       </c>
       <c r="N3">
-        <v>2.875</v>
+        <v>3</v>
       </c>
       <c r="O3">
-        <v>2.7</v>
+        <v>2.625</v>
       </c>
       <c r="P3">
         <v>0</v>
       </c>
       <c r="Q3">
-        <v>1.825</v>
+        <v>1.8</v>
       </c>
       <c r="R3">
-        <v>1.975</v>
+        <v>2</v>
       </c>
       <c r="S3">
+        <v>2.25</v>
+      </c>
+      <c r="T3">
+        <v>1.925</v>
+      </c>
+      <c r="U3">
+        <v>1.875</v>
+      </c>
+      <c r="V3">
+        <v>-1</v>
+      </c>
+      <c r="W3">
         <v>2</v>
       </c>
-      <c r="T3">
-        <v>1.775</v>
-      </c>
-      <c r="U3">
-        <v>2.025</v>
-      </c>
-      <c r="V3">
-        <v>1.5</v>
-      </c>
-      <c r="W3">
-        <v>-1</v>
-      </c>
       <c r="X3">
         <v>-1</v>
       </c>
       <c r="Y3">
-        <v>0.825</v>
+        <v>0</v>
       </c>
       <c r="Z3">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AA3">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="AB3">
-        <v>0</v>
+        <v>0.4375</v>
       </c>
     </row>
     <row r="4" spans="1:28">
@@ -758,85 +758,85 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>6227808</v>
+        <v>6227809</v>
       </c>
       <c r="C4" t="s">
         <v>27</v>
       </c>
       <c r="D4" s="2">
-        <v>45080.70833333334</v>
+        <v>45080.83333333334</v>
       </c>
       <c r="E4" t="s">
         <v>30</v>
       </c>
       <c r="F4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4" t="s">
         <v>38</v>
       </c>
       <c r="J4">
+        <v>2.1</v>
+      </c>
+      <c r="K4">
+        <v>3.1</v>
+      </c>
+      <c r="L4">
         <v>3.2</v>
       </c>
-      <c r="K4">
-        <v>2.75</v>
-      </c>
-      <c r="L4">
-        <v>2.3</v>
-      </c>
       <c r="M4">
-        <v>2.55</v>
+        <v>2.5</v>
       </c>
       <c r="N4">
-        <v>3</v>
+        <v>2.875</v>
       </c>
       <c r="O4">
-        <v>2.625</v>
+        <v>2.7</v>
       </c>
       <c r="P4">
         <v>0</v>
       </c>
       <c r="Q4">
-        <v>1.8</v>
+        <v>1.825</v>
       </c>
       <c r="R4">
+        <v>1.975</v>
+      </c>
+      <c r="S4">
         <v>2</v>
       </c>
-      <c r="S4">
-        <v>2.25</v>
-      </c>
       <c r="T4">
-        <v>1.925</v>
+        <v>1.775</v>
       </c>
       <c r="U4">
-        <v>1.875</v>
+        <v>2.025</v>
       </c>
       <c r="V4">
-        <v>-1</v>
+        <v>1.5</v>
       </c>
       <c r="W4">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="X4">
         <v>-1</v>
       </c>
       <c r="Y4">
-        <v>0</v>
+        <v>0.825</v>
       </c>
       <c r="Z4">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AA4">
-        <v>-0.5</v>
+        <v>0</v>
       </c>
       <c r="AB4">
-        <v>0.4375</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:28">
@@ -865,7 +865,7 @@
         <v>1</v>
       </c>
       <c r="I5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J5">
         <v>3.25</v>
@@ -942,7 +942,7 @@
         <v>32</v>
       </c>
       <c r="F6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G6">
         <v>2</v>
@@ -951,7 +951,7 @@
         <v>1</v>
       </c>
       <c r="I6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J6">
         <v>2.45</v>
@@ -1037,7 +1037,7 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J7">
         <v>2.7</v>
@@ -1197,7 +1197,7 @@
         <v>45088.75</v>
       </c>
       <c r="E9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F9" t="s">
         <v>28</v>
@@ -1209,7 +1209,7 @@
         <v>1</v>
       </c>
       <c r="I9" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J9">
         <v>1.909</v>
@@ -1295,7 +1295,7 @@
         <v>0</v>
       </c>
       <c r="I10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J10">
         <v>2.1</v>
@@ -1369,7 +1369,7 @@
         <v>45094.625</v>
       </c>
       <c r="E11" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F11" t="s">
         <v>28</v>
@@ -1381,7 +1381,7 @@
         <v>0</v>
       </c>
       <c r="I11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J11">
         <v>1.571</v>
@@ -1458,7 +1458,7 @@
         <v>33</v>
       </c>
       <c r="F12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G12">
         <v>3</v>
@@ -1467,7 +1467,7 @@
         <v>1</v>
       </c>
       <c r="I12" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J12">
         <v>2.6</v>
@@ -1553,7 +1553,7 @@
         <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J13">
         <v>1.615</v>
@@ -1639,7 +1639,7 @@
         <v>0</v>
       </c>
       <c r="I14" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J14">
         <v>5.2</v>
@@ -1725,7 +1725,7 @@
         <v>2</v>
       </c>
       <c r="I15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J15">
         <v>2.5</v>
@@ -1811,7 +1811,7 @@
         <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J16">
         <v>1.666</v>
@@ -1885,7 +1885,7 @@
         <v>45101.75</v>
       </c>
       <c r="E17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F17" t="s">
         <v>32</v>
@@ -1897,7 +1897,7 @@
         <v>1</v>
       </c>
       <c r="I17" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J17">
         <v>1.8</v>
@@ -1983,7 +1983,7 @@
         <v>0</v>
       </c>
       <c r="I18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J18">
         <v>1.571</v>
@@ -2060,7 +2060,7 @@
         <v>34</v>
       </c>
       <c r="F19" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G19">
         <v>4</v>
@@ -2069,7 +2069,7 @@
         <v>3</v>
       </c>
       <c r="I19" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J19">
         <v>1.909</v>
@@ -2134,82 +2134,82 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>6227822</v>
+        <v>6227821</v>
       </c>
       <c r="C20" t="s">
         <v>27</v>
       </c>
       <c r="D20" s="2">
-        <v>45107.9375</v>
+        <v>45107.79166666666</v>
       </c>
       <c r="E20" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F20" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="G20">
         <v>2</v>
       </c>
       <c r="H20">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I20" t="s">
         <v>38</v>
       </c>
       <c r="J20">
-        <v>1.727</v>
+        <v>2.4</v>
       </c>
       <c r="K20">
-        <v>3.4</v>
+        <v>3</v>
       </c>
       <c r="L20">
-        <v>4.333</v>
+        <v>2.75</v>
       </c>
       <c r="M20">
-        <v>1.833</v>
+        <v>2.75</v>
       </c>
       <c r="N20">
-        <v>3.4</v>
+        <v>2.9</v>
       </c>
       <c r="O20">
-        <v>4</v>
+        <v>2.4</v>
       </c>
       <c r="P20">
-        <v>-0.5</v>
+        <v>0</v>
       </c>
       <c r="Q20">
-        <v>1.85</v>
+        <v>2.025</v>
       </c>
       <c r="R20">
-        <v>1.95</v>
+        <v>1.775</v>
       </c>
       <c r="S20">
-        <v>2.5</v>
+        <v>2.25</v>
       </c>
       <c r="T20">
-        <v>2.075</v>
+        <v>1.8</v>
       </c>
       <c r="U20">
-        <v>1.725</v>
+        <v>2</v>
       </c>
       <c r="V20">
-        <v>-1</v>
+        <v>1.75</v>
       </c>
       <c r="W20">
-        <v>2.4</v>
+        <v>-1</v>
       </c>
       <c r="X20">
         <v>-1</v>
       </c>
       <c r="Y20">
-        <v>-1</v>
+        <v>1.025</v>
       </c>
       <c r="Z20">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AA20">
-        <v>1.075</v>
+        <v>0.8</v>
       </c>
       <c r="AB20">
         <v>-1</v>
@@ -2220,82 +2220,82 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>6227821</v>
+        <v>6227822</v>
       </c>
       <c r="C21" t="s">
         <v>27</v>
       </c>
       <c r="D21" s="2">
-        <v>45107.79166666666</v>
+        <v>45107.9375</v>
       </c>
       <c r="E21" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F21" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="G21">
         <v>2</v>
       </c>
       <c r="H21">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I21" t="s">
         <v>37</v>
       </c>
       <c r="J21">
+        <v>1.727</v>
+      </c>
+      <c r="K21">
+        <v>3.4</v>
+      </c>
+      <c r="L21">
+        <v>4.333</v>
+      </c>
+      <c r="M21">
+        <v>1.833</v>
+      </c>
+      <c r="N21">
+        <v>3.4</v>
+      </c>
+      <c r="O21">
+        <v>4</v>
+      </c>
+      <c r="P21">
+        <v>-0.5</v>
+      </c>
+      <c r="Q21">
+        <v>1.85</v>
+      </c>
+      <c r="R21">
+        <v>1.95</v>
+      </c>
+      <c r="S21">
+        <v>2.5</v>
+      </c>
+      <c r="T21">
+        <v>2.075</v>
+      </c>
+      <c r="U21">
+        <v>1.725</v>
+      </c>
+      <c r="V21">
+        <v>-1</v>
+      </c>
+      <c r="W21">
         <v>2.4</v>
       </c>
-      <c r="K21">
-        <v>3</v>
-      </c>
-      <c r="L21">
-        <v>2.75</v>
-      </c>
-      <c r="M21">
-        <v>2.75</v>
-      </c>
-      <c r="N21">
-        <v>2.9</v>
-      </c>
-      <c r="O21">
-        <v>2.4</v>
-      </c>
-      <c r="P21">
-        <v>0</v>
-      </c>
-      <c r="Q21">
-        <v>2.025</v>
-      </c>
-      <c r="R21">
-        <v>1.775</v>
-      </c>
-      <c r="S21">
-        <v>2.25</v>
-      </c>
-      <c r="T21">
-        <v>1.8</v>
-      </c>
-      <c r="U21">
-        <v>2</v>
-      </c>
-      <c r="V21">
-        <v>1.75</v>
-      </c>
-      <c r="W21">
-        <v>-1</v>
-      </c>
       <c r="X21">
         <v>-1</v>
       </c>
       <c r="Y21">
-        <v>1.025</v>
+        <v>-1</v>
       </c>
       <c r="Z21">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="AA21">
-        <v>0.8</v>
+        <v>1.075</v>
       </c>
       <c r="AB21">
         <v>-1</v>
@@ -2318,7 +2318,7 @@
         <v>31</v>
       </c>
       <c r="F22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G22">
         <v>0</v>
@@ -2499,7 +2499,7 @@
         <v>1</v>
       </c>
       <c r="I24" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J24">
         <v>4.5</v>
@@ -2576,7 +2576,7 @@
         <v>35</v>
       </c>
       <c r="F25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G25">
         <v>1</v>
@@ -2650,58 +2650,58 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>6227826</v>
+        <v>6227825</v>
       </c>
       <c r="C26" t="s">
         <v>27</v>
       </c>
       <c r="D26" s="2">
-        <v>45116.85416666666</v>
+        <v>45116.66666666666</v>
       </c>
       <c r="E26" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F26" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G26">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H26">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="I26" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="J26">
-        <v>2.6</v>
+        <v>2.25</v>
       </c>
       <c r="K26">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="L26">
-        <v>2.5</v>
+        <v>2.75</v>
       </c>
       <c r="M26">
+        <v>2.45</v>
+      </c>
+      <c r="N26">
         <v>3.1</v>
       </c>
-      <c r="N26">
-        <v>3.2</v>
-      </c>
       <c r="O26">
-        <v>2.1</v>
+        <v>2.55</v>
       </c>
       <c r="P26">
-        <v>0.25</v>
+        <v>0</v>
       </c>
       <c r="Q26">
-        <v>1.9</v>
+        <v>1.85</v>
       </c>
       <c r="R26">
-        <v>1.9</v>
+        <v>1.95</v>
       </c>
       <c r="S26">
-        <v>2.75</v>
+        <v>2.25</v>
       </c>
       <c r="T26">
         <v>1.975</v>
@@ -2710,25 +2710,25 @@
         <v>1.825</v>
       </c>
       <c r="V26">
-        <v>-1</v>
+        <v>1.45</v>
       </c>
       <c r="W26">
         <v>-1</v>
       </c>
       <c r="X26">
-        <v>1.1</v>
+        <v>-1</v>
       </c>
       <c r="Y26">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="Z26">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
       <c r="AA26">
-        <v>0.9750000000000001</v>
+        <v>-0.5</v>
       </c>
       <c r="AB26">
-        <v>-1</v>
+        <v>0.4125</v>
       </c>
     </row>
     <row r="27" spans="1:28">
@@ -2736,58 +2736,58 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>6227825</v>
+        <v>6227826</v>
       </c>
       <c r="C27" t="s">
         <v>27</v>
       </c>
       <c r="D27" s="2">
-        <v>45116.66666666666</v>
+        <v>45116.85416666666</v>
       </c>
       <c r="E27" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="F27" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G27">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H27">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="I27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J27">
-        <v>2.25</v>
+        <v>2.6</v>
       </c>
       <c r="K27">
-        <v>3.25</v>
+        <v>3</v>
       </c>
       <c r="L27">
+        <v>2.5</v>
+      </c>
+      <c r="M27">
+        <v>3.1</v>
+      </c>
+      <c r="N27">
+        <v>3.2</v>
+      </c>
+      <c r="O27">
+        <v>2.1</v>
+      </c>
+      <c r="P27">
+        <v>0.25</v>
+      </c>
+      <c r="Q27">
+        <v>1.9</v>
+      </c>
+      <c r="R27">
+        <v>1.9</v>
+      </c>
+      <c r="S27">
         <v>2.75</v>
-      </c>
-      <c r="M27">
-        <v>2.45</v>
-      </c>
-      <c r="N27">
-        <v>3.1</v>
-      </c>
-      <c r="O27">
-        <v>2.55</v>
-      </c>
-      <c r="P27">
-        <v>0</v>
-      </c>
-      <c r="Q27">
-        <v>1.85</v>
-      </c>
-      <c r="R27">
-        <v>1.95</v>
-      </c>
-      <c r="S27">
-        <v>2.25</v>
       </c>
       <c r="T27">
         <v>1.975</v>
@@ -2796,25 +2796,25 @@
         <v>1.825</v>
       </c>
       <c r="V27">
-        <v>1.45</v>
+        <v>-1</v>
       </c>
       <c r="W27">
         <v>-1</v>
       </c>
       <c r="X27">
-        <v>-1</v>
+        <v>1.1</v>
       </c>
       <c r="Y27">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="Z27">
-        <v>-1</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AA27">
-        <v>-0.5</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AB27">
-        <v>0.4125</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="28" spans="1:28">
@@ -2843,7 +2843,7 @@
         <v>1</v>
       </c>
       <c r="I28" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J28">
         <v>2.75</v>
@@ -2917,10 +2917,10 @@
         <v>45119.89583333334</v>
       </c>
       <c r="E29" t="s">
+        <v>29</v>
+      </c>
+      <c r="F29" t="s">
         <v>30</v>
-      </c>
-      <c r="F29" t="s">
-        <v>29</v>
       </c>
       <c r="G29">
         <v>0</v>
@@ -3015,7 +3015,7 @@
         <v>0</v>
       </c>
       <c r="I30" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J30">
         <v>3.5</v>
@@ -3080,85 +3080,85 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>6227831</v>
+        <v>6227830</v>
       </c>
       <c r="C31" t="s">
         <v>27</v>
       </c>
       <c r="D31" s="2">
-        <v>45122.83333333334</v>
+        <v>45122.70833333334</v>
       </c>
       <c r="E31" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="F31" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G31">
         <v>1</v>
       </c>
       <c r="H31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I31" t="s">
         <v>38</v>
       </c>
       <c r="J31">
-        <v>1.909</v>
+        <v>2.1</v>
       </c>
       <c r="K31">
+        <v>3</v>
+      </c>
+      <c r="L31">
         <v>3.25</v>
       </c>
-      <c r="L31">
-        <v>3.5</v>
-      </c>
       <c r="M31">
-        <v>1.7</v>
+        <v>1.95</v>
       </c>
       <c r="N31">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="O31">
-        <v>4.2</v>
+        <v>3.75</v>
       </c>
       <c r="P31">
-        <v>-0.75</v>
+        <v>-0.5</v>
       </c>
       <c r="Q31">
+        <v>1.975</v>
+      </c>
+      <c r="R31">
+        <v>1.825</v>
+      </c>
+      <c r="S31">
+        <v>2.25</v>
+      </c>
+      <c r="T31">
         <v>1.85</v>
       </c>
-      <c r="R31">
+      <c r="U31">
         <v>1.95</v>
       </c>
-      <c r="S31">
-        <v>2.5</v>
-      </c>
-      <c r="T31">
-        <v>1.9</v>
-      </c>
-      <c r="U31">
-        <v>1.9</v>
-      </c>
       <c r="V31">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="W31">
-        <v>2.5</v>
+        <v>-1</v>
       </c>
       <c r="X31">
         <v>-1</v>
       </c>
       <c r="Y31">
-        <v>-1</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="Z31">
+        <v>-1</v>
+      </c>
+      <c r="AA31">
+        <v>-1</v>
+      </c>
+      <c r="AB31">
         <v>0.95</v>
-      </c>
-      <c r="AA31">
-        <v>-1</v>
-      </c>
-      <c r="AB31">
-        <v>0.8999999999999999</v>
       </c>
     </row>
     <row r="32" spans="1:28">
@@ -3166,85 +3166,85 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>6227830</v>
+        <v>6227831</v>
       </c>
       <c r="C32" t="s">
         <v>27</v>
       </c>
       <c r="D32" s="2">
-        <v>45122.70833333334</v>
+        <v>45122.83333333334</v>
       </c>
       <c r="E32" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="F32" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G32">
         <v>1</v>
       </c>
       <c r="H32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I32" t="s">
         <v>37</v>
       </c>
       <c r="J32">
-        <v>2.1</v>
+        <v>1.909</v>
       </c>
       <c r="K32">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="L32">
-        <v>3.25</v>
+        <v>3.5</v>
       </c>
       <c r="M32">
+        <v>1.7</v>
+      </c>
+      <c r="N32">
+        <v>3.5</v>
+      </c>
+      <c r="O32">
+        <v>4.2</v>
+      </c>
+      <c r="P32">
+        <v>-0.75</v>
+      </c>
+      <c r="Q32">
+        <v>1.85</v>
+      </c>
+      <c r="R32">
         <v>1.95</v>
       </c>
-      <c r="N32">
-        <v>3</v>
-      </c>
-      <c r="O32">
-        <v>3.75</v>
-      </c>
-      <c r="P32">
-        <v>-0.5</v>
-      </c>
-      <c r="Q32">
-        <v>1.975</v>
-      </c>
-      <c r="R32">
-        <v>1.825</v>
-      </c>
       <c r="S32">
-        <v>2.25</v>
+        <v>2.5</v>
       </c>
       <c r="T32">
-        <v>1.85</v>
+        <v>1.9</v>
       </c>
       <c r="U32">
-        <v>1.95</v>
+        <v>1.9</v>
       </c>
       <c r="V32">
+        <v>-1</v>
+      </c>
+      <c r="W32">
+        <v>2.5</v>
+      </c>
+      <c r="X32">
+        <v>-1</v>
+      </c>
+      <c r="Y32">
+        <v>-1</v>
+      </c>
+      <c r="Z32">
         <v>0.95</v>
       </c>
-      <c r="W32">
-        <v>-1</v>
-      </c>
-      <c r="X32">
-        <v>-1</v>
-      </c>
-      <c r="Y32">
-        <v>0.9750000000000001</v>
-      </c>
-      <c r="Z32">
-        <v>-1</v>
-      </c>
       <c r="AA32">
         <v>-1</v>
       </c>
       <c r="AB32">
-        <v>0.95</v>
+        <v>0.8999999999999999</v>
       </c>
     </row>
     <row r="33" spans="1:28">
@@ -3261,7 +3261,7 @@
         <v>45123.625</v>
       </c>
       <c r="E33" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F33" t="s">
         <v>28</v>
@@ -3273,7 +3273,7 @@
         <v>1</v>
       </c>
       <c r="I33" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J33">
         <v>1.5</v>
@@ -3436,7 +3436,7 @@
         <v>28</v>
       </c>
       <c r="F35" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G35">
         <v>1</v>
@@ -3510,46 +3510,46 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>6227834</v>
+        <v>6227833</v>
       </c>
       <c r="C36" t="s">
         <v>27</v>
       </c>
       <c r="D36" s="2">
-        <v>45130.83333333334</v>
+        <v>45130.70833333334</v>
       </c>
       <c r="E36" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F36" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G36">
         <v>1</v>
       </c>
       <c r="H36">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I36" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="J36">
-        <v>2.3</v>
+        <v>2.5</v>
       </c>
       <c r="K36">
         <v>3</v>
       </c>
       <c r="L36">
-        <v>2.9</v>
+        <v>2.6</v>
       </c>
       <c r="M36">
         <v>2.625</v>
       </c>
       <c r="N36">
-        <v>2.9</v>
+        <v>3.1</v>
       </c>
       <c r="O36">
-        <v>2.55</v>
+        <v>2.375</v>
       </c>
       <c r="P36">
         <v>0</v>
@@ -3564,31 +3564,31 @@
         <v>2.5</v>
       </c>
       <c r="T36">
-        <v>2</v>
+        <v>1.9</v>
       </c>
       <c r="U36">
-        <v>1.8</v>
+        <v>1.9</v>
       </c>
       <c r="V36">
-        <v>-1</v>
+        <v>1.625</v>
       </c>
       <c r="W36">
         <v>-1</v>
       </c>
       <c r="X36">
-        <v>1.55</v>
+        <v>-1</v>
       </c>
       <c r="Y36">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="Z36">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
       <c r="AA36">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="AB36">
-        <v>-1</v>
+        <v>0.8999999999999999</v>
       </c>
     </row>
     <row r="37" spans="1:28">
@@ -3596,46 +3596,46 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>6227833</v>
+        <v>6227834</v>
       </c>
       <c r="C37" t="s">
         <v>27</v>
       </c>
       <c r="D37" s="2">
-        <v>45130.70833333334</v>
+        <v>45130.83333333334</v>
       </c>
       <c r="E37" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F37" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="G37">
         <v>1</v>
       </c>
       <c r="H37">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I37" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J37">
-        <v>2.5</v>
+        <v>2.3</v>
       </c>
       <c r="K37">
         <v>3</v>
       </c>
       <c r="L37">
-        <v>2.6</v>
+        <v>2.9</v>
       </c>
       <c r="M37">
         <v>2.625</v>
       </c>
       <c r="N37">
-        <v>3.1</v>
+        <v>2.9</v>
       </c>
       <c r="O37">
-        <v>2.375</v>
+        <v>2.55</v>
       </c>
       <c r="P37">
         <v>0</v>
@@ -3650,31 +3650,31 @@
         <v>2.5</v>
       </c>
       <c r="T37">
-        <v>1.9</v>
+        <v>2</v>
       </c>
       <c r="U37">
-        <v>1.9</v>
+        <v>1.8</v>
       </c>
       <c r="V37">
-        <v>1.625</v>
+        <v>-1</v>
       </c>
       <c r="W37">
         <v>-1</v>
       </c>
       <c r="X37">
-        <v>-1</v>
+        <v>1.55</v>
       </c>
       <c r="Y37">
+        <v>-1</v>
+      </c>
+      <c r="Z37">
+        <v>0.8</v>
+      </c>
+      <c r="AA37">
         <v>1</v>
       </c>
-      <c r="Z37">
-        <v>-1</v>
-      </c>
-      <c r="AA37">
-        <v>-1</v>
-      </c>
       <c r="AB37">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="38" spans="1:28">
@@ -3703,7 +3703,7 @@
         <v>0</v>
       </c>
       <c r="I38" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J38">
         <v>1.3</v>
@@ -3863,10 +3863,10 @@
         <v>45136.83333333334</v>
       </c>
       <c r="E40" t="s">
+        <v>30</v>
+      </c>
+      <c r="F40" t="s">
         <v>29</v>
-      </c>
-      <c r="F40" t="s">
-        <v>30</v>
       </c>
       <c r="G40">
         <v>1</v>
@@ -3875,7 +3875,7 @@
         <v>0</v>
       </c>
       <c r="I40" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J40">
         <v>2.6</v>
@@ -4035,7 +4035,7 @@
         <v>45142.91666666666</v>
       </c>
       <c r="E42" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F42" t="s">
         <v>34</v>
@@ -4047,7 +4047,7 @@
         <v>0</v>
       </c>
       <c r="I42" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J42">
         <v>2.625</v>
@@ -4121,7 +4121,7 @@
         <v>45143.83333333334</v>
       </c>
       <c r="E43" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F43" t="s">
         <v>32</v>
@@ -4133,7 +4133,7 @@
         <v>3</v>
       </c>
       <c r="I43" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J43">
         <v>2</v>
@@ -4219,7 +4219,7 @@
         <v>0</v>
       </c>
       <c r="I44" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J44">
         <v>2.9</v>
@@ -4382,7 +4382,7 @@
         <v>31</v>
       </c>
       <c r="F46" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G46">
         <v>3</v>
@@ -4391,7 +4391,7 @@
         <v>2</v>
       </c>
       <c r="I46" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J46">
         <v>2.875</v>
@@ -4456,85 +4456,85 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>6227842</v>
+        <v>6240271</v>
       </c>
       <c r="C47" t="s">
         <v>27</v>
       </c>
       <c r="D47" s="2">
-        <v>45150.83333333334</v>
+        <v>45150.66666666666</v>
       </c>
       <c r="E47" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F47" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G47">
         <v>3</v>
       </c>
       <c r="H47">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I47" t="s">
         <v>38</v>
       </c>
       <c r="J47">
-        <v>1.727</v>
+        <v>1.444</v>
       </c>
       <c r="K47">
-        <v>3.2</v>
+        <v>3.6</v>
       </c>
       <c r="L47">
-        <v>4.5</v>
+        <v>7</v>
       </c>
       <c r="M47">
-        <v>1.5</v>
+        <v>1.4</v>
       </c>
       <c r="N47">
-        <v>3.6</v>
+        <v>3.75</v>
       </c>
       <c r="O47">
-        <v>5.75</v>
+        <v>7</v>
       </c>
       <c r="P47">
-        <v>-1</v>
+        <v>-1.25</v>
       </c>
       <c r="Q47">
-        <v>2</v>
+        <v>1.95</v>
       </c>
       <c r="R47">
-        <v>1.8</v>
+        <v>1.85</v>
       </c>
       <c r="S47">
         <v>2.75</v>
       </c>
       <c r="T47">
-        <v>1.85</v>
+        <v>1.975</v>
       </c>
       <c r="U47">
-        <v>1.95</v>
+        <v>1.825</v>
       </c>
       <c r="V47">
-        <v>-1</v>
+        <v>0.3999999999999999</v>
       </c>
       <c r="W47">
-        <v>2.6</v>
+        <v>-1</v>
       </c>
       <c r="X47">
         <v>-1</v>
       </c>
       <c r="Y47">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="Z47">
-        <v>0.8</v>
+        <v>-1</v>
       </c>
       <c r="AA47">
-        <v>0.8500000000000001</v>
+        <v>0.4875</v>
       </c>
       <c r="AB47">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
     </row>
     <row r="48" spans="1:28">
@@ -4542,85 +4542,85 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>6240271</v>
+        <v>6227842</v>
       </c>
       <c r="C48" t="s">
         <v>27</v>
       </c>
       <c r="D48" s="2">
-        <v>45150.66666666666</v>
+        <v>45150.83333333334</v>
       </c>
       <c r="E48" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F48" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="G48">
         <v>3</v>
       </c>
       <c r="H48">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I48" t="s">
         <v>37</v>
       </c>
       <c r="J48">
-        <v>1.444</v>
+        <v>1.727</v>
       </c>
       <c r="K48">
+        <v>3.2</v>
+      </c>
+      <c r="L48">
+        <v>4.5</v>
+      </c>
+      <c r="M48">
+        <v>1.5</v>
+      </c>
+      <c r="N48">
         <v>3.6</v>
       </c>
-      <c r="L48">
-        <v>7</v>
-      </c>
-      <c r="M48">
-        <v>1.4</v>
-      </c>
-      <c r="N48">
-        <v>3.75</v>
-      </c>
       <c r="O48">
-        <v>7</v>
+        <v>5.75</v>
       </c>
       <c r="P48">
-        <v>-1.25</v>
+        <v>-1</v>
       </c>
       <c r="Q48">
-        <v>1.95</v>
+        <v>2</v>
       </c>
       <c r="R48">
-        <v>1.85</v>
+        <v>1.8</v>
       </c>
       <c r="S48">
         <v>2.75</v>
       </c>
       <c r="T48">
-        <v>1.975</v>
+        <v>1.85</v>
       </c>
       <c r="U48">
-        <v>1.825</v>
+        <v>1.95</v>
       </c>
       <c r="V48">
-        <v>0.3999999999999999</v>
+        <v>-1</v>
       </c>
       <c r="W48">
-        <v>-1</v>
+        <v>2.6</v>
       </c>
       <c r="X48">
         <v>-1</v>
       </c>
       <c r="Y48">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="Z48">
-        <v>-1</v>
+        <v>0.8</v>
       </c>
       <c r="AA48">
-        <v>0.4875</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="AB48">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="49" spans="1:28">
@@ -4640,7 +4640,7 @@
         <v>35</v>
       </c>
       <c r="F49" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G49">
         <v>0</v>
@@ -4726,7 +4726,7 @@
         <v>31</v>
       </c>
       <c r="F50" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G50">
         <v>1</v>
@@ -4821,7 +4821,7 @@
         <v>2</v>
       </c>
       <c r="I51" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J51">
         <v>7</v>
@@ -4907,7 +4907,7 @@
         <v>1</v>
       </c>
       <c r="I52" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J52">
         <v>1.727</v>
@@ -4981,7 +4981,7 @@
         <v>45158.75</v>
       </c>
       <c r="E53" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F53" t="s">
         <v>32</v>
@@ -4993,7 +4993,7 @@
         <v>1</v>
       </c>
       <c r="I53" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J53">
         <v>1.571</v>
@@ -5079,7 +5079,7 @@
         <v>1</v>
       </c>
       <c r="I54" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J54">
         <v>1.8</v>
@@ -5144,22 +5144,22 @@
         <v>53</v>
       </c>
       <c r="B55">
-        <v>6227863</v>
+        <v>6227862</v>
       </c>
       <c r="C55" t="s">
         <v>27</v>
       </c>
       <c r="D55" s="2">
-        <v>45164.83333333334</v>
+        <v>45164.66666666666</v>
       </c>
       <c r="E55" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="F55" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="G55">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H55">
         <v>0</v>
@@ -5168,61 +5168,61 @@
         <v>38</v>
       </c>
       <c r="J55">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="K55">
         <v>3</v>
       </c>
       <c r="L55">
-        <v>2.6</v>
+        <v>3.6</v>
       </c>
       <c r="M55">
-        <v>2.6</v>
+        <v>1.85</v>
       </c>
       <c r="N55">
         <v>3.1</v>
       </c>
       <c r="O55">
-        <v>2.55</v>
+        <v>4</v>
       </c>
       <c r="P55">
-        <v>0</v>
+        <v>-0.5</v>
       </c>
       <c r="Q55">
-        <v>1.925</v>
+        <v>1.95</v>
       </c>
       <c r="R55">
-        <v>1.875</v>
+        <v>1.85</v>
       </c>
       <c r="S55">
-        <v>2.5</v>
+        <v>2.25</v>
       </c>
       <c r="T55">
-        <v>1.925</v>
+        <v>1.825</v>
       </c>
       <c r="U55">
-        <v>1.875</v>
+        <v>1.975</v>
       </c>
       <c r="V55">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
       <c r="W55">
-        <v>2.1</v>
+        <v>-1</v>
       </c>
       <c r="X55">
         <v>-1</v>
       </c>
       <c r="Y55">
-        <v>0</v>
+        <v>0.95</v>
       </c>
       <c r="Z55">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AA55">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
       <c r="AB55">
-        <v>0.875</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="56" spans="1:28">
@@ -5230,22 +5230,22 @@
         <v>54</v>
       </c>
       <c r="B56">
-        <v>6227862</v>
+        <v>6227863</v>
       </c>
       <c r="C56" t="s">
         <v>27</v>
       </c>
       <c r="D56" s="2">
-        <v>45164.66666666666</v>
+        <v>45164.83333333334</v>
       </c>
       <c r="E56" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F56" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G56">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H56">
         <v>0</v>
@@ -5254,61 +5254,61 @@
         <v>37</v>
       </c>
       <c r="J56">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="K56">
         <v>3</v>
       </c>
       <c r="L56">
-        <v>3.6</v>
+        <v>2.6</v>
       </c>
       <c r="M56">
-        <v>1.85</v>
+        <v>2.6</v>
       </c>
       <c r="N56">
         <v>3.1</v>
       </c>
       <c r="O56">
-        <v>4</v>
+        <v>2.55</v>
       </c>
       <c r="P56">
-        <v>-0.5</v>
+        <v>0</v>
       </c>
       <c r="Q56">
-        <v>1.95</v>
+        <v>1.925</v>
       </c>
       <c r="R56">
-        <v>1.85</v>
+        <v>1.875</v>
       </c>
       <c r="S56">
-        <v>2.25</v>
+        <v>2.5</v>
       </c>
       <c r="T56">
-        <v>1.825</v>
+        <v>1.925</v>
       </c>
       <c r="U56">
-        <v>1.975</v>
+        <v>1.875</v>
       </c>
       <c r="V56">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
       <c r="W56">
-        <v>-1</v>
+        <v>2.1</v>
       </c>
       <c r="X56">
         <v>-1</v>
       </c>
       <c r="Y56">
-        <v>0.95</v>
+        <v>0</v>
       </c>
       <c r="Z56">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AA56">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
       <c r="AB56">
-        <v>-1</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="57" spans="1:28">
@@ -5325,7 +5325,7 @@
         <v>45165.75</v>
       </c>
       <c r="E57" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F57" t="s">
         <v>35</v>
@@ -5337,7 +5337,7 @@
         <v>0</v>
       </c>
       <c r="I57" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J57">
         <v>2.4</v>
@@ -5402,82 +5402,82 @@
         <v>56</v>
       </c>
       <c r="B58">
-        <v>6227866</v>
+        <v>6227865</v>
       </c>
       <c r="C58" t="s">
         <v>27</v>
       </c>
       <c r="D58" s="2">
-        <v>45171.83333333334</v>
+        <v>45171.70833333334</v>
       </c>
       <c r="E58" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="F58" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G58">
+        <v>2</v>
+      </c>
+      <c r="H58">
         <v>1</v>
       </c>
-      <c r="H58">
-        <v>2</v>
-      </c>
       <c r="I58" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="J58">
-        <v>2.4</v>
+        <v>1.7</v>
       </c>
       <c r="K58">
-        <v>3.2</v>
+        <v>3.4</v>
       </c>
       <c r="L58">
-        <v>2.6</v>
+        <v>4.333</v>
       </c>
       <c r="M58">
-        <v>2.8</v>
+        <v>1.65</v>
       </c>
       <c r="N58">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="O58">
-        <v>2.375</v>
+        <v>4.75</v>
       </c>
       <c r="P58">
-        <v>0</v>
+        <v>-0.75</v>
       </c>
       <c r="Q58">
-        <v>2.05</v>
+        <v>1.85</v>
       </c>
       <c r="R58">
-        <v>1.75</v>
+        <v>1.95</v>
       </c>
       <c r="S58">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="T58">
-        <v>1.775</v>
+        <v>1.925</v>
       </c>
       <c r="U58">
-        <v>2.025</v>
+        <v>1.875</v>
       </c>
       <c r="V58">
-        <v>-1</v>
+        <v>0.6499999999999999</v>
       </c>
       <c r="W58">
         <v>-1</v>
       </c>
       <c r="X58">
-        <v>1.375</v>
+        <v>-1</v>
       </c>
       <c r="Y58">
-        <v>-1</v>
+        <v>0.425</v>
       </c>
       <c r="Z58">
-        <v>0.75</v>
+        <v>-0.5</v>
       </c>
       <c r="AA58">
-        <v>0.7749999999999999</v>
+        <v>0.925</v>
       </c>
       <c r="AB58">
         <v>-1</v>
@@ -5488,82 +5488,82 @@
         <v>57</v>
       </c>
       <c r="B59">
-        <v>6227865</v>
+        <v>6227866</v>
       </c>
       <c r="C59" t="s">
         <v>27</v>
       </c>
       <c r="D59" s="2">
-        <v>45171.70833333334</v>
+        <v>45171.83333333334</v>
       </c>
       <c r="E59" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="F59" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G59">
+        <v>1</v>
+      </c>
+      <c r="H59">
         <v>2</v>
       </c>
-      <c r="H59">
-        <v>1</v>
-      </c>
       <c r="I59" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J59">
-        <v>1.7</v>
+        <v>2.4</v>
       </c>
       <c r="K59">
-        <v>3.4</v>
+        <v>3.2</v>
       </c>
       <c r="L59">
-        <v>4.333</v>
+        <v>2.6</v>
       </c>
       <c r="M59">
-        <v>1.65</v>
+        <v>2.8</v>
       </c>
       <c r="N59">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="O59">
-        <v>4.75</v>
+        <v>2.375</v>
       </c>
       <c r="P59">
-        <v>-0.75</v>
+        <v>0</v>
       </c>
       <c r="Q59">
-        <v>1.85</v>
+        <v>2.05</v>
       </c>
       <c r="R59">
-        <v>1.95</v>
+        <v>1.75</v>
       </c>
       <c r="S59">
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="T59">
-        <v>1.925</v>
+        <v>1.775</v>
       </c>
       <c r="U59">
-        <v>1.875</v>
+        <v>2.025</v>
       </c>
       <c r="V59">
-        <v>0.6499999999999999</v>
+        <v>-1</v>
       </c>
       <c r="W59">
         <v>-1</v>
       </c>
       <c r="X59">
-        <v>-1</v>
+        <v>1.375</v>
       </c>
       <c r="Y59">
-        <v>0.425</v>
+        <v>-1</v>
       </c>
       <c r="Z59">
-        <v>-0.5</v>
+        <v>0.75</v>
       </c>
       <c r="AA59">
-        <v>0.925</v>
+        <v>0.7749999999999999</v>
       </c>
       <c r="AB59">
         <v>-1</v>
@@ -5746,85 +5746,85 @@
         <v>60</v>
       </c>
       <c r="B62">
-        <v>6227869</v>
+        <v>6227868</v>
       </c>
       <c r="C62" t="s">
         <v>27</v>
       </c>
       <c r="D62" s="2">
-        <v>45177.95833333334</v>
+        <v>45177.83333333334</v>
       </c>
       <c r="E62" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F62" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G62">
         <v>1</v>
       </c>
       <c r="H62">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I62" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J62">
-        <v>1.75</v>
+        <v>2.15</v>
       </c>
       <c r="K62">
-        <v>3.3</v>
+        <v>3.25</v>
       </c>
       <c r="L62">
-        <v>4.2</v>
+        <v>3</v>
       </c>
       <c r="M62">
-        <v>1.6</v>
+        <v>1.85</v>
       </c>
       <c r="N62">
+        <v>3.4</v>
+      </c>
+      <c r="O62">
         <v>3.6</v>
       </c>
-      <c r="O62">
-        <v>5</v>
-      </c>
       <c r="P62">
-        <v>-0.75</v>
+        <v>-0.5</v>
       </c>
       <c r="Q62">
-        <v>1.8</v>
+        <v>1.9</v>
       </c>
       <c r="R62">
-        <v>2</v>
+        <v>1.9</v>
       </c>
       <c r="S62">
-        <v>2.5</v>
+        <v>2.75</v>
       </c>
       <c r="T62">
-        <v>1.85</v>
+        <v>1.825</v>
       </c>
       <c r="U62">
-        <v>1.95</v>
+        <v>1.975</v>
       </c>
       <c r="V62">
         <v>-1</v>
       </c>
       <c r="W62">
+        <v>-1</v>
+      </c>
+      <c r="X62">
         <v>2.6</v>
       </c>
-      <c r="X62">
-        <v>-1</v>
-      </c>
       <c r="Y62">
         <v>-1</v>
       </c>
       <c r="Z62">
-        <v>1</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="AA62">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
       <c r="AB62">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="63" spans="1:28">
@@ -5832,85 +5832,85 @@
         <v>61</v>
       </c>
       <c r="B63">
-        <v>6227868</v>
+        <v>6227869</v>
       </c>
       <c r="C63" t="s">
         <v>27</v>
       </c>
       <c r="D63" s="2">
-        <v>45177.83333333334</v>
+        <v>45177.95833333334</v>
       </c>
       <c r="E63" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F63" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G63">
         <v>1</v>
       </c>
       <c r="H63">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I63" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J63">
-        <v>2.15</v>
+        <v>1.75</v>
       </c>
       <c r="K63">
-        <v>3.25</v>
+        <v>3.3</v>
       </c>
       <c r="L63">
-        <v>3</v>
+        <v>4.2</v>
       </c>
       <c r="M63">
+        <v>1.6</v>
+      </c>
+      <c r="N63">
+        <v>3.6</v>
+      </c>
+      <c r="O63">
+        <v>5</v>
+      </c>
+      <c r="P63">
+        <v>-0.75</v>
+      </c>
+      <c r="Q63">
+        <v>1.8</v>
+      </c>
+      <c r="R63">
+        <v>2</v>
+      </c>
+      <c r="S63">
+        <v>2.5</v>
+      </c>
+      <c r="T63">
         <v>1.85</v>
       </c>
-      <c r="N63">
-        <v>3.4</v>
-      </c>
-      <c r="O63">
-        <v>3.6</v>
-      </c>
-      <c r="P63">
-        <v>-0.5</v>
-      </c>
-      <c r="Q63">
-        <v>1.9</v>
-      </c>
-      <c r="R63">
-        <v>1.9</v>
-      </c>
-      <c r="S63">
-        <v>2.75</v>
-      </c>
-      <c r="T63">
-        <v>1.825</v>
-      </c>
       <c r="U63">
-        <v>1.975</v>
+        <v>1.95</v>
       </c>
       <c r="V63">
         <v>-1</v>
       </c>
       <c r="W63">
-        <v>-1</v>
+        <v>2.6</v>
       </c>
       <c r="X63">
-        <v>2.6</v>
+        <v>-1</v>
       </c>
       <c r="Y63">
         <v>-1</v>
       </c>
       <c r="Z63">
-        <v>0.8999999999999999</v>
+        <v>1</v>
       </c>
       <c r="AA63">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
       <c r="AB63">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
     </row>
     <row r="64" spans="1:28">
@@ -5918,85 +5918,85 @@
         <v>62</v>
       </c>
       <c r="B64">
-        <v>6240267</v>
+        <v>6227870</v>
       </c>
       <c r="C64" t="s">
         <v>27</v>
       </c>
       <c r="D64" s="2">
-        <v>45178.95833333334</v>
+        <v>45178.83333333334</v>
       </c>
       <c r="E64" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F64" t="s">
         <v>29</v>
       </c>
       <c r="G64">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H64">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I64" t="s">
         <v>37</v>
       </c>
       <c r="J64">
-        <v>3.5</v>
+        <v>1.909</v>
       </c>
       <c r="K64">
-        <v>3.5</v>
+        <v>3.4</v>
       </c>
       <c r="L64">
-        <v>1.85</v>
+        <v>3.4</v>
       </c>
       <c r="M64">
-        <v>3.3</v>
+        <v>2.15</v>
       </c>
       <c r="N64">
-        <v>3.6</v>
+        <v>3.4</v>
       </c>
       <c r="O64">
-        <v>1.909</v>
+        <v>2.8</v>
       </c>
       <c r="P64">
-        <v>0.5</v>
+        <v>-0.25</v>
       </c>
       <c r="Q64">
-        <v>1.9</v>
+        <v>1.825</v>
       </c>
       <c r="R64">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="S64">
         <v>2.5</v>
       </c>
       <c r="T64">
-        <v>1.75</v>
+        <v>1.95</v>
       </c>
       <c r="U64">
-        <v>1.95</v>
+        <v>1.85</v>
       </c>
       <c r="V64">
-        <v>2.3</v>
+        <v>-1</v>
       </c>
       <c r="W64">
-        <v>-1</v>
+        <v>2.4</v>
       </c>
       <c r="X64">
         <v>-1</v>
       </c>
       <c r="Y64">
-        <v>0.8999999999999999</v>
+        <v>-0.5</v>
       </c>
       <c r="Z64">
-        <v>-1</v>
+        <v>0.4875</v>
       </c>
       <c r="AA64">
-        <v>0.75</v>
+        <v>-1</v>
       </c>
       <c r="AB64">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
     </row>
     <row r="65" spans="1:28">
@@ -6004,85 +6004,85 @@
         <v>63</v>
       </c>
       <c r="B65">
-        <v>6227870</v>
+        <v>6240267</v>
       </c>
       <c r="C65" t="s">
         <v>27</v>
       </c>
       <c r="D65" s="2">
-        <v>45178.83333333334</v>
+        <v>45178.95833333334</v>
       </c>
       <c r="E65" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F65" t="s">
         <v>30</v>
       </c>
       <c r="G65">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H65">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I65" t="s">
         <v>38</v>
       </c>
       <c r="J65">
+        <v>3.5</v>
+      </c>
+      <c r="K65">
+        <v>3.5</v>
+      </c>
+      <c r="L65">
+        <v>1.85</v>
+      </c>
+      <c r="M65">
+        <v>3.3</v>
+      </c>
+      <c r="N65">
+        <v>3.6</v>
+      </c>
+      <c r="O65">
         <v>1.909</v>
       </c>
-      <c r="K65">
-        <v>3.4</v>
-      </c>
-      <c r="L65">
-        <v>3.4</v>
-      </c>
-      <c r="M65">
-        <v>2.15</v>
-      </c>
-      <c r="N65">
-        <v>3.4</v>
-      </c>
-      <c r="O65">
-        <v>2.8</v>
-      </c>
       <c r="P65">
-        <v>-0.25</v>
+        <v>0.5</v>
       </c>
       <c r="Q65">
-        <v>1.825</v>
+        <v>1.9</v>
       </c>
       <c r="R65">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="S65">
         <v>2.5</v>
       </c>
       <c r="T65">
+        <v>1.75</v>
+      </c>
+      <c r="U65">
         <v>1.95</v>
       </c>
-      <c r="U65">
-        <v>1.85</v>
-      </c>
       <c r="V65">
-        <v>-1</v>
+        <v>2.3</v>
       </c>
       <c r="W65">
-        <v>2.4</v>
+        <v>-1</v>
       </c>
       <c r="X65">
         <v>-1</v>
       </c>
       <c r="Y65">
-        <v>-0.5</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="Z65">
-        <v>0.4875</v>
+        <v>-1</v>
       </c>
       <c r="AA65">
-        <v>-1</v>
+        <v>0.75</v>
       </c>
       <c r="AB65">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="66" spans="1:28">
@@ -6102,7 +6102,7 @@
         <v>33</v>
       </c>
       <c r="F66" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G66">
         <v>1</v>
@@ -6185,7 +6185,7 @@
         <v>45182.77083333334</v>
       </c>
       <c r="E67" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F67" t="s">
         <v>35</v>
@@ -6197,7 +6197,7 @@
         <v>1</v>
       </c>
       <c r="I67" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J67">
         <v>2.5</v>
@@ -6271,7 +6271,7 @@
         <v>45185.75</v>
       </c>
       <c r="E68" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F68" t="s">
         <v>28</v>
@@ -6283,7 +6283,7 @@
         <v>1</v>
       </c>
       <c r="I68" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J68">
         <v>1.285</v>
@@ -6532,7 +6532,7 @@
         <v>33</v>
       </c>
       <c r="F71" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G71">
         <v>3</v>
@@ -6541,7 +6541,7 @@
         <v>2</v>
       </c>
       <c r="I71" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J71">
         <v>2.625</v>
@@ -6704,7 +6704,7 @@
         <v>32</v>
       </c>
       <c r="F73" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G73">
         <v>0</v>
@@ -6799,7 +6799,7 @@
         <v>1</v>
       </c>
       <c r="I74" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J74">
         <v>3.75</v>
@@ -6885,7 +6885,7 @@
         <v>1</v>
       </c>
       <c r="I75" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J75">
         <v>2</v>
@@ -6959,7 +6959,7 @@
         <v>45193.625</v>
       </c>
       <c r="E76" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F76" t="s">
         <v>31</v>
@@ -7045,7 +7045,7 @@
         <v>45198.91666666666</v>
       </c>
       <c r="E77" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F77" t="s">
         <v>31</v>
@@ -7057,7 +7057,7 @@
         <v>1</v>
       </c>
       <c r="I77" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J77">
         <v>1.615</v>
@@ -7143,7 +7143,7 @@
         <v>1</v>
       </c>
       <c r="I78" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J78">
         <v>2.625</v>
@@ -7306,7 +7306,7 @@
         <v>32</v>
       </c>
       <c r="F80" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G80">
         <v>1</v>
@@ -7315,7 +7315,7 @@
         <v>0</v>
       </c>
       <c r="I80" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J80">
         <v>2.375</v>
@@ -7380,65 +7380,65 @@
         <v>79</v>
       </c>
       <c r="B81">
-        <v>6240262</v>
+        <v>6227882</v>
       </c>
       <c r="C81" t="s">
         <v>27</v>
       </c>
       <c r="D81" s="2">
-        <v>45205.97916666666</v>
+        <v>45205.85416666666</v>
       </c>
       <c r="E81" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F81" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G81">
+        <v>0</v>
+      </c>
+      <c r="H81">
         <v>1</v>
-      </c>
-      <c r="H81">
-        <v>2</v>
       </c>
       <c r="I81" t="s">
         <v>36</v>
       </c>
       <c r="J81">
-        <v>3</v>
+        <v>2.75</v>
       </c>
       <c r="K81">
-        <v>3.4</v>
+        <v>3.2</v>
       </c>
       <c r="L81">
+        <v>2.3</v>
+      </c>
+      <c r="M81">
+        <v>2.7</v>
+      </c>
+      <c r="N81">
+        <v>3.25</v>
+      </c>
+      <c r="O81">
+        <v>2.3</v>
+      </c>
+      <c r="P81">
+        <v>0.25</v>
+      </c>
+      <c r="Q81">
+        <v>1.75</v>
+      </c>
+      <c r="R81">
         <v>2.05</v>
       </c>
-      <c r="M81">
-        <v>3.1</v>
-      </c>
-      <c r="N81">
-        <v>3.6</v>
-      </c>
-      <c r="O81">
-        <v>1.95</v>
-      </c>
-      <c r="P81">
-        <v>0.5</v>
-      </c>
-      <c r="Q81">
+      <c r="S81">
+        <v>2.5</v>
+      </c>
+      <c r="T81">
         <v>1.825</v>
       </c>
-      <c r="R81">
+      <c r="U81">
         <v>1.975</v>
       </c>
-      <c r="S81">
-        <v>3.25</v>
-      </c>
-      <c r="T81">
-        <v>1.95</v>
-      </c>
-      <c r="U81">
-        <v>1.85</v>
-      </c>
       <c r="V81">
         <v>-1</v>
       </c>
@@ -7446,19 +7446,19 @@
         <v>-1</v>
       </c>
       <c r="X81">
-        <v>0.95</v>
+        <v>1.3</v>
       </c>
       <c r="Y81">
         <v>-1</v>
       </c>
       <c r="Z81">
+        <v>1.05</v>
+      </c>
+      <c r="AA81">
+        <v>-1</v>
+      </c>
+      <c r="AB81">
         <v>0.9750000000000001</v>
-      </c>
-      <c r="AA81">
-        <v>-0.5</v>
-      </c>
-      <c r="AB81">
-        <v>0.425</v>
       </c>
     </row>
     <row r="82" spans="1:28">
@@ -7466,64 +7466,64 @@
         <v>80</v>
       </c>
       <c r="B82">
-        <v>6227882</v>
+        <v>6240262</v>
       </c>
       <c r="C82" t="s">
         <v>27</v>
       </c>
       <c r="D82" s="2">
-        <v>45205.85416666666</v>
+        <v>45205.97916666666</v>
       </c>
       <c r="E82" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="F82" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G82">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H82">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I82" t="s">
         <v>36</v>
       </c>
       <c r="J82">
-        <v>2.75</v>
+        <v>3</v>
       </c>
       <c r="K82">
-        <v>3.2</v>
+        <v>3.4</v>
       </c>
       <c r="L82">
-        <v>2.3</v>
+        <v>2.05</v>
       </c>
       <c r="M82">
-        <v>2.7</v>
+        <v>3.1</v>
       </c>
       <c r="N82">
+        <v>3.6</v>
+      </c>
+      <c r="O82">
+        <v>1.95</v>
+      </c>
+      <c r="P82">
+        <v>0.5</v>
+      </c>
+      <c r="Q82">
+        <v>1.825</v>
+      </c>
+      <c r="R82">
+        <v>1.975</v>
+      </c>
+      <c r="S82">
         <v>3.25</v>
       </c>
-      <c r="O82">
-        <v>2.3</v>
-      </c>
-      <c r="P82">
-        <v>0.25</v>
-      </c>
-      <c r="Q82">
-        <v>1.75</v>
-      </c>
-      <c r="R82">
-        <v>2.05</v>
-      </c>
-      <c r="S82">
-        <v>2.5</v>
-      </c>
       <c r="T82">
-        <v>1.825</v>
+        <v>1.95</v>
       </c>
       <c r="U82">
-        <v>1.975</v>
+        <v>1.85</v>
       </c>
       <c r="V82">
         <v>-1</v>
@@ -7532,19 +7532,19 @@
         <v>-1</v>
       </c>
       <c r="X82">
-        <v>1.3</v>
+        <v>0.95</v>
       </c>
       <c r="Y82">
         <v>-1</v>
       </c>
       <c r="Z82">
-        <v>1.05</v>
+        <v>0.9750000000000001</v>
       </c>
       <c r="AA82">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="AB82">
-        <v>0.9750000000000001</v>
+        <v>0.425</v>
       </c>
     </row>
     <row r="83" spans="1:28">
@@ -7552,7 +7552,7 @@
         <v>81</v>
       </c>
       <c r="B83">
-        <v>7301364</v>
+        <v>6227884</v>
       </c>
       <c r="C83" t="s">
         <v>27</v>
@@ -7561,76 +7561,76 @@
         <v>45206.75</v>
       </c>
       <c r="E83" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="F83" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="G83">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H83">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I83" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="J83">
-        <v>1.8</v>
+        <v>2.25</v>
       </c>
       <c r="K83">
-        <v>3.6</v>
+        <v>3.1</v>
       </c>
       <c r="L83">
-        <v>3.5</v>
+        <v>2.875</v>
       </c>
       <c r="M83">
-        <v>1.533</v>
+        <v>2.05</v>
       </c>
       <c r="N83">
-        <v>3.8</v>
+        <v>3.2</v>
       </c>
       <c r="O83">
-        <v>5</v>
+        <v>3.2</v>
       </c>
       <c r="P83">
-        <v>-1</v>
+        <v>-0.25</v>
       </c>
       <c r="Q83">
+        <v>1.825</v>
+      </c>
+      <c r="R83">
         <v>1.975</v>
-      </c>
-      <c r="R83">
-        <v>1.825</v>
       </c>
       <c r="S83">
         <v>2.5</v>
       </c>
       <c r="T83">
-        <v>1.9</v>
+        <v>1.825</v>
       </c>
       <c r="U83">
-        <v>1.9</v>
+        <v>1.975</v>
       </c>
       <c r="V83">
-        <v>-1</v>
+        <v>1.05</v>
       </c>
       <c r="W83">
         <v>-1</v>
       </c>
       <c r="X83">
-        <v>4</v>
+        <v>-1</v>
       </c>
       <c r="Y83">
-        <v>-1</v>
+        <v>0.825</v>
       </c>
       <c r="Z83">
+        <v>-1</v>
+      </c>
+      <c r="AA83">
         <v>0.825</v>
       </c>
-      <c r="AA83">
-        <v>-1</v>
-      </c>
       <c r="AB83">
-        <v>0.8999999999999999</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="84" spans="1:28">
@@ -7638,7 +7638,7 @@
         <v>82</v>
       </c>
       <c r="B84">
-        <v>6227884</v>
+        <v>7301364</v>
       </c>
       <c r="C84" t="s">
         <v>27</v>
@@ -7647,76 +7647,76 @@
         <v>45206.75</v>
       </c>
       <c r="E84" t="s">
+        <v>34</v>
+      </c>
+      <c r="F84" t="s">
         <v>30</v>
       </c>
-      <c r="F84" t="s">
-        <v>35</v>
-      </c>
       <c r="G84">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H84">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I84" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J84">
-        <v>2.25</v>
+        <v>1.8</v>
       </c>
       <c r="K84">
-        <v>3.1</v>
+        <v>3.6</v>
       </c>
       <c r="L84">
-        <v>2.875</v>
+        <v>3.5</v>
       </c>
       <c r="M84">
-        <v>2.05</v>
+        <v>1.533</v>
       </c>
       <c r="N84">
-        <v>3.2</v>
+        <v>3.8</v>
       </c>
       <c r="O84">
-        <v>3.2</v>
+        <v>5</v>
       </c>
       <c r="P84">
-        <v>-0.25</v>
+        <v>-1</v>
       </c>
       <c r="Q84">
+        <v>1.975</v>
+      </c>
+      <c r="R84">
         <v>1.825</v>
-      </c>
-      <c r="R84">
-        <v>1.975</v>
       </c>
       <c r="S84">
         <v>2.5</v>
       </c>
       <c r="T84">
-        <v>1.825</v>
+        <v>1.9</v>
       </c>
       <c r="U84">
-        <v>1.975</v>
+        <v>1.9</v>
       </c>
       <c r="V84">
-        <v>1.05</v>
+        <v>-1</v>
       </c>
       <c r="W84">
         <v>-1</v>
       </c>
       <c r="X84">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="Y84">
+        <v>-1</v>
+      </c>
+      <c r="Z84">
         <v>0.825</v>
       </c>
-      <c r="Z84">
-        <v>-1</v>
-      </c>
       <c r="AA84">
-        <v>0.825</v>
+        <v>-1</v>
       </c>
       <c r="AB84">
-        <v>-1</v>
+        <v>0.8999999999999999</v>
       </c>
     </row>
     <row r="85" spans="1:28">
@@ -7745,7 +7745,7 @@
         <v>0</v>
       </c>
       <c r="I85" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J85">
         <v>1.727</v>
@@ -7810,55 +7810,55 @@
         <v>84</v>
       </c>
       <c r="B86">
-        <v>7314311</v>
+        <v>7334555</v>
       </c>
       <c r="C86" t="s">
         <v>27</v>
       </c>
       <c r="D86" s="2">
-        <v>45213.75</v>
+        <v>45213.625</v>
       </c>
       <c r="E86" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="F86" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G86">
+        <v>0</v>
+      </c>
+      <c r="H86">
         <v>1</v>
-      </c>
-      <c r="H86">
-        <v>2</v>
       </c>
       <c r="I86" t="s">
         <v>36</v>
       </c>
       <c r="J86">
-        <v>2.3</v>
+        <v>2.6</v>
       </c>
       <c r="K86">
         <v>3.2</v>
       </c>
       <c r="L86">
-        <v>2.7</v>
+        <v>2.375</v>
       </c>
       <c r="M86">
-        <v>2.1</v>
+        <v>2.6</v>
       </c>
       <c r="N86">
         <v>3.2</v>
       </c>
       <c r="O86">
-        <v>3.1</v>
+        <v>2.375</v>
       </c>
       <c r="P86">
-        <v>-0.25</v>
+        <v>0</v>
       </c>
       <c r="Q86">
-        <v>1.875</v>
+        <v>2</v>
       </c>
       <c r="R86">
-        <v>1.925</v>
+        <v>1.8</v>
       </c>
       <c r="S86">
         <v>2.5</v>
@@ -7876,19 +7876,19 @@
         <v>-1</v>
       </c>
       <c r="X86">
-        <v>2.1</v>
+        <v>1.375</v>
       </c>
       <c r="Y86">
         <v>-1</v>
       </c>
       <c r="Z86">
-        <v>0.925</v>
+        <v>0.8</v>
       </c>
       <c r="AA86">
-        <v>0.95</v>
+        <v>-1</v>
       </c>
       <c r="AB86">
-        <v>-1</v>
+        <v>0.8500000000000001</v>
       </c>
     </row>
     <row r="87" spans="1:28">
@@ -7896,55 +7896,55 @@
         <v>85</v>
       </c>
       <c r="B87">
-        <v>7334555</v>
+        <v>7314311</v>
       </c>
       <c r="C87" t="s">
         <v>27</v>
       </c>
       <c r="D87" s="2">
-        <v>45213.625</v>
+        <v>45213.75</v>
       </c>
       <c r="E87" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F87" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G87">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H87">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I87" t="s">
         <v>36</v>
       </c>
       <c r="J87">
-        <v>2.6</v>
+        <v>2.3</v>
       </c>
       <c r="K87">
         <v>3.2</v>
       </c>
       <c r="L87">
-        <v>2.375</v>
+        <v>2.7</v>
       </c>
       <c r="M87">
-        <v>2.6</v>
+        <v>2.1</v>
       </c>
       <c r="N87">
         <v>3.2</v>
       </c>
       <c r="O87">
-        <v>2.375</v>
+        <v>3.1</v>
       </c>
       <c r="P87">
-        <v>0</v>
+        <v>-0.25</v>
       </c>
       <c r="Q87">
-        <v>2</v>
+        <v>1.875</v>
       </c>
       <c r="R87">
-        <v>1.8</v>
+        <v>1.925</v>
       </c>
       <c r="S87">
         <v>2.5</v>
@@ -7962,19 +7962,19 @@
         <v>-1</v>
       </c>
       <c r="X87">
-        <v>1.375</v>
+        <v>2.1</v>
       </c>
       <c r="Y87">
         <v>-1</v>
       </c>
       <c r="Z87">
-        <v>0.8</v>
+        <v>0.925</v>
       </c>
       <c r="AA87">
-        <v>-1</v>
+        <v>0.95</v>
       </c>
       <c r="AB87">
-        <v>0.8500000000000001</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="88" spans="1:28">
@@ -7994,7 +7994,7 @@
         <v>34</v>
       </c>
       <c r="F88" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G88">
         <v>2</v>
@@ -8003,7 +8003,7 @@
         <v>1</v>
       </c>
       <c r="I88" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J88">
         <v>2.2</v>
@@ -8077,7 +8077,7 @@
         <v>45395.58333333334</v>
       </c>
       <c r="E89" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F89" t="s">
         <v>32</v>
@@ -8089,7 +8089,7 @@
         <v>1</v>
       </c>
       <c r="I89" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J89">
         <v>2.875</v>
@@ -8166,7 +8166,7 @@
         <v>34</v>
       </c>
       <c r="F90" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G90">
         <v>2</v>
@@ -8175,7 +8175,7 @@
         <v>1</v>
       </c>
       <c r="I90" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J90">
         <v>2.2</v>
@@ -8261,7 +8261,7 @@
         <v>0</v>
       </c>
       <c r="I91" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J91">
         <v>1.833</v>
@@ -8347,7 +8347,7 @@
         <v>1</v>
       </c>
       <c r="I92" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J92">
         <v>2.4</v>
@@ -8433,7 +8433,7 @@
         <v>0</v>
       </c>
       <c r="I93" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J93">
         <v>3.1</v>
@@ -8519,7 +8519,7 @@
         <v>0</v>
       </c>
       <c r="I94" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J94">
         <v>1.727</v>
@@ -8593,10 +8593,10 @@
         <v>45402.625</v>
       </c>
       <c r="E95" t="s">
+        <v>30</v>
+      </c>
+      <c r="F95" t="s">
         <v>29</v>
-      </c>
-      <c r="F95" t="s">
-        <v>30</v>
       </c>
       <c r="G95">
         <v>1</v>
@@ -8605,7 +8605,7 @@
         <v>1</v>
       </c>
       <c r="I95" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J95">
         <v>3.1</v>
@@ -8777,7 +8777,7 @@
         <v>0</v>
       </c>
       <c r="I97" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J97">
         <v>2.2</v>
@@ -8842,82 +8842,82 @@
         <v>96</v>
       </c>
       <c r="B98">
-        <v>7802876</v>
+        <v>7802938</v>
       </c>
       <c r="C98" t="s">
         <v>27</v>
       </c>
       <c r="D98" s="2">
-        <v>45409.70833333334</v>
+        <v>45409.58333333334</v>
       </c>
       <c r="E98" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F98" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G98">
+        <v>1</v>
+      </c>
+      <c r="H98">
+        <v>3</v>
+      </c>
+      <c r="I98" t="s">
+        <v>36</v>
+      </c>
+      <c r="J98">
         <v>2</v>
       </c>
-      <c r="H98">
-        <v>1</v>
-      </c>
-      <c r="I98" t="s">
-        <v>37</v>
-      </c>
-      <c r="J98">
-        <v>1.6</v>
-      </c>
       <c r="K98">
-        <v>3.75</v>
+        <v>3.3</v>
       </c>
       <c r="L98">
-        <v>4.5</v>
+        <v>3.2</v>
       </c>
       <c r="M98">
-        <v>1.4</v>
+        <v>2.25</v>
       </c>
       <c r="N98">
-        <v>4</v>
+        <v>3.1</v>
       </c>
       <c r="O98">
-        <v>6.5</v>
+        <v>2.875</v>
       </c>
       <c r="P98">
-        <v>-1.25</v>
+        <v>-0.25</v>
       </c>
       <c r="Q98">
-        <v>1.9</v>
+        <v>2.025</v>
       </c>
       <c r="R98">
-        <v>1.9</v>
+        <v>1.775</v>
       </c>
       <c r="S98">
-        <v>2.5</v>
+        <v>2.25</v>
       </c>
       <c r="T98">
-        <v>1.8</v>
+        <v>1.95</v>
       </c>
       <c r="U98">
-        <v>2</v>
+        <v>1.85</v>
       </c>
       <c r="V98">
-        <v>0.3999999999999999</v>
+        <v>-1</v>
       </c>
       <c r="W98">
         <v>-1</v>
       </c>
       <c r="X98">
-        <v>-1</v>
+        <v>1.875</v>
       </c>
       <c r="Y98">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
       <c r="Z98">
-        <v>0.45</v>
+        <v>0.7749999999999999</v>
       </c>
       <c r="AA98">
-        <v>0.8</v>
+        <v>0.95</v>
       </c>
       <c r="AB98">
         <v>-1</v>
@@ -8928,82 +8928,82 @@
         <v>97</v>
       </c>
       <c r="B99">
-        <v>7802938</v>
+        <v>7802876</v>
       </c>
       <c r="C99" t="s">
         <v>27</v>
       </c>
       <c r="D99" s="2">
-        <v>45409.58333333334</v>
+        <v>45409.70833333334</v>
       </c>
       <c r="E99" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F99" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G99">
+        <v>2</v>
+      </c>
+      <c r="H99">
         <v>1</v>
       </c>
-      <c r="H99">
-        <v>3</v>
-      </c>
       <c r="I99" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="J99">
+        <v>1.6</v>
+      </c>
+      <c r="K99">
+        <v>3.75</v>
+      </c>
+      <c r="L99">
+        <v>4.5</v>
+      </c>
+      <c r="M99">
+        <v>1.4</v>
+      </c>
+      <c r="N99">
+        <v>4</v>
+      </c>
+      <c r="O99">
+        <v>6.5</v>
+      </c>
+      <c r="P99">
+        <v>-1.25</v>
+      </c>
+      <c r="Q99">
+        <v>1.9</v>
+      </c>
+      <c r="R99">
+        <v>1.9</v>
+      </c>
+      <c r="S99">
+        <v>2.5</v>
+      </c>
+      <c r="T99">
+        <v>1.8</v>
+      </c>
+      <c r="U99">
         <v>2</v>
       </c>
-      <c r="K99">
-        <v>3.3</v>
-      </c>
-      <c r="L99">
-        <v>3.2</v>
-      </c>
-      <c r="M99">
-        <v>2.25</v>
-      </c>
-      <c r="N99">
-        <v>3.1</v>
-      </c>
-      <c r="O99">
-        <v>2.875</v>
-      </c>
-      <c r="P99">
-        <v>-0.25</v>
-      </c>
-      <c r="Q99">
-        <v>2.025</v>
-      </c>
-      <c r="R99">
-        <v>1.775</v>
-      </c>
-      <c r="S99">
-        <v>2.25</v>
-      </c>
-      <c r="T99">
-        <v>1.95</v>
-      </c>
-      <c r="U99">
-        <v>1.85</v>
-      </c>
       <c r="V99">
-        <v>-1</v>
+        <v>0.3999999999999999</v>
       </c>
       <c r="W99">
         <v>-1</v>
       </c>
       <c r="X99">
-        <v>1.875</v>
+        <v>-1</v>
       </c>
       <c r="Y99">
-        <v>-1</v>
+        <v>-0.5</v>
       </c>
       <c r="Z99">
-        <v>0.7749999999999999</v>
+        <v>0.45</v>
       </c>
       <c r="AA99">
-        <v>0.95</v>
+        <v>0.8</v>
       </c>
       <c r="AB99">
         <v>-1</v>
@@ -9023,7 +9023,7 @@
         <v>45410.75</v>
       </c>
       <c r="E100" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F100" t="s">
         <v>35</v>
@@ -9035,7 +9035,7 @@
         <v>0</v>
       </c>
       <c r="I100" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J100">
         <v>2</v>

</xml_diff>